<commit_message>
31 Jul 21 1024
</commit_message>
<xml_diff>
--- a/bellevue.xlsx
+++ b/bellevue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>bellevue</t>
   </si>
@@ -43,7 +43,7 @@
     <t>{"created_at": "Mon Jul 26 20:01:00 +0000 2021", "hashtags": [{"text": "BellevueUniversity"}, {"text": "BUBruins"}, {"text": "CareerSuccess"}], "id": 1419749614224293892, "id_str": "1419749614224293892", "lang": "en", "source": "&lt;a href=\"https://www.hootsuite.com\" rel=\"nofollow\"&gt;Hootsuite Inc.&lt;/a&gt;", "text": "5 Quotes About Success, Debunked https://t.co/KYBaUjtnVU success-quotes/ #BellevueUniversity  #BUBruins #CareerSuccess", "urls": [{"expanded_url": "http://ow.ly/aN1650FkWFg", "url": "https://t.co/KYBaUjtnVU"}], "user": {"created_at": "Mon May 16 21:44:54 +0000 2016", "default_profile": true, "description": "Our goal is to assist you with making connections, obtaining mentoring opportunities &amp; aid in finding employment that mirrors your desires and qualifications.", "favourites_count": 52, "followers_count": 491, "friends_count": 1518, "id": 732325979520040960, "id_str": "732325979520040960", "listed_count": 20, "location": "Bellevue, NE", "name": "Bellevue University Career Services", "profile_background_color": "F5F8FA", "profile_banner_url": "https://pbs.twimg.com/profile_banners/732325979520040960/1532537010", "profile_image_url": "http://pbs.twimg.com/profile_images/1022160813983850496/GJsD7K0B_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1022160813983850496/GJsD7K0B_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "BUCareer2", "statuses_count": 2923, "withheld_in_countries": []}, "user_mentions": []}</t>
   </si>
   <si>
-    <t>{"created_at": "Mon Jul 26 17:33:45 +0000 2021", "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}, {"text": "USL"}, {"text": "Partnership"}], "id": 1419712558857076736, "id_str": "1419712558857076736", "lang": "en", "media": [{"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686334554415106, "media_url": "http://pbs.twimg.com/media/E7O9Mw-XoAIOS_x.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9Mw-XoAIOS_x.jpg", "sizes": {"large": {"h": 1480, "resize": "fit", "w": 1984}, "medium": {"h": 895, "resize": "fit", "w": 1200}, "small": {"h": 507, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}, {"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686334550220809, "media_url": "http://pbs.twimg.com/media/E7O9Mw9XoAkaTFh.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9Mw9XoAkaTFh.jpg", "sizes": {"large": {"h": 1472, "resize": "fit", "w": 1108}, "medium": {"h": 1200, "resize": "fit", "w": 903}, "small": {"h": 680, "resize": "fit", "w": 512}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}, {"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686574271475720, "media_url": "http://pbs.twimg.com/media/E7O9at_XsAg8AAD.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9at_XsAg8AAD.jpg", "sizes": {"large": {"h": 1822, "resize": "fit", "w": 1260}, "medium": {"h": 1200, "resize": "fit", "w": 830}, "small": {"h": 680, "resize": "fit", "w": 470}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}], "retweet_count": 3, "retweeted_status": {"created_at": "Mon Jul 26 15:50:41 +0000 2021", "favorite_count": 6, "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}, {"text": "USL"}, {"text": "Partnership"}], "id": 1419686621260156933, "id_str": "1419686621260156933", "lang": "en", "media": [{"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686334554415106, "media_url": "http://pbs.twimg.com/media/E7O9Mw-XoAIOS_x.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9Mw-XoAIOS_x.jpg", "sizes": {"large": {"h": 1480, "resize": "fit", "w": 1984}, "medium": {"h": 895, "resize": "fit", "w": 1200}, "small": {"h": 507, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}, {"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686334550220809, "media_url": "http://pbs.twimg.com/media/E7O9Mw9XoAkaTFh.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9Mw9XoAkaTFh.jpg", "sizes": {"large": {"h": 1472, "resize": "fit", "w": 1108}, "medium": {"h": 1200, "resize": "fit", "w": 903}, "small": {"h": 680, "resize": "fit", "w": 512}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}, {"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686574271475720, "media_url": "http://pbs.twimg.com/media/E7O9at_XsAg8AAD.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9at_XsAg8AAD.jpg", "sizes": {"large": {"h": 1822, "resize": "fit", "w": 1260}, "medium": {"h": 1200, "resize": "fit", "w": 830}, "small": {"h": 680, "resize": "fit", "w": 470}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}], "retweet_count": 3, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "#USL Mid-Year Meeting in San Antonio! \ud83d\udc3b\u26bd\ufe0f\n\n#BellevueUniversity #USL #Partnership https://t.co/6YTrmTYG9z", "urls": [], "user": {"created_at": "Tue Oct 23 13:48:23 +0000 2007", "description": "Our learning programs combine mastery of deep, career-relevant knowledge and powerful professional skills, so you are prepared with tools for success.", "favourites_count": 4123, "followers_count": 9169, "friends_count": 2576, "id": 9623092, "id_str": "9623092", "listed_count": 210, "location": "Nebraska", "name": "Bellevue University", "profile_background_color": "4F3674", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/9623092/1614634074", "profile_image_url": "http://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_link_color": "4F3674", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "4A2334", "profile_text_color": "D5EC08", "screen_name": "BellevueU", "statuses_count": 6051, "url": "https://t.co/0hQEZBjUQK", "withheld_in_countries": []}, "user_mentions": []}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @BellevueU: #USL Mid-Year Meeting in San Antonio! \ud83d\udc3b\u26bd\ufe0f\n\n#BellevueUniversity #USL #Partnership https://t.co/6YTrmTYG9z", "urls": [], "user": {"created_at": "Sat Oct 05 14:39:11 +0000 2013", "default_profile": true, "description": "CHRIST Follower\ud83d\udd46. AC at Bellevue University WBB, RETRO HOOPS founder &amp; Coach.Husband, Father, Grandfather,Brother. Born &amp; Raised in TheD #missingoliviaforever", "favourites_count": 96582, "followers_count": 2379, "friends_count": 5000, "geo_enabled": true, "id": 1937867113, "id_str": "1937867113", "listed_count": 1, "location": "The D", "name": "COACH ICE/Bellevue University/RETRO HOOPS", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1937867113/1567087983", "profile_image_url": "http://pbs.twimg.com/profile_images/1382546624073900034/XFjoaHhL_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1382546624073900034/XFjoaHhL_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "thinmanx11", "statuses_count": 48227, "withheld_in_countries": []}, "user_mentions": [{"id": 9623092, "id_str": "9623092", "name": "Bellevue University", "screen_name": "BellevueU"}]}</t>
+    <t>{"created_at": "Mon Jul 26 17:33:45 +0000 2021", "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}, {"text": "USL"}, {"text": "Partnership"}], "id": 1419712558857076736, "id_str": "1419712558857076736", "lang": "en", "media": [{"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686334554415106, "media_url": "http://pbs.twimg.com/media/E7O9Mw-XoAIOS_x.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9Mw-XoAIOS_x.jpg", "sizes": {"large": {"h": 1480, "resize": "fit", "w": 1984}, "medium": {"h": 895, "resize": "fit", "w": 1200}, "small": {"h": 507, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}, {"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686334550220809, "media_url": "http://pbs.twimg.com/media/E7O9Mw9XoAkaTFh.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9Mw9XoAkaTFh.jpg", "sizes": {"large": {"h": 1472, "resize": "fit", "w": 1108}, "medium": {"h": 1200, "resize": "fit", "w": 903}, "small": {"h": 680, "resize": "fit", "w": 512}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}, {"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686574271475720, "media_url": "http://pbs.twimg.com/media/E7O9at_XsAg8AAD.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9at_XsAg8AAD.jpg", "sizes": {"large": {"h": 1822, "resize": "fit", "w": 1260}, "medium": {"h": 1200, "resize": "fit", "w": 830}, "small": {"h": 680, "resize": "fit", "w": 470}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}], "retweet_count": 3, "retweeted_status": {"created_at": "Mon Jul 26 15:50:41 +0000 2021", "favorite_count": 6, "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}, {"text": "USL"}, {"text": "Partnership"}], "id": 1419686621260156933, "id_str": "1419686621260156933", "lang": "en", "media": [{"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686334554415106, "media_url": "http://pbs.twimg.com/media/E7O9Mw-XoAIOS_x.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9Mw-XoAIOS_x.jpg", "sizes": {"large": {"h": 1480, "resize": "fit", "w": 1984}, "medium": {"h": 895, "resize": "fit", "w": 1200}, "small": {"h": 507, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}, {"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686334550220809, "media_url": "http://pbs.twimg.com/media/E7O9Mw9XoAkaTFh.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9Mw9XoAkaTFh.jpg", "sizes": {"large": {"h": 1472, "resize": "fit", "w": 1108}, "medium": {"h": 1200, "resize": "fit", "w": 903}, "small": {"h": 680, "resize": "fit", "w": 512}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}, {"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686574271475720, "media_url": "http://pbs.twimg.com/media/E7O9at_XsAg8AAD.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9at_XsAg8AAD.jpg", "sizes": {"large": {"h": 1822, "resize": "fit", "w": 1260}, "medium": {"h": 1200, "resize": "fit", "w": 830}, "small": {"h": 680, "resize": "fit", "w": 470}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}], "retweet_count": 3, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "#USL Mid-Year Meeting in San Antonio! \ud83d\udc3b\u26bd\ufe0f\n\n#BellevueUniversity #USL #Partnership https://t.co/6YTrmTYG9z", "urls": [], "user": {"created_at": "Tue Oct 23 13:48:23 +0000 2007", "description": "Our learning programs combine mastery of deep, career-relevant knowledge and powerful professional skills, so you are prepared with tools for success.", "favourites_count": 4123, "followers_count": 9169, "friends_count": 2576, "id": 9623092, "id_str": "9623092", "listed_count": 210, "location": "Nebraska", "name": "Bellevue University", "profile_background_color": "4F3674", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/9623092/1614634074", "profile_image_url": "http://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_link_color": "4F3674", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "4A2334", "profile_text_color": "D5EC08", "screen_name": "BellevueU", "statuses_count": 6051, "url": "https://t.co/0hQEZBjUQK", "withheld_in_countries": []}, "user_mentions": []}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @BellevueU: #USL Mid-Year Meeting in San Antonio! \ud83d\udc3b\u26bd\ufe0f\n\n#BellevueUniversity #USL #Partnership https://t.co/6YTrmTYG9z", "urls": [], "user": {"created_at": "Sat Oct 05 14:39:11 +0000 2013", "default_profile": true, "description": "CHRIST Follower\ud83d\udd46. AC at Bellevue University WBB, RETRO HOOPS founder &amp; Coach.Husband, Father, Grandfather,Brother. Born &amp; Raised in TheD #missingoliviaforever", "favourites_count": 96591, "followers_count": 2379, "friends_count": 4999, "geo_enabled": true, "id": 1937867113, "id_str": "1937867113", "listed_count": 1, "location": "The D", "name": "COACH ICE/Bellevue University/RETRO HOOPS", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1937867113/1567087983", "profile_image_url": "http://pbs.twimg.com/profile_images/1382546624073900034/XFjoaHhL_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1382546624073900034/XFjoaHhL_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "thinmanx11", "statuses_count": 48227, "withheld_in_countries": []}, "user_mentions": [{"id": 9623092, "id_str": "9623092", "name": "Bellevue University", "screen_name": "BellevueU"}]}</t>
   </si>
   <si>
     <t>{"created_at": "Mon Jul 26 16:32:45 +0000 2021", "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}, {"text": "USL"}, {"text": "Partnership"}], "id": 1419697205309370368, "id_str": "1419697205309370368", "lang": "en", "media": [{"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686334554415106, "media_url": "http://pbs.twimg.com/media/E7O9Mw-XoAIOS_x.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9Mw-XoAIOS_x.jpg", "sizes": {"large": {"h": 1480, "resize": "fit", "w": 1984}, "medium": {"h": 895, "resize": "fit", "w": 1200}, "small": {"h": 507, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}, {"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686334550220809, "media_url": "http://pbs.twimg.com/media/E7O9Mw9XoAkaTFh.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9Mw9XoAkaTFh.jpg", "sizes": {"large": {"h": 1472, "resize": "fit", "w": 1108}, "medium": {"h": 1200, "resize": "fit", "w": 903}, "small": {"h": 680, "resize": "fit", "w": 512}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}, {"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686574271475720, "media_url": "http://pbs.twimg.com/media/E7O9at_XsAg8AAD.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9at_XsAg8AAD.jpg", "sizes": {"large": {"h": 1822, "resize": "fit", "w": 1260}, "medium": {"h": 1200, "resize": "fit", "w": 830}, "small": {"h": 680, "resize": "fit", "w": 470}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}], "retweet_count": 3, "retweeted_status": {"created_at": "Mon Jul 26 15:50:41 +0000 2021", "favorite_count": 6, "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}, {"text": "USL"}, {"text": "Partnership"}], "id": 1419686621260156933, "id_str": "1419686621260156933", "lang": "en", "media": [{"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686334554415106, "media_url": "http://pbs.twimg.com/media/E7O9Mw-XoAIOS_x.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9Mw-XoAIOS_x.jpg", "sizes": {"large": {"h": 1480, "resize": "fit", "w": 1984}, "medium": {"h": 895, "resize": "fit", "w": 1200}, "small": {"h": 507, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}, {"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686334550220809, "media_url": "http://pbs.twimg.com/media/E7O9Mw9XoAkaTFh.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9Mw9XoAkaTFh.jpg", "sizes": {"large": {"h": 1472, "resize": "fit", "w": 1108}, "medium": {"h": 1200, "resize": "fit", "w": 903}, "small": {"h": 680, "resize": "fit", "w": 512}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}, {"display_url": "pic.twitter.com/6YTrmTYG9z", "expanded_url": "https://twitter.com/BellevueU/status/1419686621260156933/photo/1", "id": 1419686574271475720, "media_url": "http://pbs.twimg.com/media/E7O9at_XsAg8AAD.jpg", "media_url_https": "https://pbs.twimg.com/media/E7O9at_XsAg8AAD.jpg", "sizes": {"large": {"h": 1822, "resize": "fit", "w": 1260}, "medium": {"h": 1200, "resize": "fit", "w": 830}, "small": {"h": 680, "resize": "fit", "w": 470}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/6YTrmTYG9z"}], "retweet_count": 3, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "#USL Mid-Year Meeting in San Antonio! \ud83d\udc3b\u26bd\ufe0f\n\n#BellevueUniversity #USL #Partnership https://t.co/6YTrmTYG9z", "urls": [], "user": {"created_at": "Tue Oct 23 13:48:23 +0000 2007", "description": "Our learning programs combine mastery of deep, career-relevant knowledge and powerful professional skills, so you are prepared with tools for success.", "favourites_count": 4123, "followers_count": 9169, "friends_count": 2576, "id": 9623092, "id_str": "9623092", "listed_count": 210, "location": "Nebraska", "name": "Bellevue University", "profile_background_color": "4F3674", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/9623092/1614634074", "profile_image_url": "http://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_link_color": "4F3674", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "4A2334", "profile_text_color": "D5EC08", "screen_name": "BellevueU", "statuses_count": 6051, "url": "https://t.co/0hQEZBjUQK", "withheld_in_countries": []}, "user_mentions": []}, "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "RT @BellevueU: #USL Mid-Year Meeting in San Antonio! \ud83d\udc3b\u26bd\ufe0f\n\n#BellevueUniversity #USL #Partnership https://t.co/6YTrmTYG9z", "urls": [], "user": {"created_at": "Mon Feb 28 06:37:14 +0000 2011", "description": "Nebraskan who doesn\u2019t wear (Husker) red.", "favourites_count": 10915, "followers_count": 544, "friends_count": 1892, "geo_enabled": true, "id": 258674528, "id_str": "258674528", "listed_count": 6, "location": "Nebraska", "name": "Emily", "profile_background_color": "FFFFFF", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme13/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme13/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/258674528/1625683360", "profile_image_url": "http://pbs.twimg.com/profile_images/1412844527300354049/A5eRce9F_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1412844527300354049/A5eRce9F_normal.jpg", "profile_link_color": "1B95E0", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "38524F", "profile_text_color": "7A7A7A", "profile_use_background_image": true, "screen_name": "emilylutz2010", "statuses_count": 10529, "url": "https://t.co/5bpNGQGMd3", "withheld_in_countries": []}, "user_mentions": [{"id": 9623092, "id_str": "9623092", "name": "Bellevue University", "screen_name": "BellevueU"}]}</t>
@@ -61,7 +61,7 @@
     <t>{"created_at": "Mon Jul 26 04:08:52 +0000 2021", "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}], "id": 1419510003690610690, "id_str": "1419510003690610690", "lang": "en", "media": [{"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979419151077382, "media_url": "http://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "sizes": {"large": {"h": 1195, "resize": "fit", "w": 2048}, "medium": {"h": 700, "resize": "fit", "w": 1200}, "small": {"h": 397, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979442421112838, "media_url": "http://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "sizes": {"large": {"h": 1334, "resize": "fit", "w": 1424}, "medium": {"h": 1124, "resize": "fit", "w": 1200}, "small": {"h": 637, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979467846950919, "media_url": "http://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "sizes": {"large": {"h": 1540, "resize": "fit", "w": 1508}, "medium": {"h": 1200, "resize": "fit", "w": 1175}, "small": {"h": 680, "resize": "fit", "w": 666}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}], "retweet_count": 4, "retweeted_status": {"created_at": "Sat Jul 24 17:00:45 +0000 2021", "favorite_count": 22, "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}], "id": 1418979477061779468, "id_str": "1418979477061779468", "lang": "en", "media": [{"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979419151077382, "media_url": "http://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "sizes": {"large": {"h": 1195, "resize": "fit", "w": 2048}, "medium": {"h": 700, "resize": "fit", "w": 1200}, "small": {"h": 397, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979442421112838, "media_url": "http://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "sizes": {"large": {"h": 1334, "resize": "fit", "w": 1424}, "medium": {"h": 1124, "resize": "fit", "w": 1200}, "small": {"h": 637, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979467846950919, "media_url": "http://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "sizes": {"large": {"h": 1540, "resize": "fit", "w": 1508}, "medium": {"h": 1200, "resize": "fit", "w": 1175}, "small": {"h": 680, "resize": "fit", "w": 666}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}], "retweet_count": 4, "source": "&lt;a href=\"http://gainapp.com\" rel=\"nofollow\"&gt;Gain Platform&lt;/a&gt;", "text": "The beginning of a beautiful partnership! \u26bd\ufe0f\ud83d\udc3b\n\n#USL \n#BellevueUniversity https://t.co/zQsYiwWPfO", "urls": [], "user": {"created_at": "Tue Oct 23 13:48:23 +0000 2007", "description": "Our learning programs combine mastery of deep, career-relevant knowledge and powerful professional skills, so you are prepared with tools for success.", "favourites_count": 4123, "followers_count": 9169, "friends_count": 2576, "id": 9623092, "id_str": "9623092", "listed_count": 210, "location": "Nebraska", "name": "Bellevue University", "profile_background_color": "4F3674", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/9623092/1614634074", "profile_image_url": "http://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_link_color": "4F3674", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "4A2334", "profile_text_color": "D5EC08", "screen_name": "BellevueU", "statuses_count": 6051, "url": "https://t.co/0hQEZBjUQK", "withheld_in_countries": []}, "user_mentions": []}, "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "RT @BellevueU: The beginning of a beautiful partnership! \u26bd\ufe0f\ud83d\udc3b\n\n#USL \n#BellevueUniversity https://t.co/zQsYiwWPfO", "urls": [], "user": {"created_at": "Sun Sep 14 14:26:11 +0000 2014", "default_profile": true, "description": "The Official Twitter Page Of Bellevue University Women\u2019s Soccer", "favourites_count": 1412, "followers_count": 592, "friends_count": 221, "id": 2770104502, "id_str": "2770104502", "listed_count": 3, "location": "Bellevue,NE", "name": "Bellevue University Women's Soccer", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/2770104502/1581997624", "profile_image_url": "http://pbs.twimg.com/profile_images/1085231631512813569/KE2mbqP1_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1085231631512813569/KE2mbqP1_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "BU_WomenSoccer", "statuses_count": 774, "url": "https://t.co/MYHfKbDI59", "withheld_in_countries": []}, "user_mentions": [{"id": 9623092, "id_str": "9623092", "name": "Bellevue University", "screen_name": "BellevueU"}]}</t>
   </si>
   <si>
-    <t>{"created_at": "Sun Jul 25 23:45:35 +0000 2021", "hashtags": [{"text": "DisneyAspire"}], "id": 1419443745951453186, "id_str": "1419443745951453186", "lang": "en", "retweet_count": 1, "retweeted_status": {"created_at": "Sun Jul 25 17:00:58 +0000 2021", "favorite_count": 5, "hashtags": [{"text": "DisneyAspire"}], "id": 1419341918094467074, "id_str": "1419341918094467074", "lang": "en", "retweet_count": 1, "source": "&lt;a href=\"http://gainapp.com\" rel=\"nofollow\"&gt;Gain Platform&lt;/a&gt;", "text": "Graduating was magical \u2728\ud83d\udc51\n\nCongratulations on this amazing accomplishment, Mary! \n\n\ud83d\udcf7: @maryfoster\n\n#DisneyAspire\u2026 https://t.co/suX6cYdHne", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1419341918094467074", "url": "https://t.co/suX6cYdHne"}], "user": {"created_at": "Tue Oct 23 13:48:23 +0000 2007", "description": "Our learning programs combine mastery of deep, career-relevant knowledge and powerful professional skills, so you are prepared with tools for success.", "favourites_count": 4123, "followers_count": 9169, "friends_count": 2576, "id": 9623092, "id_str": "9623092", "listed_count": 210, "location": "Nebraska", "name": "Bellevue University", "profile_background_color": "4F3674", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/9623092/1614634074", "profile_image_url": "http://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_link_color": "4F3674", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "4A2334", "profile_text_color": "D5EC08", "screen_name": "BellevueU", "statuses_count": 6051, "url": "https://t.co/0hQEZBjUQK", "withheld_in_countries": []}, "user_mentions": [{"id": 19129143, "id_str": "19129143", "name": "MaryFoster", "screen_name": "MaryFoster"}]}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @BellevueU: Graduating was magical \u2728\ud83d\udc51\n\nCongratulations on this amazing accomplishment, Mary! \n\n\ud83d\udcf7: @maryfoster\n\n#DisneyAspire #GuildEduca\u2026", "urls": [], "user": {"created_at": "Fri Jul 05 00:46:32 +0000 2013", "default_profile": true, "description": "Prevent the Impact of Virtual Stalking's goal is to raise awareness through socialmedia activism.", "favourites_count": 50856, "followers_count": 693, "friends_count": 2116, "id": 1569393812, "id_str": "1569393812", "listed_count": 136, "name": "PSIVS", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1569393812/1393541909", "profile_image_url": "http://pbs.twimg.com/profile_images/378800000089056418/fd509d51f1648f0cf1b923bb5bad63f6_normal.jpeg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/378800000089056418/fd509d51f1648f0cf1b923bb5bad63f6_normal.jpeg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "StopVirtuaStalk", "statuses_count": 118750, "url": "http://t.co/MJqBSekNQm", "withheld_in_countries": []}, "user_mentions": [{"id": 9623092, "id_str": "9623092", "name": "Bellevue University", "screen_name": "BellevueU"}, {"id": 19129143, "id_str": "19129143", "name": "MaryFoster", "screen_name": "MaryFoster"}]}</t>
+    <t>{"created_at": "Sun Jul 25 23:45:35 +0000 2021", "hashtags": [{"text": "DisneyAspire"}], "id": 1419443745951453186, "id_str": "1419443745951453186", "lang": "en", "retweet_count": 1, "retweeted_status": {"created_at": "Sun Jul 25 17:00:58 +0000 2021", "favorite_count": 5, "hashtags": [{"text": "DisneyAspire"}], "id": 1419341918094467074, "id_str": "1419341918094467074", "lang": "en", "retweet_count": 1, "source": "&lt;a href=\"http://gainapp.com\" rel=\"nofollow\"&gt;Gain Platform&lt;/a&gt;", "text": "Graduating was magical \u2728\ud83d\udc51\n\nCongratulations on this amazing accomplishment, Mary! \n\n\ud83d\udcf7: @maryfoster\n\n#DisneyAspire\u2026 https://t.co/suX6cYdHne", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1419341918094467074", "url": "https://t.co/suX6cYdHne"}], "user": {"created_at": "Tue Oct 23 13:48:23 +0000 2007", "description": "Our learning programs combine mastery of deep, career-relevant knowledge and powerful professional skills, so you are prepared with tools for success.", "favourites_count": 4123, "followers_count": 9169, "friends_count": 2576, "id": 9623092, "id_str": "9623092", "listed_count": 210, "location": "Nebraska", "name": "Bellevue University", "profile_background_color": "4F3674", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/9623092/1614634074", "profile_image_url": "http://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_link_color": "4F3674", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "4A2334", "profile_text_color": "D5EC08", "screen_name": "BellevueU", "statuses_count": 6051, "url": "https://t.co/0hQEZBjUQK", "withheld_in_countries": []}, "user_mentions": [{"id": 19129143, "id_str": "19129143", "name": "MaryFoster", "screen_name": "MaryFoster"}]}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @BellevueU: Graduating was magical \u2728\ud83d\udc51\n\nCongratulations on this amazing accomplishment, Mary! \n\n\ud83d\udcf7: @maryfoster\n\n#DisneyAspire #GuildEduca\u2026", "urls": [], "user": {"created_at": "Fri Jul 05 00:46:32 +0000 2013", "default_profile": true, "description": "Prevent the Impact of Virtual Stalking's goal is to raise awareness through socialmedia activism.", "favourites_count": 50850, "followers_count": 692, "friends_count": 2113, "id": 1569393812, "id_str": "1569393812", "listed_count": 136, "name": "PSIVS", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1569393812/1393541909", "profile_image_url": "http://pbs.twimg.com/profile_images/378800000089056418/fd509d51f1648f0cf1b923bb5bad63f6_normal.jpeg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/378800000089056418/fd509d51f1648f0cf1b923bb5bad63f6_normal.jpeg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "StopVirtuaStalk", "statuses_count": 118750, "url": "http://t.co/MJqBSekNQm", "withheld_in_countries": []}, "user_mentions": [{"id": 9623092, "id_str": "9623092", "name": "Bellevue University", "screen_name": "BellevueU"}, {"id": 19129143, "id_str": "19129143", "name": "MaryFoster", "screen_name": "MaryFoster"}]}</t>
   </si>
   <si>
     <t>{"created_at": "Sun Jul 25 17:00:58 +0000 2021", "favorite_count": 5, "hashtags": [{"text": "DisneyAspire"}], "id": 1419341918094467074, "id_str": "1419341918094467074", "lang": "en", "retweet_count": 1, "source": "&lt;a href=\"http://gainapp.com\" rel=\"nofollow\"&gt;Gain Platform&lt;/a&gt;", "text": "Graduating was magical \u2728\ud83d\udc51\n\nCongratulations on this amazing accomplishment, Mary! \n\n\ud83d\udcf7: @maryfoster\n\n#DisneyAspire\u2026 https://t.co/suX6cYdHne", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1419341918094467074", "url": "https://t.co/suX6cYdHne"}], "user": {"created_at": "Tue Oct 23 13:48:23 +0000 2007", "description": "Our learning programs combine mastery of deep, career-relevant knowledge and powerful professional skills, so you are prepared with tools for success.", "favourites_count": 4123, "followers_count": 9169, "friends_count": 2576, "id": 9623092, "id_str": "9623092", "listed_count": 210, "location": "Nebraska", "name": "Bellevue University", "profile_background_color": "4F3674", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/9623092/1614634074", "profile_image_url": "http://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_link_color": "4F3674", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "4A2334", "profile_text_color": "D5EC08", "screen_name": "BellevueU", "statuses_count": 6051, "url": "https://t.co/0hQEZBjUQK", "withheld_in_countries": []}, "user_mentions": [{"id": 19129143, "id_str": "19129143", "name": "MaryFoster", "screen_name": "MaryFoster"}]}</t>
@@ -70,16 +70,16 @@
     <t>{"created_at": "Sun Jul 25 01:30:49 +0000 2021", "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}], "id": 1419107838325047298, "id_str": "1419107838325047298", "lang": "en", "media": [{"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979419151077382, "media_url": "http://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "sizes": {"large": {"h": 1195, "resize": "fit", "w": 2048}, "medium": {"h": 700, "resize": "fit", "w": 1200}, "small": {"h": 397, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979442421112838, "media_url": "http://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "sizes": {"large": {"h": 1334, "resize": "fit", "w": 1424}, "medium": {"h": 1124, "resize": "fit", "w": 1200}, "small": {"h": 637, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979467846950919, "media_url": "http://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "sizes": {"large": {"h": 1540, "resize": "fit", "w": 1508}, "medium": {"h": 1200, "resize": "fit", "w": 1175}, "small": {"h": 680, "resize": "fit", "w": 666}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}], "retweet_count": 4, "retweeted_status": {"created_at": "Sat Jul 24 17:00:45 +0000 2021", "favorite_count": 22, "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}], "id": 1418979477061779468, "id_str": "1418979477061779468", "lang": "en", "media": [{"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979419151077382, "media_url": "http://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "sizes": {"large": {"h": 1195, "resize": "fit", "w": 2048}, "medium": {"h": 700, "resize": "fit", "w": 1200}, "small": {"h": 397, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979442421112838, "media_url": "http://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "sizes": {"large": {"h": 1334, "resize": "fit", "w": 1424}, "medium": {"h": 1124, "resize": "fit", "w": 1200}, "small": {"h": 637, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979467846950919, "media_url": "http://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "sizes": {"large": {"h": 1540, "resize": "fit", "w": 1508}, "medium": {"h": 1200, "resize": "fit", "w": 1175}, "small": {"h": 680, "resize": "fit", "w": 666}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}], "retweet_count": 4, "source": "&lt;a href=\"http://gainapp.com\" rel=\"nofollow\"&gt;Gain Platform&lt;/a&gt;", "text": "The beginning of a beautiful partnership! \u26bd\ufe0f\ud83d\udc3b\n\n#USL \n#BellevueUniversity https://t.co/zQsYiwWPfO", "urls": [], "user": {"created_at": "Tue Oct 23 13:48:23 +0000 2007", "description": "Our learning programs combine mastery of deep, career-relevant knowledge and powerful professional skills, so you are prepared with tools for success.", "favourites_count": 4123, "followers_count": 9169, "friends_count": 2576, "id": 9623092, "id_str": "9623092", "listed_count": 210, "location": "Nebraska", "name": "Bellevue University", "profile_background_color": "4F3674", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/9623092/1614634074", "profile_image_url": "http://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_link_color": "4F3674", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "4A2334", "profile_text_color": "D5EC08", "screen_name": "BellevueU", "statuses_count": 6051, "url": "https://t.co/0hQEZBjUQK", "withheld_in_countries": []}, "user_mentions": []}, "source": "&lt;a href=\"http://twitter.com/download/android\" rel=\"nofollow\"&gt;Twitter for Android&lt;/a&gt;", "text": "RT @BellevueU: The beginning of a beautiful partnership! \u26bd\ufe0f\ud83d\udc3b\n\n#USL \n#BellevueUniversity https://t.co/zQsYiwWPfO", "urls": [], "user": {"created_at": "Thu Mar 05 16:35:51 +0000 2009", "description": "Certified Personal/Executive Coach, Fundraiser, former Zookeeper, avid reader, walker and dog lover.", "favourites_count": 3850, "followers_count": 376, "friends_count": 1627, "id": 22940541, "id_str": "22940541", "listed_count": 7, "location": "Omaha, NE", "name": "Lisa C Jorgensen", "profile_background_color": "9266CC", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_image_url": "http://pbs.twimg.com/profile_images/2264057530/5z22ci8cxms8jd07knh9_normal.jpeg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/2264057530/5z22ci8cxms8jd07knh9_normal.jpeg", "profile_link_color": "9266CC", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "pizzalisa", "statuses_count": 1445, "withheld_in_countries": []}, "user_mentions": [{"id": 9623092, "id_str": "9623092", "name": "Bellevue University", "screen_name": "BellevueU"}]}</t>
   </si>
   <si>
-    <t>{"created_at": "Sat Jul 24 22:14:55 +0000 2021", "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}], "id": 1419058538832355332, "id_str": "1419058538832355332", "lang": "en", "media": [{"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979419151077382, "media_url": "http://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "sizes": {"large": {"h": 1195, "resize": "fit", "w": 2048}, "medium": {"h": 700, "resize": "fit", "w": 1200}, "small": {"h": 397, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979442421112838, "media_url": "http://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "sizes": {"large": {"h": 1334, "resize": "fit", "w": 1424}, "medium": {"h": 1124, "resize": "fit", "w": 1200}, "small": {"h": 637, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979467846950919, "media_url": "http://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "sizes": {"large": {"h": 1540, "resize": "fit", "w": 1508}, "medium": {"h": 1200, "resize": "fit", "w": 1175}, "small": {"h": 680, "resize": "fit", "w": 666}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}], "retweet_count": 4, "retweeted_status": {"created_at": "Sat Jul 24 17:00:45 +0000 2021", "favorite_count": 22, "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}], "id": 1418979477061779468, "id_str": "1418979477061779468", "lang": "en", "media": [{"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979419151077382, "media_url": "http://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "sizes": {"large": {"h": 1195, "resize": "fit", "w": 2048}, "medium": {"h": 700, "resize": "fit", "w": 1200}, "small": {"h": 397, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979442421112838, "media_url": "http://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "sizes": {"large": {"h": 1334, "resize": "fit", "w": 1424}, "medium": {"h": 1124, "resize": "fit", "w": 1200}, "small": {"h": 637, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979467846950919, "media_url": "http://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "sizes": {"large": {"h": 1540, "resize": "fit", "w": 1508}, "medium": {"h": 1200, "resize": "fit", "w": 1175}, "small": {"h": 680, "resize": "fit", "w": 666}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}], "retweet_count": 4, "source": "&lt;a href=\"http://gainapp.com\" rel=\"nofollow\"&gt;Gain Platform&lt;/a&gt;", "text": "The beginning of a beautiful partnership! \u26bd\ufe0f\ud83d\udc3b\n\n#USL \n#BellevueUniversity https://t.co/zQsYiwWPfO", "urls": [], "user": {"created_at": "Tue Oct 23 13:48:23 +0000 2007", "description": "Our learning programs combine mastery of deep, career-relevant knowledge and powerful professional skills, so you are prepared with tools for success.", "favourites_count": 4123, "followers_count": 9169, "friends_count": 2576, "id": 9623092, "id_str": "9623092", "listed_count": 210, "location": "Nebraska", "name": "Bellevue University", "profile_background_color": "4F3674", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/9623092/1614634074", "profile_image_url": "http://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_link_color": "4F3674", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "4A2334", "profile_text_color": "D5EC08", "screen_name": "BellevueU", "statuses_count": 6051, "url": "https://t.co/0hQEZBjUQK", "withheld_in_countries": []}, "user_mentions": []}, "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "RT @BellevueU: The beginning of a beautiful partnership! \u26bd\ufe0f\ud83d\udc3b\n\n#USL \n#BellevueUniversity https://t.co/zQsYiwWPfO", "urls": [], "user": {"created_at": "Tue Apr 06 19:27:15 +0000 2021", "default_profile": true, "description": "\u2022 Bellevue Men\u2019s Basketball \ud83d\udc3b \u2022 Follow My Gaming Twitter: @vbdagoat", "favourites_count": 3861, "followers_count": 58, "friends_count": 94, "geo_enabled": true, "id": 1379516021598396417, "id_str": "1379516021598396417", "location": "Bellevue, NE", "name": "Vinny Belcaster", "profile_background_color": "F5F8FA", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1379516021598396417/1617738969", "profile_image_url": "http://pbs.twimg.com/profile_images/1379516277631246337/FYa99Ucn_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1379516277631246337/FYa99Ucn_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "belcaster_vinny", "statuses_count": 1410, "withheld_in_countries": []}, "user_mentions": [{"id": 9623092, "id_str": "9623092", "name": "Bellevue University", "screen_name": "BellevueU"}]}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Sat Jul 24 17:09:44 +0000 2021", "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}], "id": 1418981736759894020, "id_str": "1418981736759894020", "lang": "en", "media": [{"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979419151077382, "media_url": "http://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "sizes": {"large": {"h": 1195, "resize": "fit", "w": 2048}, "medium": {"h": 700, "resize": "fit", "w": 1200}, "small": {"h": 397, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979442421112838, "media_url": "http://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "sizes": {"large": {"h": 1334, "resize": "fit", "w": 1424}, "medium": {"h": 1124, "resize": "fit", "w": 1200}, "small": {"h": 637, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979467846950919, "media_url": "http://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "sizes": {"large": {"h": 1540, "resize": "fit", "w": 1508}, "medium": {"h": 1200, "resize": "fit", "w": 1175}, "small": {"h": 680, "resize": "fit", "w": 666}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}], "retweet_count": 4, "retweeted_status": {"created_at": "Sat Jul 24 17:00:45 +0000 2021", "favorite_count": 22, "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}], "id": 1418979477061779468, "id_str": "1418979477061779468", "lang": "en", "media": [{"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979419151077382, "media_url": "http://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "sizes": {"large": {"h": 1195, "resize": "fit", "w": 2048}, "medium": {"h": 700, "resize": "fit", "w": 1200}, "small": {"h": 397, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979442421112838, "media_url": "http://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "sizes": {"large": {"h": 1334, "resize": "fit", "w": 1424}, "medium": {"h": 1124, "resize": "fit", "w": 1200}, "small": {"h": 637, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979467846950919, "media_url": "http://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "sizes": {"large": {"h": 1540, "resize": "fit", "w": 1508}, "medium": {"h": 1200, "resize": "fit", "w": 1175}, "small": {"h": 680, "resize": "fit", "w": 666}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}], "retweet_count": 4, "source": "&lt;a href=\"http://gainapp.com\" rel=\"nofollow\"&gt;Gain Platform&lt;/a&gt;", "text": "The beginning of a beautiful partnership! \u26bd\ufe0f\ud83d\udc3b\n\n#USL \n#BellevueUniversity https://t.co/zQsYiwWPfO", "urls": [], "user": {"created_at": "Tue Oct 23 13:48:23 +0000 2007", "description": "Our learning programs combine mastery of deep, career-relevant knowledge and powerful professional skills, so you are prepared with tools for success.", "favourites_count": 4123, "followers_count": 9169, "friends_count": 2576, "id": 9623092, "id_str": "9623092", "listed_count": 210, "location": "Nebraska", "name": "Bellevue University", "profile_background_color": "4F3674", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/9623092/1614634074", "profile_image_url": "http://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_link_color": "4F3674", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "4A2334", "profile_text_color": "D5EC08", "screen_name": "BellevueU", "statuses_count": 6051, "url": "https://t.co/0hQEZBjUQK", "withheld_in_countries": []}, "user_mentions": []}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @BellevueU: The beginning of a beautiful partnership! \u26bd\ufe0f\ud83d\udc3b\n\n#USL \n#BellevueUniversity https://t.co/zQsYiwWPfO", "urls": [], "user": {"created_at": "Sat Oct 05 14:39:11 +0000 2013", "default_profile": true, "description": "CHRIST Follower\ud83d\udd46. AC at Bellevue University WBB, RETRO HOOPS founder &amp; Coach.Husband, Father, Grandfather,Brother. Born &amp; Raised in TheD #missingoliviaforever", "favourites_count": 96582, "followers_count": 2379, "friends_count": 5000, "geo_enabled": true, "id": 1937867113, "id_str": "1937867113", "listed_count": 1, "location": "The D", "name": "COACH ICE/Bellevue University/RETRO HOOPS", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1937867113/1567087983", "profile_image_url": "http://pbs.twimg.com/profile_images/1382546624073900034/XFjoaHhL_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1382546624073900034/XFjoaHhL_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "thinmanx11", "statuses_count": 48227, "withheld_in_countries": []}, "user_mentions": [{"id": 9623092, "id_str": "9623092", "name": "Bellevue University", "screen_name": "BellevueU"}]}</t>
+    <t>{"created_at": "Sat Jul 24 22:14:55 +0000 2021", "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}], "id": 1419058538832355332, "id_str": "1419058538832355332", "lang": "en", "media": [{"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979419151077382, "media_url": "http://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "sizes": {"large": {"h": 1195, "resize": "fit", "w": 2048}, "medium": {"h": 700, "resize": "fit", "w": 1200}, "small": {"h": 397, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979442421112838, "media_url": "http://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "sizes": {"large": {"h": 1334, "resize": "fit", "w": 1424}, "medium": {"h": 1124, "resize": "fit", "w": 1200}, "small": {"h": 637, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979467846950919, "media_url": "http://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "sizes": {"large": {"h": 1540, "resize": "fit", "w": 1508}, "medium": {"h": 1200, "resize": "fit", "w": 1175}, "small": {"h": 680, "resize": "fit", "w": 666}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}], "retweet_count": 4, "retweeted_status": {"created_at": "Sat Jul 24 17:00:45 +0000 2021", "favorite_count": 22, "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}], "id": 1418979477061779468, "id_str": "1418979477061779468", "lang": "en", "media": [{"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979419151077382, "media_url": "http://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "sizes": {"large": {"h": 1195, "resize": "fit", "w": 2048}, "medium": {"h": 700, "resize": "fit", "w": 1200}, "small": {"h": 397, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979442421112838, "media_url": "http://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "sizes": {"large": {"h": 1334, "resize": "fit", "w": 1424}, "medium": {"h": 1124, "resize": "fit", "w": 1200}, "small": {"h": 637, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979467846950919, "media_url": "http://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "sizes": {"large": {"h": 1540, "resize": "fit", "w": 1508}, "medium": {"h": 1200, "resize": "fit", "w": 1175}, "small": {"h": 680, "resize": "fit", "w": 666}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}], "retweet_count": 4, "source": "&lt;a href=\"http://gainapp.com\" rel=\"nofollow\"&gt;Gain Platform&lt;/a&gt;", "text": "The beginning of a beautiful partnership! \u26bd\ufe0f\ud83d\udc3b\n\n#USL \n#BellevueUniversity https://t.co/zQsYiwWPfO", "urls": [], "user": {"created_at": "Tue Oct 23 13:48:23 +0000 2007", "description": "Our learning programs combine mastery of deep, career-relevant knowledge and powerful professional skills, so you are prepared with tools for success.", "favourites_count": 4123, "followers_count": 9169, "friends_count": 2576, "id": 9623092, "id_str": "9623092", "listed_count": 210, "location": "Nebraska", "name": "Bellevue University", "profile_background_color": "4F3674", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/9623092/1614634074", "profile_image_url": "http://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_link_color": "4F3674", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "4A2334", "profile_text_color": "D5EC08", "screen_name": "BellevueU", "statuses_count": 6051, "url": "https://t.co/0hQEZBjUQK", "withheld_in_countries": []}, "user_mentions": []}, "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "RT @BellevueU: The beginning of a beautiful partnership! \u26bd\ufe0f\ud83d\udc3b\n\n#USL \n#BellevueUniversity https://t.co/zQsYiwWPfO", "urls": [], "user": {"created_at": "Tue Apr 06 19:27:15 +0000 2021", "default_profile": true, "description": "\u2022 Bellevue Men\u2019s Basketball \ud83d\udc3b \u2022 Follow My Gaming Twitter: @vbdagoat", "favourites_count": 3880, "followers_count": 58, "friends_count": 94, "geo_enabled": true, "id": 1379516021598396417, "id_str": "1379516021598396417", "location": "Bellevue, NE", "name": "Vinny Belcaster", "profile_background_color": "F5F8FA", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1379516021598396417/1617738969", "profile_image_url": "http://pbs.twimg.com/profile_images/1379516277631246337/FYa99Ucn_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1379516277631246337/FYa99Ucn_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "belcaster_vinny", "statuses_count": 1421, "withheld_in_countries": []}, "user_mentions": [{"id": 9623092, "id_str": "9623092", "name": "Bellevue University", "screen_name": "BellevueU"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Sat Jul 24 17:09:44 +0000 2021", "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}], "id": 1418981736759894020, "id_str": "1418981736759894020", "lang": "en", "media": [{"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979419151077382, "media_url": "http://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "sizes": {"large": {"h": 1195, "resize": "fit", "w": 2048}, "medium": {"h": 700, "resize": "fit", "w": 1200}, "small": {"h": 397, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979442421112838, "media_url": "http://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "sizes": {"large": {"h": 1334, "resize": "fit", "w": 1424}, "medium": {"h": 1124, "resize": "fit", "w": 1200}, "small": {"h": 637, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979467846950919, "media_url": "http://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "sizes": {"large": {"h": 1540, "resize": "fit", "w": 1508}, "medium": {"h": 1200, "resize": "fit", "w": 1175}, "small": {"h": 680, "resize": "fit", "w": 666}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}], "retweet_count": 4, "retweeted_status": {"created_at": "Sat Jul 24 17:00:45 +0000 2021", "favorite_count": 22, "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}], "id": 1418979477061779468, "id_str": "1418979477061779468", "lang": "en", "media": [{"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979419151077382, "media_url": "http://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "sizes": {"large": {"h": 1195, "resize": "fit", "w": 2048}, "medium": {"h": 700, "resize": "fit", "w": 1200}, "small": {"h": 397, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979442421112838, "media_url": "http://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "sizes": {"large": {"h": 1334, "resize": "fit", "w": 1424}, "medium": {"h": 1124, "resize": "fit", "w": 1200}, "small": {"h": 637, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979467846950919, "media_url": "http://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "sizes": {"large": {"h": 1540, "resize": "fit", "w": 1508}, "medium": {"h": 1200, "resize": "fit", "w": 1175}, "small": {"h": 680, "resize": "fit", "w": 666}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}], "retweet_count": 4, "source": "&lt;a href=\"http://gainapp.com\" rel=\"nofollow\"&gt;Gain Platform&lt;/a&gt;", "text": "The beginning of a beautiful partnership! \u26bd\ufe0f\ud83d\udc3b\n\n#USL \n#BellevueUniversity https://t.co/zQsYiwWPfO", "urls": [], "user": {"created_at": "Tue Oct 23 13:48:23 +0000 2007", "description": "Our learning programs combine mastery of deep, career-relevant knowledge and powerful professional skills, so you are prepared with tools for success.", "favourites_count": 4123, "followers_count": 9169, "friends_count": 2576, "id": 9623092, "id_str": "9623092", "listed_count": 210, "location": "Nebraska", "name": "Bellevue University", "profile_background_color": "4F3674", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/9623092/1614634074", "profile_image_url": "http://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_link_color": "4F3674", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "4A2334", "profile_text_color": "D5EC08", "screen_name": "BellevueU", "statuses_count": 6051, "url": "https://t.co/0hQEZBjUQK", "withheld_in_countries": []}, "user_mentions": []}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @BellevueU: The beginning of a beautiful partnership! \u26bd\ufe0f\ud83d\udc3b\n\n#USL \n#BellevueUniversity https://t.co/zQsYiwWPfO", "urls": [], "user": {"created_at": "Sat Oct 05 14:39:11 +0000 2013", "default_profile": true, "description": "CHRIST Follower\ud83d\udd46. AC at Bellevue University WBB, RETRO HOOPS founder &amp; Coach.Husband, Father, Grandfather,Brother. Born &amp; Raised in TheD #missingoliviaforever", "favourites_count": 96591, "followers_count": 2379, "friends_count": 4999, "geo_enabled": true, "id": 1937867113, "id_str": "1937867113", "listed_count": 1, "location": "The D", "name": "COACH ICE/Bellevue University/RETRO HOOPS", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1937867113/1567087983", "profile_image_url": "http://pbs.twimg.com/profile_images/1382546624073900034/XFjoaHhL_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1382546624073900034/XFjoaHhL_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "thinmanx11", "statuses_count": 48227, "withheld_in_countries": []}, "user_mentions": [{"id": 9623092, "id_str": "9623092", "name": "Bellevue University", "screen_name": "BellevueU"}]}</t>
   </si>
   <si>
     <t>{"created_at": "Sat Jul 24 17:00:45 +0000 2021", "favorite_count": 22, "hashtags": [{"text": "USL"}, {"text": "BellevueUniversity"}], "id": 1418979477061779468, "id_str": "1418979477061779468", "lang": "en", "media": [{"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979419151077382, "media_url": "http://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6Q34XEAYC9C1.jpg", "sizes": {"large": {"h": 1195, "resize": "fit", "w": 2048}, "medium": {"h": 700, "resize": "fit", "w": 1200}, "small": {"h": 397, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979442421112838, "media_url": "http://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6SOkXoAYj4cI.jpg", "sizes": {"large": {"h": 1334, "resize": "fit", "w": 1424}, "medium": {"h": 1124, "resize": "fit", "w": 1200}, "small": {"h": 637, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}, {"display_url": "pic.twitter.com/zQsYiwWPfO", "expanded_url": "https://twitter.com/BellevueU/status/1418979477061779468/photo/1", "id": 1418979467846950919, "media_url": "http://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "media_url_https": "https://pbs.twimg.com/media/E7E6TtSXIAcP9p7.jpg", "sizes": {"large": {"h": 1540, "resize": "fit", "w": 1508}, "medium": {"h": 1200, "resize": "fit", "w": 1175}, "small": {"h": 680, "resize": "fit", "w": 666}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/zQsYiwWPfO"}], "retweet_count": 4, "source": "&lt;a href=\"http://gainapp.com\" rel=\"nofollow\"&gt;Gain Platform&lt;/a&gt;", "text": "The beginning of a beautiful partnership! \u26bd\ufe0f\ud83d\udc3b\n\n#USL \n#BellevueUniversity https://t.co/zQsYiwWPfO", "urls": [], "user": {"created_at": "Tue Oct 23 13:48:23 +0000 2007", "description": "Our learning programs combine mastery of deep, career-relevant knowledge and powerful professional skills, so you are prepared with tools for success.", "favourites_count": 4123, "followers_count": 9169, "friends_count": 2576, "id": 9623092, "id_str": "9623092", "listed_count": 210, "location": "Nebraska", "name": "Bellevue University", "profile_background_color": "4F3674", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/9623092/1614634074", "profile_image_url": "http://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_link_color": "4F3674", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "4A2334", "profile_text_color": "D5EC08", "screen_name": "BellevueU", "statuses_count": 6051, "url": "https://t.co/0hQEZBjUQK", "withheld_in_countries": []}, "user_mentions": []}</t>
   </si>
   <si>
-    <t>{"created_at": "Fri Jul 23 23:38:56 +0000 2021", "hashtags": [{"text": "IllbeThereForYou"}, {"text": "BUGrads"}, {"text": "Family"}, {"text": "BellevueUniversity"}], "id": 1418717295547924481, "id_str": "1418717295547924481", "lang": "en", "media": [{"display_url": "pic.twitter.com/juWVH1XCfv", "expanded_url": "https://twitter.com/BellevueU/status/1418254807412916228/photo/1", "id": 1418254785170612224, "media_url": "http://pbs.twimg.com/media/E66nNn8XoAAGXmI.jpg", "media_url_https": "https://pbs.twimg.com/media/E66nNn8XoAAGXmI.jpg", "sizes": {"large": {"h": 436, "resize": "fit", "w": 822}, "medium": {"h": 436, "resize": "fit", "w": 822}, "small": {"h": 361, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/juWVH1XCfv"}, {"display_url": "pic.twitter.com/juWVH1XCfv", "expanded_url": "https://twitter.com/BellevueU/status/1418254807412916228/photo/1", "id": 1418254791701114884, "media_url": "http://pbs.twimg.com/media/E66nOARXMAQHVtU.jpg", "media_url_https": "https://pbs.twimg.com/media/E66nOARXMAQHVtU.jpg", "sizes": {"large": {"h": 797, "resize": "fit", "w": 828}, "medium": {"h": 797, "resize": "fit", "w": 828}, "small": {"h": 655, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/juWVH1XCfv"}, {"display_url": "pic.twitter.com/juWVH1XCfv", "expanded_url": "https://twitter.com/BellevueU/status/1418254807412916228/photo/1", "id": 1418254804044890113, "media_url": "http://pbs.twimg.com/media/E66nOuQWQAEgaFF.jpg", "media_url_https": "https://pbs.twimg.com/media/E66nOuQWQAEgaFF.jpg", "sizes": {"large": {"h": 802, "resize": "fit", "w": 828}, "medium": {"h": 802, "resize": "fit", "w": 828}, "small": {"h": 659, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/juWVH1XCfv"}], "retweet_count": 1, "retweeted_status": {"created_at": "Thu Jul 22 17:01:10 +0000 2021", "favorite_count": 5, "hashtags": [{"text": "IllbeThereForYou"}, {"text": "BUGrads"}, {"text": "Family"}, {"text": "BellevueUniversity"}], "id": 1418254807412916228, "id_str": "1418254807412916228", "lang": "en", "media": [{"display_url": "pic.twitter.com/juWVH1XCfv", "expanded_url": "https://twitter.com/BellevueU/status/1418254807412916228/photo/1", "id": 1418254785170612224, "media_url": "http://pbs.twimg.com/media/E66nNn8XoAAGXmI.jpg", "media_url_https": "https://pbs.twimg.com/media/E66nNn8XoAAGXmI.jpg", "sizes": {"large": {"h": 436, "resize": "fit", "w": 822}, "medium": {"h": 436, "resize": "fit", "w": 822}, "small": {"h": 361, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/juWVH1XCfv"}, {"display_url": "pic.twitter.com/juWVH1XCfv", "expanded_url": "https://twitter.com/BellevueU/status/1418254807412916228/photo/1", "id": 1418254791701114884, "media_url": "http://pbs.twimg.com/media/E66nOARXMAQHVtU.jpg", "media_url_https": "https://pbs.twimg.com/media/E66nOARXMAQHVtU.jpg", "sizes": {"large": {"h": 797, "resize": "fit", "w": 828}, "medium": {"h": 797, "resize": "fit", "w": 828}, "small": {"h": 655, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/juWVH1XCfv"}, {"display_url": "pic.twitter.com/juWVH1XCfv", "expanded_url": "https://twitter.com/BellevueU/status/1418254807412916228/photo/1", "id": 1418254804044890113, "media_url": "http://pbs.twimg.com/media/E66nOuQWQAEgaFF.jpg", "media_url_https": "https://pbs.twimg.com/media/E66nOuQWQAEgaFF.jpg", "sizes": {"large": {"h": 802, "resize": "fit", "w": 828}, "medium": {"h": 802, "resize": "fit", "w": 828}, "small": {"h": 659, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/juWVH1XCfv"}], "retweet_count": 1, "source": "&lt;a href=\"http://gainapp.com\" rel=\"nofollow\"&gt;Gain Platform&lt;/a&gt;", "text": "The one where we all graduate \ud83c\udf93\n\n#IllbeThereForYou #BUGrads #Family #BellevueUniversity https://t.co/juWVH1XCfv", "urls": [], "user": {"created_at": "Tue Oct 23 13:48:23 +0000 2007", "description": "Our learning programs combine mastery of deep, career-relevant knowledge and powerful professional skills, so you are prepared with tools for success.", "favourites_count": 4123, "followers_count": 9169, "friends_count": 2576, "id": 9623092, "id_str": "9623092", "listed_count": 210, "location": "Nebraska", "name": "Bellevue University", "profile_background_color": "4F3674", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/9623092/1614634074", "profile_image_url": "http://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_link_color": "4F3674", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "4A2334", "profile_text_color": "D5EC08", "screen_name": "BellevueU", "statuses_count": 6051, "url": "https://t.co/0hQEZBjUQK", "withheld_in_countries": []}, "user_mentions": []}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @BellevueU: The one where we all graduate \ud83c\udf93\n\n#IllbeThereForYou #BUGrads #Family #BellevueUniversity https://t.co/juWVH1XCfv", "urls": [], "user": {"created_at": "Fri Jul 05 00:46:32 +0000 2013", "default_profile": true, "description": "Prevent the Impact of Virtual Stalking's goal is to raise awareness through socialmedia activism.", "favourites_count": 50856, "followers_count": 693, "friends_count": 2116, "id": 1569393812, "id_str": "1569393812", "listed_count": 136, "name": "PSIVS", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1569393812/1393541909", "profile_image_url": "http://pbs.twimg.com/profile_images/378800000089056418/fd509d51f1648f0cf1b923bb5bad63f6_normal.jpeg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/378800000089056418/fd509d51f1648f0cf1b923bb5bad63f6_normal.jpeg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "StopVirtuaStalk", "statuses_count": 118750, "url": "http://t.co/MJqBSekNQm", "withheld_in_countries": []}, "user_mentions": [{"id": 9623092, "id_str": "9623092", "name": "Bellevue University", "screen_name": "BellevueU"}]}</t>
+    <t>{"created_at": "Fri Jul 23 23:38:56 +0000 2021", "hashtags": [{"text": "IllbeThereForYou"}, {"text": "BUGrads"}, {"text": "Family"}, {"text": "BellevueUniversity"}], "id": 1418717295547924481, "id_str": "1418717295547924481", "lang": "en", "media": [{"display_url": "pic.twitter.com/juWVH1XCfv", "expanded_url": "https://twitter.com/BellevueU/status/1418254807412916228/photo/1", "id": 1418254785170612224, "media_url": "http://pbs.twimg.com/media/E66nNn8XoAAGXmI.jpg", "media_url_https": "https://pbs.twimg.com/media/E66nNn8XoAAGXmI.jpg", "sizes": {"large": {"h": 436, "resize": "fit", "w": 822}, "medium": {"h": 436, "resize": "fit", "w": 822}, "small": {"h": 361, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/juWVH1XCfv"}, {"display_url": "pic.twitter.com/juWVH1XCfv", "expanded_url": "https://twitter.com/BellevueU/status/1418254807412916228/photo/1", "id": 1418254791701114884, "media_url": "http://pbs.twimg.com/media/E66nOARXMAQHVtU.jpg", "media_url_https": "https://pbs.twimg.com/media/E66nOARXMAQHVtU.jpg", "sizes": {"large": {"h": 797, "resize": "fit", "w": 828}, "medium": {"h": 797, "resize": "fit", "w": 828}, "small": {"h": 655, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/juWVH1XCfv"}, {"display_url": "pic.twitter.com/juWVH1XCfv", "expanded_url": "https://twitter.com/BellevueU/status/1418254807412916228/photo/1", "id": 1418254804044890113, "media_url": "http://pbs.twimg.com/media/E66nOuQWQAEgaFF.jpg", "media_url_https": "https://pbs.twimg.com/media/E66nOuQWQAEgaFF.jpg", "sizes": {"large": {"h": 802, "resize": "fit", "w": 828}, "medium": {"h": 802, "resize": "fit", "w": 828}, "small": {"h": 659, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/juWVH1XCfv"}], "retweet_count": 1, "retweeted_status": {"created_at": "Thu Jul 22 17:01:10 +0000 2021", "favorite_count": 5, "hashtags": [{"text": "IllbeThereForYou"}, {"text": "BUGrads"}, {"text": "Family"}, {"text": "BellevueUniversity"}], "id": 1418254807412916228, "id_str": "1418254807412916228", "lang": "en", "media": [{"display_url": "pic.twitter.com/juWVH1XCfv", "expanded_url": "https://twitter.com/BellevueU/status/1418254807412916228/photo/1", "id": 1418254785170612224, "media_url": "http://pbs.twimg.com/media/E66nNn8XoAAGXmI.jpg", "media_url_https": "https://pbs.twimg.com/media/E66nNn8XoAAGXmI.jpg", "sizes": {"large": {"h": 436, "resize": "fit", "w": 822}, "medium": {"h": 436, "resize": "fit", "w": 822}, "small": {"h": 361, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/juWVH1XCfv"}, {"display_url": "pic.twitter.com/juWVH1XCfv", "expanded_url": "https://twitter.com/BellevueU/status/1418254807412916228/photo/1", "id": 1418254791701114884, "media_url": "http://pbs.twimg.com/media/E66nOARXMAQHVtU.jpg", "media_url_https": "https://pbs.twimg.com/media/E66nOARXMAQHVtU.jpg", "sizes": {"large": {"h": 797, "resize": "fit", "w": 828}, "medium": {"h": 797, "resize": "fit", "w": 828}, "small": {"h": 655, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/juWVH1XCfv"}, {"display_url": "pic.twitter.com/juWVH1XCfv", "expanded_url": "https://twitter.com/BellevueU/status/1418254807412916228/photo/1", "id": 1418254804044890113, "media_url": "http://pbs.twimg.com/media/E66nOuQWQAEgaFF.jpg", "media_url_https": "https://pbs.twimg.com/media/E66nOuQWQAEgaFF.jpg", "sizes": {"large": {"h": 802, "resize": "fit", "w": 828}, "medium": {"h": 802, "resize": "fit", "w": 828}, "small": {"h": 659, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/juWVH1XCfv"}], "retweet_count": 1, "source": "&lt;a href=\"http://gainapp.com\" rel=\"nofollow\"&gt;Gain Platform&lt;/a&gt;", "text": "The one where we all graduate \ud83c\udf93\n\n#IllbeThereForYou #BUGrads #Family #BellevueUniversity https://t.co/juWVH1XCfv", "urls": [], "user": {"created_at": "Tue Oct 23 13:48:23 +0000 2007", "description": "Our learning programs combine mastery of deep, career-relevant knowledge and powerful professional skills, so you are prepared with tools for success.", "favourites_count": 4123, "followers_count": 9169, "friends_count": 2576, "id": 9623092, "id_str": "9623092", "listed_count": 210, "location": "Nebraska", "name": "Bellevue University", "profile_background_color": "4F3674", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/9623092/1614634074", "profile_image_url": "http://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_link_color": "4F3674", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "4A2334", "profile_text_color": "D5EC08", "screen_name": "BellevueU", "statuses_count": 6051, "url": "https://t.co/0hQEZBjUQK", "withheld_in_countries": []}, "user_mentions": []}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @BellevueU: The one where we all graduate \ud83c\udf93\n\n#IllbeThereForYou #BUGrads #Family #BellevueUniversity https://t.co/juWVH1XCfv", "urls": [], "user": {"created_at": "Fri Jul 05 00:46:32 +0000 2013", "default_profile": true, "description": "Prevent the Impact of Virtual Stalking's goal is to raise awareness through socialmedia activism.", "favourites_count": 50850, "followers_count": 692, "friends_count": 2113, "id": 1569393812, "id_str": "1569393812", "listed_count": 136, "name": "PSIVS", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1569393812/1393541909", "profile_image_url": "http://pbs.twimg.com/profile_images/378800000089056418/fd509d51f1648f0cf1b923bb5bad63f6_normal.jpeg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/378800000089056418/fd509d51f1648f0cf1b923bb5bad63f6_normal.jpeg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "StopVirtuaStalk", "statuses_count": 118750, "url": "http://t.co/MJqBSekNQm", "withheld_in_countries": []}, "user_mentions": [{"id": 9623092, "id_str": "9623092", "name": "Bellevue University", "screen_name": "BellevueU"}]}</t>
   </si>
   <si>
     <t>{"created_at": "Fri Jul 23 20:01:06 +0000 2021", "hashtags": [{"text": "BellevueUniversity"}, {"text": "BUBruins"}, {"text": "FindajobFriday"}], "id": 1418662474551865346, "id_str": "1418662474551865346", "lang": "en", "source": "&lt;a href=\"https://www.hootsuite.com\" rel=\"nofollow\"&gt;Hootsuite Inc.&lt;/a&gt;", "text": "Ace the Entry Level Job Interview &amp;amp; Get the JOB! https://t.co/gmSdnvxxdQ #BellevueUniversity #BUBruins #FindajobFriday", "urls": [{"expanded_url": "http://ow.ly/XL4k50FkWCQ", "url": "https://t.co/gmSdnvxxdQ"}], "user": {"created_at": "Mon May 16 21:44:54 +0000 2016", "default_profile": true, "description": "Our goal is to assist you with making connections, obtaining mentoring opportunities &amp; aid in finding employment that mirrors your desires and qualifications.", "favourites_count": 52, "followers_count": 491, "friends_count": 1518, "id": 732325979520040960, "id_str": "732325979520040960", "listed_count": 20, "location": "Bellevue, NE", "name": "Bellevue University Career Services", "profile_background_color": "F5F8FA", "profile_banner_url": "https://pbs.twimg.com/profile_banners/732325979520040960/1532537010", "profile_image_url": "http://pbs.twimg.com/profile_images/1022160813983850496/GJsD7K0B_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1022160813983850496/GJsD7K0B_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "BUCareer2", "statuses_count": 2923, "withheld_in_countries": []}, "user_mentions": []}</t>
@@ -91,34 +91,40 @@
     <t>{"created_at": "Fri Jul 23 12:08:58 +0000 2021", "hashtags": [{"text": "BellevueUniversity"}], "id": 1418543660044455938, "id_str": "1418543660044455938", "lang": "en", "retweet_count": 1, "retweeted_status": {"created_at": "Thu Jul 22 13:37:52 +0000 2021", "favorite_count": 4, "hashtags": [{"text": "BellevueUniversity"}], "id": 1418203645418553349, "id_str": "1418203645418553349", "lang": "en", "retweet_count": 1, "source": "&lt;a href=\"http://gainapp.com\" rel=\"nofollow\"&gt;Gain Platform&lt;/a&gt;", "text": "Brandi Kindell, a mom and Walmart associate, graduated from #BellevueUniversity, earning her degree for $1 a day th\u2026 https://t.co/4lqsZGJqQ5", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1418203645418553349", "url": "https://t.co/4lqsZGJqQ5"}], "user": {"created_at": "Wed Mar 11 14:27:22 +0000 2009", "description": "We help develop learning programs that align with company goals, fill knowledge and performance gaps, and deliver ROI - with metrics to back it up.", "favourites_count": 706, "followers_count": 1293, "friends_count": 2021, "geo_enabled": true, "id": 23769513, "id_str": "23769513", "listed_count": 30, "location": "Bellevue University", "name": "BU-CorporateLearning", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/23769513/1497622027", "profile_image_url": "http://pbs.twimg.com/profile_images/787019624592224256/_C7AJNrZ_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/787019624592224256/_C7AJNrZ_normal.jpg", "profile_link_color": "000000", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "000000", "profile_text_color": "000000", "screen_name": "corporatelearn", "statuses_count": 3862, "url": "http://t.co/r4QzATkcxC", "withheld_in_countries": []}, "user_mentions": []}, "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "RT @corporatelearn: Brandi Kindell, a mom and Walmart associate, graduated from #BellevueUniversity, earning her degree for $1 a day throug\u2026", "urls": [], "user": {"created_at": "Sun Nov 01 15:16:35 +0000 2009", "description": "Lead, manage, innovate! Vice President, Strategic Partnerships - Bellevue University, Former Vice-Chair of Sarpy County Board, Former Chair Metro College Board.", "favourites_count": 1253, "followers_count": 1257, "friends_count": 1123, "geo_enabled": true, "id": 86739249, "id_str": "86739249", "listed_count": 30, "location": "Bellevue, Nebraska", "name": "Jim Nekuda", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme14/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme14/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/86739249/1530202217", "profile_image_url": "http://pbs.twimg.com/profile_images/1167053077440016384/1lOLBQUx_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1167053077440016384/1lOLBQUx_normal.jpg", "profile_link_color": "981CEB", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "000000", "profile_text_color": "000000", "screen_name": "JimNekuda", "statuses_count": 6612, "url": "https://t.co/kurNnRDPQe", "withheld_in_countries": []}, "user_mentions": [{"id": 23769513, "id_str": "23769513", "name": "BU-CorporateLearning", "screen_name": "corporatelearn"}]}</t>
   </si>
   <si>
-    <t>{"created_at": "Thu Jul 22 17:01:10 +0000 2021", "favorite_count": 5, "hashtags": [{"text": "IllbeThereForYou"}, {"text": "BUGrads"}, {"text": "Family"}, {"text": "BellevueUniversity"}], "id": 1418254807412916228, "id_str": "1418254807412916228", "lang": "en", "media": [{"display_url": "pic.twitter.com/juWVH1XCfv", "expanded_url": "https://twitter.com/BellevueU/status/1418254807412916228/photo/1", "id": 1418254785170612224, "media_url": "http://pbs.twimg.com/media/E66nNn8XoAAGXmI.jpg", "media_url_https": "https://pbs.twimg.com/media/E66nNn8XoAAGXmI.jpg", "sizes": {"large": {"h": 436, "resize": "fit", "w": 822}, "medium": {"h": 436, "resize": "fit", "w": 822}, "small": {"h": 361, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/juWVH1XCfv"}, {"display_url": "pic.twitter.com/juWVH1XCfv", "expanded_url": "https://twitter.com/BellevueU/status/1418254807412916228/photo/1", "id": 1418254791701114884, "media_url": "http://pbs.twimg.com/media/E66nOARXMAQHVtU.jpg", "media_url_https": "https://pbs.twimg.com/media/E66nOARXMAQHVtU.jpg", "sizes": {"large": {"h": 797, "resize": "fit", "w": 828}, "medium": {"h": 797, "resize": "fit", "w": 828}, "small": {"h": 655, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/juWVH1XCfv"}, {"display_url": "pic.twitter.com/juWVH1XCfv", "expanded_url": "https://twitter.com/BellevueU/status/1418254807412916228/photo/1", "id": 1418254804044890113, "media_url": "http://pbs.twimg.com/media/E66nOuQWQAEgaFF.jpg", "media_url_https": "https://pbs.twimg.com/media/E66nOuQWQAEgaFF.jpg", "sizes": {"large": {"h": 802, "resize": "fit", "w": 828}, "medium": {"h": 802, "resize": "fit", "w": 828}, "small": {"h": 659, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/juWVH1XCfv"}], "retweet_count": 1, "source": "&lt;a href=\"http://gainapp.com\" rel=\"nofollow\"&gt;Gain Platform&lt;/a&gt;", "text": "The one where we all graduate \ud83c\udf93\n\n#IllbeThereForYou #BUGrads #Family #BellevueUniversity https://t.co/juWVH1XCfv", "urls": [], "user": {"created_at": "Tue Oct 23 13:48:23 +0000 2007", "description": "Our learning programs combine mastery of deep, career-relevant knowledge and powerful professional skills, so you are prepared with tools for success.", "favourites_count": 4123, "followers_count": 9169, "friends_count": 2576, "id": 9623092, "id_str": "9623092", "listed_count": 210, "location": "Nebraska", "name": "Bellevue University", "profile_background_color": "4F3674", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/9623092/1614634074", "profile_image_url": "http://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_link_color": "4F3674", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "4A2334", "profile_text_color": "D5EC08", "screen_name": "BellevueU", "statuses_count": 6051, "url": "https://t.co/0hQEZBjUQK", "withheld_in_countries": []}, "user_mentions": []}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Fri Jul 30 23:05:10 +0000 2021", "hashtags": [], "id": 1421245514423668739, "id_str": "1421245514423668739", "lang": "en", "retweet_count": 1, "retweeted_status": {"created_at": "Fri Jul 30 23:05:05 +0000 2021", "favorite_count": 6, "hashtags": [], "id": 1421245490558119938, "id_str": "1421245490558119938", "lang": "en", "retweet_count": 1, "source": "&lt;a href=\"https://www.hootsuite.com\" rel=\"nofollow\"&gt;Hootsuite Inc.&lt;/a&gt;", "text": "Thank you to our Omaha intern, Lauren Wiegand! She is from Bellevue, Nebraska and graduated in 2020 from the Univer\u2026 https://t.co/j9pwf13t7i", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1421245490558119938", "url": "https://t.co/j9pwf13t7i"}], "user": {"created_at": "Wed Jan 11 00:17:40 +0000 2017", "description": "Serving the great people of NE-02 \ud83c\uddfa\ud83c\uddf8. Married to Angie, 4 children, 6 grandkids. Brig Gen \u2b50\ufe0f USAF (Ret.) Send questions to our office (link below).", "favourites_count": 11695, "followers_count": 16770, "friends_count": 653, "geo_enabled": true, "id": 818975124460335106, "id_str": "818975124460335106", "listed_count": 569, "location": "Papillion, NE", "name": "Rep. Don Bacon", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/818975124460335106/1540489680", "profile_image_url": "http://pbs.twimg.com/profile_images/1223963541167837186/KXYmFUf5_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1223963541167837186/KXYmFUf5_normal.jpg", "profile_link_color": "E81C4F", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "000000", "profile_text_color": "000000", "screen_name": "RepDonBacon", "statuses_count": 11856, "url": "https://t.co/mkCpzgSdUD", "verified": true, "withheld_in_countries": []}, "user_mentions": []}, "source": "&lt;a href=\"https://nathandharris.com\" rel=\"nofollow\"&gt;All 435 Reps&lt;/a&gt;", "text": "RT @RepDonBacon: Thank you to our Omaha intern, Lauren Wiegand! She is from Bellevue, Nebraska and graduated in 2020 from the University of\u2026", "urls": [], "user": {"created_at": "Fri May 03 22:54:54 +0000 2019", "default_profile": true, "description": "Collecting and retweeting tweets by all members of the US House of Representatives. Archived at: https://t.co/pr8ZcQwGNu", "followers_count": 5419, "friends_count": 746, "id": 1124447266205503488, "id_str": "1124447266205503488", "listed_count": 72, "name": "All 435 Reps", "profile_background_color": "F5F8FA", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1124447266205503488/1556988108", "profile_image_url": "http://pbs.twimg.com/profile_images/1124713248211783680/dISvFwue_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1124713248211783680/dISvFwue_normal.png", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "All435Reps", "statuses_count": 623818, "withheld_in_countries": []}, "user_mentions": [{"id": 818975124460335106, "id_str": "818975124460335106", "name": "Rep. Don Bacon", "screen_name": "RepDonBacon"}]}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Fri Jul 30 23:05:05 +0000 2021", "favorite_count": 6, "hashtags": [], "id": 1421245490558119938, "id_str": "1421245490558119938", "lang": "en", "retweet_count": 1, "source": "&lt;a href=\"https://www.hootsuite.com\" rel=\"nofollow\"&gt;Hootsuite Inc.&lt;/a&gt;", "text": "Thank you to our Omaha intern, Lauren Wiegand! She is from Bellevue, Nebraska and graduated in 2020 from the Univer\u2026 https://t.co/j9pwf13t7i", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1421245490558119938", "url": "https://t.co/j9pwf13t7i"}], "user": {"created_at": "Wed Jan 11 00:17:40 +0000 2017", "description": "Serving the great people of NE-02 \ud83c\uddfa\ud83c\uddf8. Married to Angie, 4 children, 6 grandkids. Brig Gen \u2b50\ufe0f USAF (Ret.) Send questions to our office (link below).", "favourites_count": 11695, "followers_count": 16770, "friends_count": 653, "geo_enabled": true, "id": 818975124460335106, "id_str": "818975124460335106", "listed_count": 569, "location": "Papillion, NE", "name": "Rep. Don Bacon", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/818975124460335106/1540489680", "profile_image_url": "http://pbs.twimg.com/profile_images/1223963541167837186/KXYmFUf5_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1223963541167837186/KXYmFUf5_normal.jpg", "profile_link_color": "E81C4F", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "000000", "profile_text_color": "000000", "screen_name": "RepDonBacon", "statuses_count": 11856, "url": "https://t.co/mkCpzgSdUD", "verified": true, "withheld_in_countries": []}, "user_mentions": []}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Fri Jul 30 09:21:14 +0000 2021", "hashtags": [], "id": 1421038163770892290, "id_str": "1421038163770892290", "lang": "fr", "media": [{"display_url": "pic.twitter.com/WrR091Nk6C", "expanded_url": "https://twitter.com/YoreChart/status/1421038163770892290/photo/1", "id": 1421038162772639744, "media_url": "http://pbs.twimg.com/media/E7iKrhhWQAAMXME.jpg", "media_url_https": "https://pbs.twimg.com/media/E7iKrhhWQAAMXME.jpg", "sizes": {"large": {"h": 570, "resize": "fit", "w": 570}, "medium": {"h": 570, "resize": "fit", "w": 570}, "small": {"h": 570, "resize": "fit", "w": 570}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/WrR091Nk6C"}], "source": "&lt;a href=\"https://ifttt.com\" rel=\"nofollow\"&gt;IFTTT&lt;/a&gt;", "text": "In the minouette shop: Bellevue, NE. Bellevue University Latte Map Mug. by YoreChart at https://t.co/1inqoh6AxY https://t.co/WrR091Nk6C", "urls": [{"expanded_url": "https://ift.tt/3g9dvdf", "url": "https://t.co/1inqoh6AxY"}], "user": {"created_at": "Tue Aug 11 19:43:31 +0000 2020", "default_profile": true, "description": "We Create Custom University Map Products Including Mugs, Latte Mugs, Tumblers, and Custom Premium Prints.", "followers_count": 3, "id": 1293271824180981766, "id_str": "1293271824180981766", "name": "YoreChart", "profile_background_color": "F5F8FA", "profile_image_url": "http://pbs.twimg.com/profile_images/1293272052007227393/98nJCKxl_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1293272052007227393/98nJCKxl_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "YoreChart", "statuses_count": 2414, "withheld_in_countries": []}, "user_mentions": []}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Fri Jul 30 03:23:12 +0000 2021", "hashtags": [], "id": 1420948062755856386, "id_str": "1420948062755856386", "lang": "en", "source": "&lt;a href=\"http://www.socialnewsdesk.com\" rel=\"nofollow\"&gt;SocialNewsDesk&lt;/a&gt;", "text": "Brendon Walker heads to Bellevue University to tee it up for the Bruins https://t.co/3ITWaHURa7", "urls": [{"expanded_url": "https://www.knopnews2.com/2021/07/30/brendon-walker-heads-bellevue-university-tee-it-up-bruins/?utm_campaign=snd-autopilot&amp;utm_source=twitter&amp;utm_medium=social&amp;utm_campaign=snd&amp;utm_content=knop", "url": "https://t.co/3ITWaHURa7"}], "user": {"created_at": "Thu Oct 13 15:28:08 +0000 2011", "default_profile": true, "description": "Official twitter account for @KNOPTV News 2. Be sure to download our KNOP News app.", "favourites_count": 1253, "followers_count": 3027, "friends_count": 830, "geo_enabled": true, "id": 390167719, "id_str": "390167719", "listed_count": 124, "location": "North Platte, NE", "name": "KNOP-TV", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/390167719/1614187690", "profile_image_url": "http://pbs.twimg.com/profile_images/1252290567947632641/v6YZHwIH_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1252290567947632641/v6YZHwIH_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "KNOPTV", "statuses_count": 46114, "url": "http://t.co/b5HFOcv6v6", "verified": true, "withheld_in_countries": []}, "user_mentions": []}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Thu Jul 29 21:13:28 +0000 2021", "favorite_count": 5, "hashtags": [], "id": 1420855014290038785, "id_str": "1420855014290038785", "in_reply_to_screen_name": "OmahaParliament", "in_reply_to_status_id": 1420855010611580936, "in_reply_to_user_id": 1179951924235386881, "lang": "en", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "Let\u2019s help get them closer to their goal!\n\nPledge to donate per goal @Union_Omaha scores July 31-August 31 (note: t\u2026 https://t.co/RIEVpfZQUX", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420855014290038785", "url": "https://t.co/RIEVpfZQUX"}], "user": {"created_at": "Fri Oct 04 02:50:44 +0000 2019", "default_profile": true, "description": "Independent Supporters of @union_omaha! #VivaB\u00fahos #EyesontheOwls\ud83e\udd89\u26bd\ufe0f", "favourites_count": 14504, "followers_count": 1469, "friends_count": 453, "geo_enabled": true, "id": 1179951924235386881, "id_str": "1179951924235386881", "listed_count": 15, "location": "Omaha, NE", "name": "Omaha Parliament", "profile_background_color": "F5F8FA", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1179951924235386881/1626113144", "profile_image_url": "http://pbs.twimg.com/profile_images/1350940153506897921/HmwI2VN3_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1350940153506897921/HmwI2VN3_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "OmahaParliament", "statuses_count": 5021, "url": "https://t.co/QkXTcAz92f", "withheld_in_countries": []}, "user_mentions": [{"id": 1006630180981485568, "id_str": "1006630180981485568", "name": "Union Omaha", "screen_name": "Union_Omaha"}]}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Thu Jul 29 18:00:02 +0000 2021", "hashtags": [], "id": 1420806337986957315, "id_str": "1420806337986957315", "lang": "en", "source": "&lt;a href=\"https://www.townnews.com/\" rel=\"nofollow\"&gt;BLOX CMS&lt;/a&gt;", "text": "COLLEGE DECISION: A joking threat from a neighbor convinced Plattsmouth's Kaleb Wooten to go out for cross country\u2026 https://t.co/t7x4ky26sN", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420806337986957315", "url": "https://t.co/t7x4ky26sN"}], "user": {"created_at": "Tue Sep 06 15:25:28 +0000 2011", "default_profile": true, "description": "Sports in KMAland", "favourites_count": 544, "followers_count": 8487, "friends_count": 600, "id": 368983881, "id_str": "368983881", "listed_count": 33, "location": "KMA land", "name": "KMA Sports", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/368983881/1567604900", "profile_image_url": "http://pbs.twimg.com/profile_images/1032619990925496321/FeU6SO3w_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1032619990925496321/FeU6SO3w_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "KMASports", "statuses_count": 41156, "url": "https://t.co/e1rrr5WNfU", "withheld_in_countries": []}, "user_mentions": []}</t>
+    <t>{"created_at": "Sat Jul 31 02:58:30 +0000 2021", "hashtags": [], "id": 1421304233027067911, "id_str": "1421304233027067911", "lang": "en", "retweet_count": 3, "retweeted_status": {"created_at": "Fri Jul 30 23:05:05 +0000 2021", "favorite_count": 25, "hashtags": [], "id": 1421245490558119938, "id_str": "1421245490558119938", "lang": "en", "retweet_count": 3, "source": "&lt;a href=\"https://www.hootsuite.com\" rel=\"nofollow\"&gt;Hootsuite Inc.&lt;/a&gt;", "text": "Thank you to our Omaha intern, Lauren Wiegand! She is from Bellevue, Nebraska and graduated in 2020 from the Univer\u2026 https://t.co/j9pwf13t7i", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1421245490558119938", "url": "https://t.co/j9pwf13t7i"}], "user": {"created_at": "Wed Jan 11 00:17:40 +0000 2017", "description": "Serving the great people of NE-02 \ud83c\uddfa\ud83c\uddf8. Married to Angie, 4 children, 6 grandkids. Brig Gen \u2b50\ufe0f USAF (Ret.) Send questions to our office (link below).", "favourites_count": 11702, "followers_count": 16773, "friends_count": 653, "geo_enabled": true, "id": 818975124460335106, "id_str": "818975124460335106", "listed_count": 569, "location": "Papillion, NE", "name": "Rep. Don Bacon", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/818975124460335106/1540489680", "profile_image_url": "http://pbs.twimg.com/profile_images/1223963541167837186/KXYmFUf5_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1223963541167837186/KXYmFUf5_normal.jpg", "profile_link_color": "E81C4F", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "000000", "profile_text_color": "000000", "screen_name": "RepDonBacon", "statuses_count": 11869, "url": "https://t.co/mkCpzgSdUD", "verified": true, "withheld_in_countries": []}, "user_mentions": []}, "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "RT @RepDonBacon: Thank you to our Omaha intern, Lauren Wiegand! She is from Bellevue, Nebraska and graduated in 2020 from the University of\u2026", "urls": [], "user": {"created_at": "Fri Mar 06 23:19:31 +0000 2009", "description": "Douglas County Republican Party\n#NE02", "favourites_count": 3385, "followers_count": 1838, "friends_count": 577, "geo_enabled": true, "id": 23134706, "id_str": "23134706", "listed_count": 23, "location": "Omaha, NE", "name": "Douglas County Republican Party", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme14/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme14/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/23134706/1551070879", "profile_image_url": "http://pbs.twimg.com/profile_images/1099896628838916098/iVZEx8Bd_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1099896628838916098/iVZEx8Bd_normal.jpg", "profile_link_color": "E81C4F", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "000000", "profile_text_color": "000000", "screen_name": "dcrponline", "statuses_count": 4788, "url": "https://t.co/PgtCPcuca3", "withheld_in_countries": []}, "user_mentions": [{"id": 818975124460335106, "id_str": "818975124460335106", "name": "Rep. Don Bacon", "screen_name": "RepDonBacon"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Sat Jul 31 02:57:41 +0000 2021", "hashtags": [], "id": 1421304025987883018, "id_str": "1421304025987883018", "lang": "en", "retweet_count": 3, "retweeted_status": {"created_at": "Fri Jul 30 23:05:05 +0000 2021", "favorite_count": 25, "hashtags": [], "id": 1421245490558119938, "id_str": "1421245490558119938", "lang": "en", "retweet_count": 3, "source": "&lt;a href=\"https://www.hootsuite.com\" rel=\"nofollow\"&gt;Hootsuite Inc.&lt;/a&gt;", "text": "Thank you to our Omaha intern, Lauren Wiegand! She is from Bellevue, Nebraska and graduated in 2020 from the Univer\u2026 https://t.co/j9pwf13t7i", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1421245490558119938", "url": "https://t.co/j9pwf13t7i"}], "user": {"created_at": "Wed Jan 11 00:17:40 +0000 2017", "description": "Serving the great people of NE-02 \ud83c\uddfa\ud83c\uddf8. Married to Angie, 4 children, 6 grandkids. Brig Gen \u2b50\ufe0f USAF (Ret.) Send questions to our office (link below).", "favourites_count": 11702, "followers_count": 16773, "friends_count": 653, "geo_enabled": true, "id": 818975124460335106, "id_str": "818975124460335106", "listed_count": 569, "location": "Papillion, NE", "name": "Rep. Don Bacon", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/818975124460335106/1540489680", "profile_image_url": "http://pbs.twimg.com/profile_images/1223963541167837186/KXYmFUf5_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1223963541167837186/KXYmFUf5_normal.jpg", "profile_link_color": "E81C4F", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "000000", "profile_text_color": "000000", "screen_name": "RepDonBacon", "statuses_count": 11869, "url": "https://t.co/mkCpzgSdUD", "verified": true, "withheld_in_countries": []}, "user_mentions": []}, "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "RT @RepDonBacon: Thank you to our Omaha intern, Lauren Wiegand! She is from Bellevue, Nebraska and graduated in 2020 from the University of\u2026", "urls": [], "user": {"created_at": "Tue Dec 02 03:02:34 +0000 2014", "description": "President of WSC Student Senate, WSC Grad 2022. Fmr. @RepAdrianSmith Hillrat. I love Nebraska.", "favourites_count": 189213, "followers_count": 1188, "friends_count": 4717, "id": 2901798442, "id_str": "2901798442", "listed_count": 5, "location": "Hastings, NE / Wayne, NE ", "name": "Blake Aspen", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/2901798442/1626931224", "profile_image_url": "http://pbs.twimg.com/profile_images/1418078451840561154/osKPMQXu_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1418078451840561154/osKPMQXu_normal.jpg", "profile_link_color": "DD2E44", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "000000", "profile_text_color": "000000", "screen_name": "blakeaspenne", "statuses_count": 68437, "withheld_in_countries": []}, "user_mentions": [{"id": 818975124460335106, "id_str": "818975124460335106", "name": "Rep. Don Bacon", "screen_name": "RepDonBacon"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Sat Jul 31 00:21:30 +0000 2021", "hashtags": [], "id": 1421264721257320448, "id_str": "1421264721257320448", "lang": "en", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "HII!!! thank youwu to our omahaww intern, lauren wiegand! she is from bellevue, nebraska and graduated in 2020 from\u2026 https://t.co/YZdihq73gW", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1421264721257320448", "url": "https://t.co/YZdihq73gW"}], "user": {"created_at": "Thu Jun 03 22:18:01 +0000 2021", "default_profile": true, "description": "(\u25e1 \u03c9 \u25e1) ne-02 cawwangressional @repdonbacon &amp; @donjbacon translator bot \u0ca0_\u0ca0  obvious parody (\u00b4\u25c9\u25de\u0c6a\u25df\u25c9)", "favourites_count": 2, "followers_count": 24, "friends_count": 97, "id": 1400577471154622473, "id_str": "1400577471154622473", "location": "omahaww, nebraska OwO", "name": "dOwOn baocn", "profile_background_color": "F5F8FA", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1400577471154622473/1626745880", "profile_image_url": "http://pbs.twimg.com/profile_images/1408547963287310336/fExLmqyh_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1408547963287310336/fExLmqyh_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "DuwunB", "statuses_count": 294, "url": "https://t.co/yVtEE7VdMN", "withheld_in_countries": []}, "user_mentions": []}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Fri Jul 30 23:05:10 +0000 2021", "hashtags": [], "id": 1421245514423668739, "id_str": "1421245514423668739", "lang": "en", "retweet_count": 3, "retweeted_status": {"created_at": "Fri Jul 30 23:05:05 +0000 2021", "favorite_count": 25, "hashtags": [], "id": 1421245490558119938, "id_str": "1421245490558119938", "lang": "en", "retweet_count": 3, "source": "&lt;a href=\"https://www.hootsuite.com\" rel=\"nofollow\"&gt;Hootsuite Inc.&lt;/a&gt;", "text": "Thank you to our Omaha intern, Lauren Wiegand! She is from Bellevue, Nebraska and graduated in 2020 from the Univer\u2026 https://t.co/j9pwf13t7i", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1421245490558119938", "url": "https://t.co/j9pwf13t7i"}], "user": {"created_at": "Wed Jan 11 00:17:40 +0000 2017", "description": "Serving the great people of NE-02 \ud83c\uddfa\ud83c\uddf8. Married to Angie, 4 children, 6 grandkids. Brig Gen \u2b50\ufe0f USAF (Ret.) Send questions to our office (link below).", "favourites_count": 11702, "followers_count": 16773, "friends_count": 653, "geo_enabled": true, "id": 818975124460335106, "id_str": "818975124460335106", "listed_count": 569, "location": "Papillion, NE", "name": "Rep. Don Bacon", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/818975124460335106/1540489680", "profile_image_url": "http://pbs.twimg.com/profile_images/1223963541167837186/KXYmFUf5_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1223963541167837186/KXYmFUf5_normal.jpg", "profile_link_color": "E81C4F", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "000000", "profile_text_color": "000000", "screen_name": "RepDonBacon", "statuses_count": 11869, "url": "https://t.co/mkCpzgSdUD", "verified": true, "withheld_in_countries": []}, "user_mentions": []}, "source": "&lt;a href=\"https://nathandharris.com\" rel=\"nofollow\"&gt;All 435 Reps&lt;/a&gt;", "text": "RT @RepDonBacon: Thank you to our Omaha intern, Lauren Wiegand! She is from Bellevue, Nebraska and graduated in 2020 from the University of\u2026", "urls": [], "user": {"created_at": "Fri May 03 22:54:54 +0000 2019", "default_profile": true, "description": "Collecting and retweeting tweets by all members of the US House of Representatives. Archived at: https://t.co/pr8ZcQwGNu", "followers_count": 5420, "friends_count": 746, "id": 1124447266205503488, "id_str": "1124447266205503488", "listed_count": 72, "name": "All 435 Reps", "profile_background_color": "F5F8FA", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1124447266205503488/1556988108", "profile_image_url": "http://pbs.twimg.com/profile_images/1124713248211783680/dISvFwue_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1124713248211783680/dISvFwue_normal.png", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "All435Reps", "statuses_count": 623946, "withheld_in_countries": []}, "user_mentions": [{"id": 818975124460335106, "id_str": "818975124460335106", "name": "Rep. Don Bacon", "screen_name": "RepDonBacon"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Fri Jul 30 23:05:05 +0000 2021", "favorite_count": 25, "hashtags": [], "id": 1421245490558119938, "id_str": "1421245490558119938", "lang": "en", "retweet_count": 3, "source": "&lt;a href=\"https://www.hootsuite.com\" rel=\"nofollow\"&gt;Hootsuite Inc.&lt;/a&gt;", "text": "Thank you to our Omaha intern, Lauren Wiegand! She is from Bellevue, Nebraska and graduated in 2020 from the Univer\u2026 https://t.co/j9pwf13t7i", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1421245490558119938", "url": "https://t.co/j9pwf13t7i"}], "user": {"created_at": "Wed Jan 11 00:17:40 +0000 2017", "description": "Serving the great people of NE-02 \ud83c\uddfa\ud83c\uddf8. Married to Angie, 4 children, 6 grandkids. Brig Gen \u2b50\ufe0f USAF (Ret.) Send questions to our office (link below).", "favourites_count": 11702, "followers_count": 16773, "friends_count": 653, "geo_enabled": true, "id": 818975124460335106, "id_str": "818975124460335106", "listed_count": 569, "location": "Papillion, NE", "name": "Rep. Don Bacon", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/818975124460335106/1540489680", "profile_image_url": "http://pbs.twimg.com/profile_images/1223963541167837186/KXYmFUf5_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1223963541167837186/KXYmFUf5_normal.jpg", "profile_link_color": "E81C4F", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "000000", "profile_text_color": "000000", "screen_name": "RepDonBacon", "statuses_count": 11869, "url": "https://t.co/mkCpzgSdUD", "verified": true, "withheld_in_countries": []}, "user_mentions": []}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Fri Jul 30 09:21:14 +0000 2021", "hashtags": [], "id": 1421038163770892290, "id_str": "1421038163770892290", "lang": "fr", "media": [{"display_url": "pic.twitter.com/WrR091Nk6C", "expanded_url": "https://twitter.com/YoreChart/status/1421038163770892290/photo/1", "id": 1421038162772639744, "media_url": "http://pbs.twimg.com/media/E7iKrhhWQAAMXME.jpg", "media_url_https": "https://pbs.twimg.com/media/E7iKrhhWQAAMXME.jpg", "sizes": {"large": {"h": 570, "resize": "fit", "w": 570}, "medium": {"h": 570, "resize": "fit", "w": 570}, "small": {"h": 570, "resize": "fit", "w": 570}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/WrR091Nk6C"}], "source": "&lt;a href=\"https://ifttt.com\" rel=\"nofollow\"&gt;IFTTT&lt;/a&gt;", "text": "In the minouette shop: Bellevue, NE. Bellevue University Latte Map Mug. by YoreChart at https://t.co/1inqoh6AxY https://t.co/WrR091Nk6C", "urls": [{"expanded_url": "https://ift.tt/3g9dvdf", "url": "https://t.co/1inqoh6AxY"}], "user": {"created_at": "Tue Aug 11 19:43:31 +0000 2020", "default_profile": true, "description": "We Create Custom University Map Products Including Mugs, Latte Mugs, Tumblers, and Custom Premium Prints.", "followers_count": 3, "id": 1293271824180981766, "id_str": "1293271824180981766", "name": "YoreChart", "profile_background_color": "F5F8FA", "profile_image_url": "http://pbs.twimg.com/profile_images/1293272052007227393/98nJCKxl_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1293272052007227393/98nJCKxl_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "YoreChart", "statuses_count": 2419, "withheld_in_countries": []}, "user_mentions": []}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Fri Jul 30 03:23:12 +0000 2021", "hashtags": [], "id": 1420948062755856386, "id_str": "1420948062755856386", "lang": "en", "source": "&lt;a href=\"http://www.socialnewsdesk.com\" rel=\"nofollow\"&gt;SocialNewsDesk&lt;/a&gt;", "text": "Brendon Walker heads to Bellevue University to tee it up for the Bruins https://t.co/3ITWaHURa7", "urls": [{"expanded_url": "https://www.knopnews2.com/2021/07/30/brendon-walker-heads-bellevue-university-tee-it-up-bruins/?utm_campaign=snd-autopilot&amp;utm_source=twitter&amp;utm_medium=social&amp;utm_campaign=snd&amp;utm_content=knop", "url": "https://t.co/3ITWaHURa7"}], "user": {"created_at": "Thu Oct 13 15:28:08 +0000 2011", "default_profile": true, "description": "Official twitter account for @KNOPTV News 2. Be sure to download our KNOP News app.", "favourites_count": 1253, "followers_count": 3027, "friends_count": 830, "geo_enabled": true, "id": 390167719, "id_str": "390167719", "listed_count": 124, "location": "North Platte, NE", "name": "KNOP-TV", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/390167719/1614187690", "profile_image_url": "http://pbs.twimg.com/profile_images/1252290567947632641/v6YZHwIH_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1252290567947632641/v6YZHwIH_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "KNOPTV", "statuses_count": 46125, "url": "http://t.co/b5HFOcv6v6", "verified": true, "withheld_in_countries": []}, "user_mentions": []}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Thu Jul 29 21:13:28 +0000 2021", "favorite_count": 5, "hashtags": [], "id": 1420855014290038785, "id_str": "1420855014290038785", "in_reply_to_screen_name": "OmahaParliament", "in_reply_to_status_id": 1420855010611580936, "in_reply_to_user_id": 1179951924235386881, "lang": "en", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "Let\u2019s help get them closer to their goal!\n\nPledge to donate per goal @Union_Omaha scores July 31-August 31 (note: t\u2026 https://t.co/RIEVpfZQUX", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420855014290038785", "url": "https://t.co/RIEVpfZQUX"}], "user": {"created_at": "Fri Oct 04 02:50:44 +0000 2019", "default_profile": true, "description": "Independent Supporters of @union_omaha! #VivaB\u00fahos #EyesontheOwls\ud83e\udd89\u26bd\ufe0f", "favourites_count": 14510, "followers_count": 1469, "friends_count": 453, "geo_enabled": true, "id": 1179951924235386881, "id_str": "1179951924235386881", "listed_count": 15, "location": "Omaha, NE", "name": "Omaha Parliament", "profile_background_color": "F5F8FA", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1179951924235386881/1626113144", "profile_image_url": "http://pbs.twimg.com/profile_images/1350940153506897921/HmwI2VN3_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1350940153506897921/HmwI2VN3_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "OmahaParliament", "statuses_count": 5024, "url": "https://t.co/QkXTcAz92f", "withheld_in_countries": []}, "user_mentions": [{"id": 1006630180981485568, "id_str": "1006630180981485568", "name": "Union Omaha", "screen_name": "Union_Omaha"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Thu Jul 29 18:00:02 +0000 2021", "hashtags": [], "id": 1420806337986957315, "id_str": "1420806337986957315", "lang": "en", "source": "&lt;a href=\"https://www.townnews.com/\" rel=\"nofollow\"&gt;BLOX CMS&lt;/a&gt;", "text": "COLLEGE DECISION: A joking threat from a neighbor convinced Plattsmouth's Kaleb Wooten to go out for cross country\u2026 https://t.co/t7x4ky26sN", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420806337986957315", "url": "https://t.co/t7x4ky26sN"}], "user": {"created_at": "Tue Sep 06 15:25:28 +0000 2011", "default_profile": true, "description": "Sports in KMAland", "favourites_count": 544, "followers_count": 8487, "friends_count": 600, "id": 368983881, "id_str": "368983881", "listed_count": 33, "location": "KMA land", "name": "KMA Sports", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/368983881/1567604900", "profile_image_url": "http://pbs.twimg.com/profile_images/1032619990925496321/FeU6SO3w_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1032619990925496321/FeU6SO3w_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "KMASports", "statuses_count": 41167, "url": "https://t.co/e1rrr5WNfU", "withheld_in_countries": []}, "user_mentions": []}</t>
   </si>
   <si>
     <t>{"created_at": "Thu Jul 29 16:39:22 +0000 2021", "favorite_count": 1, "hashtags": [], "id": 1420786035336916996, "id_str": "1420786035336916996", "lang": "en", "source": "&lt;a href=\"http://twitter.com/download/android\" rel=\"nofollow\"&gt;Twitter for Android&lt;/a&gt;", "text": "There is an exciting opportunity for your player to train with college athletes!! Camp is tomorrow with Bellevue Un\u2026 https://t.co/8Vb2IUP0UO", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420786035336916996", "url": "https://t.co/8Vb2IUP0UO"}], "user": {"created_at": "Sun Apr 26 16:28:49 +0000 2009", "default_profile": true, "description": "Belleve Soccer Club", "favourites_count": 407, "followers_count": 799, "friends_count": 126, "geo_enabled": true, "id": 35500098, "id_str": "35500098", "listed_count": 10, "location": "Bellevue, NE", "name": "Bellevue Soccer Club", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/35500098/1620334723", "profile_image_url": "http://pbs.twimg.com/profile_images/1401001824946114562/CgGiapnt_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1401001824946114562/CgGiapnt_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "bellevuesc", "statuses_count": 2188, "url": "https://t.co/DvDnFIWCzZ", "withheld_in_countries": []}, "user_mentions": []}</t>
   </si>
   <si>
-    <t>{"created_at": "Thu Jul 29 09:48:25 +0000 2021", "hashtags": [], "id": 1420682618736156674, "id_str": "1420682618736156674", "lang": "en", "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "Today in History\nJuly 29th\n1927 First electric artificial respirator is installed, at Bellevue Hospital in New York\u2026 https://t.co/9D5sj0i9RZ", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420682618736156674", "url": "https://t.co/9D5sj0i9RZ"}], "user": {"created_at": "Tue May 18 22:58:59 +0000 2010", "default_profile": true, "description": "Born and raised in NYC. Wherever I may travel - Always a New Yorker at heart. My passion: History #nuyorican. Inappropriate tweets &amp; people will be blocked", "favourites_count": 10651, "followers_count": 725, "friends_count": 2338, "geo_enabled": true, "id": 145413782, "id_str": "145413782", "listed_count": 27, "location": "Manhattan, NY", "name": "Connie Landro", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/145413782/1495837634", "profile_image_url": "http://pbs.twimg.com/profile_images/895775213350264832/r5HBoEyG_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/895775213350264832/r5HBoEyG_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "clandro", "statuses_count": 16412, "withheld_in_countries": []}, "user_mentions": []}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Thu Jul 29 04:56:54 +0000 2021", "hashtags": [], "id": 1420609255657312256, "id_str": "1420609255657312256", "in_reply_to_screen_name": "AnaMonet2020", "in_reply_to_status_id": 1420604681131200513, "in_reply_to_user_id": 985624101376028672, "lang": "en", "source": "&lt;a href=\"http://twitter.com/download/android\" rel=\"nofollow\"&gt;Twitter for Android&lt;/a&gt;", "text": "@AnaMonet2020 @travisakers I studied mental health counselling through Bellevue university in NE. Couldn't get a pr\u2026 https://t.co/dU3jIaKlfw", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420609255657312256", "url": "https://t.co/dU3jIaKlfw"}], "user": {"created_at": "Tue Jun 10 15:25:24 +0000 2014", "default_profile": true, "description": "Disabled, fmr. Detroit hardcore punk. Eccentric Polymath. Socially awkward\n\nModerate. Knows right from wrong &amp; recognizes competence and decency. (Biden)", "favourites_count": 19877, "followers_count": 443, "friends_count": 727, "geo_enabled": true, "id": 2598098253, "id_str": "2598098253", "location": "Oscoda, MI", "name": "IJS Babcock\u2615\ud83e\udde2", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/2598098253/1610278340", "profile_image_url": "http://pbs.twimg.com/profile_images/1421084503699767298/UK2MdOpM_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1421084503699767298/UK2MdOpM_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "OldDetroitPunk", "statuses_count": 7314, "withheld_in_countries": []}, "user_mentions": [{"id": 985624101376028672, "id_str": "985624101376028672", "name": "AnnaM", "screen_name": "AnaMonet2020"}, {"id": 101005636, "id_str": "101005636", "name": "Travis Akers", "screen_name": "travisakers"}]}</t>
+    <t>{"created_at": "Thu Jul 29 09:48:25 +0000 2021", "hashtags": [], "id": 1420682618736156674, "id_str": "1420682618736156674", "lang": "en", "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "Today in History\nJuly 29th\n1927 First electric artificial respirator is installed, at Bellevue Hospital in New York\u2026 https://t.co/9D5sj0i9RZ", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420682618736156674", "url": "https://t.co/9D5sj0i9RZ"}], "user": {"created_at": "Tue May 18 22:58:59 +0000 2010", "default_profile": true, "description": "Born and raised in NYC. Wherever I may travel - Always a New Yorker at heart. My passion: History #nuyorican. Inappropriate tweets &amp; people will be blocked", "favourites_count": 10651, "followers_count": 725, "friends_count": 2339, "geo_enabled": true, "id": 145413782, "id_str": "145413782", "listed_count": 27, "location": "Manhattan, NY", "name": "Connie Landro", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/145413782/1495837634", "profile_image_url": "http://pbs.twimg.com/profile_images/895775213350264832/r5HBoEyG_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/895775213350264832/r5HBoEyG_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "clandro", "statuses_count": 16412, "withheld_in_countries": []}, "user_mentions": []}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Thu Jul 29 04:56:54 +0000 2021", "hashtags": [], "id": 1420609255657312256, "id_str": "1420609255657312256", "in_reply_to_screen_name": "AnaMonet2020", "in_reply_to_status_id": 1420604681131200513, "in_reply_to_user_id": 985624101376028672, "lang": "en", "source": "&lt;a href=\"http://twitter.com/download/android\" rel=\"nofollow\"&gt;Twitter for Android&lt;/a&gt;", "text": "@AnaMonet2020 @travisakers I studied mental health counselling through Bellevue university in NE. Couldn't get a pr\u2026 https://t.co/dU3jIaKlfw", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420609255657312256", "url": "https://t.co/dU3jIaKlfw"}], "user": {"created_at": "Tue Jun 10 15:25:24 +0000 2014", "default_profile": true, "description": "Disabled, fmr. Detroit hardcore punk. Eccentric Polymath. Socially awkward\n\nModerate. Knows right from wrong &amp; recognizes competence and decency. (Biden)", "favourites_count": 19981, "followers_count": 446, "friends_count": 731, "geo_enabled": true, "id": 2598098253, "id_str": "2598098253", "location": "Oscoda, MI", "name": "IJS Babcock\u2615\ud83e\udde2", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/2598098253/1610278340", "profile_image_url": "http://pbs.twimg.com/profile_images/1421084503699767298/UK2MdOpM_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1421084503699767298/UK2MdOpM_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "OldDetroitPunk", "statuses_count": 7348, "withheld_in_countries": []}, "user_mentions": [{"id": 985624101376028672, "id_str": "985624101376028672", "name": "AnnaM", "screen_name": "AnaMonet2020"}, {"id": 101005636, "id_str": "101005636", "name": "Travis Akers", "screen_name": "travisakers"}]}</t>
   </si>
   <si>
     <t>{"created_at": "Thu Jul 29 01:39:37 +0000 2021", "hashtags": [], "id": 1420559607982817281, "id_str": "1420559607982817281", "in_reply_to_screen_name": "maeveynott", "in_reply_to_status_id": 1420559598444945409, "in_reply_to_user_id": 1414523228588896257, "lang": "fr", "media": [{"display_url": "pic.twitter.com/oLijixNAH7", "expanded_url": "https://twitter.com/maeveynott/status/1420559607982817281/photo/1", "id": 1420559602572173313, "media_url": "http://pbs.twimg.com/media/E7bXbp2VoAEbebQ.jpg", "media_url_https": "https://pbs.twimg.com/media/E7bXbp2VoAEbebQ.jpg", "sizes": {"large": {"h": 1030, "resize": "fit", "w": 1241}, "medium": {"h": 996, "resize": "fit", "w": 1200}, "small": {"h": 564, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/oLijixNAH7"}, {"display_url": "pic.twitter.com/oLijixNAH7", "expanded_url": "https://twitter.com/maeveynott/status/1420559607982817281/photo/1", "id": 1420559602697924609, "media_url": "http://pbs.twimg.com/media/E7bXbqUUcAEmvC2.jpg", "media_url_https": "https://pbs.twimg.com/media/E7bXbqUUcAEmvC2.jpg", "sizes": {"large": {"h": 1029, "resize": "fit", "w": 1241}, "medium": {"h": 995, "resize": "fit", "w": 1200}, "small": {"h": 564, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/oLijixNAH7"}, {"display_url": "pic.twitter.com/oLijixNAH7", "expanded_url": "https://twitter.com/maeveynott/status/1420559607982817281/photo/1", "id": 1420559602962165761, "media_url": "http://pbs.twimg.com/media/E7bXbrTUcAEaMVW.jpg", "media_url_https": "https://pbs.twimg.com/media/E7bXbrTUcAEaMVW.jpg", "sizes": {"large": {"h": 1018, "resize": "fit", "w": 1241}, "medium": {"h": 984, "resize": "fit", "w": 1200}, "small": {"h": 558, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/oLijixNAH7"}], "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "bellevue university \u2022 les gar\u00e7ons, the alpha three https://t.co/oLijixNAH7", "urls": [], "user": {"created_at": "Mon Jul 12 09:54:00 +0000 2021", "default_profile": true, "description": "dump", "favourites_count": 2, "friends_count": 13, "id": 1414523228588896257, "id_str": "1414523228588896257", "name": "maeve", "profile_background_color": "F5F8FA", "profile_image_url": "http://pbs.twimg.com/profile_images/1414523612850122753/68v-8uUb_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1414523612850122753/68v-8uUb_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "maeveynott", "statuses_count": 15, "withheld_in_countries": []}, "user_mentions": []}</t>
@@ -127,52 +133,52 @@
     <t>{"created_at": "Thu Jul 29 01:39:35 +0000 2021", "hashtags": [], "id": 1420559598444945409, "id_str": "1420559598444945409", "in_reply_to_screen_name": "maeveynott", "in_reply_to_status_id": 1420559583223828480, "in_reply_to_user_id": 1414523228588896257, "lang": "fr", "media": [{"display_url": "pic.twitter.com/tqqYxeaSyV", "expanded_url": "https://twitter.com/maeveynott/status/1420559598444945409/photo/1", "id": 1420559592585498625, "media_url": "http://pbs.twimg.com/media/E7bXbEpVEAEy-gx.jpg", "media_url_https": "https://pbs.twimg.com/media/E7bXbEpVEAEy-gx.jpg", "sizes": {"large": {"h": 1026, "resize": "fit", "w": 1241}, "medium": {"h": 992, "resize": "fit", "w": 1200}, "small": {"h": 562, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/tqqYxeaSyV"}, {"display_url": "pic.twitter.com/tqqYxeaSyV", "expanded_url": "https://twitter.com/maeveynott/status/1420559598444945409/photo/1", "id": 1420559592606498819, "media_url": "http://pbs.twimg.com/media/E7bXbEuVgAM_03i.jpg", "media_url_https": "https://pbs.twimg.com/media/E7bXbEuVgAM_03i.jpg", "sizes": {"large": {"h": 961, "resize": "fit", "w": 1241}, "medium": {"h": 929, "resize": "fit", "w": 1200}, "small": {"h": 527, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/tqqYxeaSyV"}, {"display_url": "pic.twitter.com/tqqYxeaSyV", "expanded_url": "https://twitter.com/maeveynott/status/1420559598444945409/photo/1", "id": 1420559592614817795, "media_url": "http://pbs.twimg.com/media/E7bXbEwUcAMsykr.jpg", "media_url_https": "https://pbs.twimg.com/media/E7bXbEwUcAMsykr.jpg", "sizes": {"large": {"h": 1094, "resize": "fit", "w": 1241}, "medium": {"h": 1058, "resize": "fit", "w": 1200}, "small": {"h": 599, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/tqqYxeaSyV"}, {"display_url": "pic.twitter.com/tqqYxeaSyV", "expanded_url": "https://twitter.com/maeveynott/status/1420559598444945409/photo/1", "id": 1420559592606429186, "media_url": "http://pbs.twimg.com/media/E7bXbEuUcAIh-1b.jpg", "media_url_https": "https://pbs.twimg.com/media/E7bXbEuUcAIh-1b.jpg", "sizes": {"large": {"h": 1033, "resize": "fit", "w": 1241}, "medium": {"h": 999, "resize": "fit", "w": 1200}, "small": {"h": 566, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/tqqYxeaSyV"}], "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "bellevue university \u2022 les filles https://t.co/tqqYxeaSyV", "urls": [], "user": {"created_at": "Mon Jul 12 09:54:00 +0000 2021", "default_profile": true, "description": "dump", "favourites_count": 2, "friends_count": 13, "id": 1414523228588896257, "id_str": "1414523228588896257", "name": "maeve", "profile_background_color": "F5F8FA", "profile_image_url": "http://pbs.twimg.com/profile_images/1414523612850122753/68v-8uUb_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1414523612850122753/68v-8uUb_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "maeveynott", "statuses_count": 15, "withheld_in_countries": []}, "user_mentions": []}</t>
   </si>
   <si>
-    <t>{"created_at": "Wed Jul 28 15:21:10 +0000 2021", "favorite_count": 3, "hashtags": [], "id": 1420403967448674310, "id_str": "1420403967448674310", "in_reply_to_screen_name": "GrossmanManny", "in_reply_to_status_id": 1420382926005542915, "in_reply_to_user_id": 1391739495796596742, "lang": "en", "quoted_status": {"created_at": "Wed Jul 28 03:53:57 +0000 2021", "hashtags": [], "id": 1420231023900590086, "id_str": "1420231023900590086", "in_reply_to_screen_name": "DecoderOfTruth", "in_reply_to_status_id": 1419822806154375170, "in_reply_to_user_id": 2996519460, "lang": "en", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "HIV/AIDS at the same place where Dr. Albert LaVerne was on staff.\n\nHis wife Paule Passavant LaVerne, was gunned dow\u2026 https://t.co/9sHbDQb8D9", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420231023900590086", "url": "https://t.co/9sHbDQb8D9"}], "user": {"created_at": "Mon Jan 26 04:40:16 +0000 2015", "default_profile": true, "favourites_count": 129, "followers_count": 254, "friends_count": 7, "id": 2996519460, "id_str": "2996519460", "listed_count": 1, "name": "Julie", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/2996519460/1551662427", "profile_image_url": "http://pbs.twimg.com/profile_images/1413891794719285248/x771zpyU_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1413891794719285248/x771zpyU_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "DecoderOfTruth", "statuses_count": 4251, "withheld_in_countries": []}, "user_mentions": []}, "quoted_status_id": 1420231023900590086, "quoted_status_id_str": "1420231023900590086", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@GrossmanManny Your SOS research is bleeding over into my research\ud83d\ude2e\n\nDr. Albert LaVerne Senior psychiatrist at NY U\u2026 https://t.co/TIxqcp9kpk", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420403967448674310", "url": "https://t.co/TIxqcp9kpk"}], "user": {"created_at": "Mon Jan 26 04:40:16 +0000 2015", "default_profile": true, "favourites_count": 129, "followers_count": 254, "friends_count": 7, "id": 2996519460, "id_str": "2996519460", "listed_count": 1, "name": "Julie", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/2996519460/1551662427", "profile_image_url": "http://pbs.twimg.com/profile_images/1413891794719285248/x771zpyU_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1413891794719285248/x771zpyU_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "DecoderOfTruth", "statuses_count": 4251, "withheld_in_countries": []}, "user_mentions": [{"id": 1391739495796596742, "id_str": "1391739495796596742", "name": "Manny Grossman", "screen_name": "GrossmanManny"}]}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Wed Jul 28 07:44:47 +0000 2021", "hashtags": [], "id": 1420289114918854656, "id_str": "1420289114918854656", "lang": "en", "retweet_count": 1, "retweeted_status": {"created_at": "Tue Jul 27 17:39:00 +0000 2021", "favorite_count": 10, "hashtags": [], "id": 1420076266208776193, "id_str": "1420076266208776193", "in_reply_to_screen_name": "carlquintanilla", "in_reply_to_status_id": 1420014215255965699, "in_reply_to_user_id": 114782468, "lang": "en", "retweet_count": 1, "source": "&lt;a href=\"http://twitter.com/download/android\" rel=\"nofollow\"&gt;Twitter for Android&lt;/a&gt;", "text": "@carlquintanilla All they're doing is playing catchup to other multi-billion $ companies.\nAnd this free tuition onl\u2026 https://t.co/r2w7oW5LAE", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420076266208776193", "url": "https://t.co/r2w7oW5LAE"}], "user": {"created_at": "Wed Oct 16 03:47:56 +0000 2013", "default_profile": true, "description": "Progressive woman who believes in calling out the injustices in America, whether by Democrats or GOP; strong gun laws; science; books; baseball; rock n roll\ud83c\udfb6\ud83c\udfb5", "favourites_count": 31814, "followers_count": 189, "friends_count": 752, "geo_enabled": true, "id": 717006051, "id_str": "717006051", "listed_count": 3, "location": "Belleville, IL", "name": "Diana - The O.H.", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/717006051/1613862055", "profile_image_url": "http://pbs.twimg.com/profile_images/1369357580255002626/AM3394Bp_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1369357580255002626/AM3394Bp_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "DianaWandersOn", "statuses_count": 6172, "withheld_in_countries": []}, "user_mentions": [{"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @DianaWandersOn: @carlquintanilla All they're doing is playing catchup to other multi-billion $ companies.\nAnd this free tuition only ap\u2026", "urls": [], "user": {"created_at": "Mon Nov 10 03:45:00 +0000 2008", "description": "\ud83c\udf0a\ud83c\udf0a#Spoonie, #Disabled #Vaccinated #LGBTQI+ #Humanist #Democrat #BLM #TimesUp #MeToo sexuality/human rights advocate #RESIST #Resistance #VoteBlue \ud83c\udf0a\ud83c\udf0a #FBR", "favourites_count": 288074, "followers_count": 7480, "friends_count": 7493, "id": 17280041, "id_str": "17280041", "listed_count": 8, "location": "New Orleans, LA", "name": "JamieJoy Loves Madam VP Harris \ud83c\udf0aPOTUS Biden\ud83c\udf0a#BLM", "profile_background_color": "F5E2C1", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme11/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme11/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/17280041/1537233953", "profile_image_url": "http://pbs.twimg.com/profile_images/1212460299032416263/h1z7A1Ia_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1212460299032416263/h1z7A1Ia_normal.jpg", "profile_link_color": "E81C4F", "profile_sidebar_border_color": "DBE9ED", "profile_sidebar_fill_color": "5C0B05", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "mindcaviar", "statuses_count": 102793, "url": "https://t.co/kP8RuibYYd", "withheld_in_countries": []}, "user_mentions": [{"id": 717006051, "id_str": "717006051", "name": "Diana - The O.H.", "screen_name": "DianaWandersOn"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Wed Jul 28 07:44:26 +0000 2021", "hashtags": [], "id": 1420289027337564161, "id_str": "1420289027337564161", "lang": "en", "retweet_count": 9, "retweeted_status": {"created_at": "Tue Jul 27 13:37:31 +0000 2021", "favorite_count": 22, "hashtags": [], "id": 1420015494850129930, "id_str": "1420015494850129930", "in_reply_to_screen_name": "reassuringURL", "in_reply_to_status_id": 1420015089302654977, "in_reply_to_user_id": 3187056242, "lang": "en", "retweet_count": 9, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Uni\u2026 https://t.co/4CTPEuQTUF", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420015494850129930", "url": "https://t.co/4CTPEuQTUF"}], "user": {"created_at": "Mon Jun 27 02:44:44 +0000 2011", "description": "Finance | Tech | China \ud83d\udc40| Navy vet | #GoHoos", "favourites_count": 12892, "followers_count": 224, "friends_count": 1195, "id": 324707378, "id_str": "324707378", "listed_count": 3, "location": "Alpha Centauri", "name": "apathetic Tim", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/324707378/1413625214", "profile_image_url": "http://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_link_color": "C91616", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "0084B4", "profile_use_background_image": true, "screen_name": "DoctorDirtNasty", "statuses_count": 16942, "withheld_in_countries": []}, "user_mentions": [{"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @DoctorDirtNasty: @reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Univer\u2026", "urls": [], "user": {"created_at": "Mon Nov 10 03:45:00 +0000 2008", "description": "\ud83c\udf0a\ud83c\udf0a#Spoonie, #Disabled #Vaccinated #LGBTQI+ #Humanist #Democrat #BLM #TimesUp #MeToo sexuality/human rights advocate #RESIST #Resistance #VoteBlue \ud83c\udf0a\ud83c\udf0a #FBR", "favourites_count": 288074, "followers_count": 7480, "friends_count": 7493, "id": 17280041, "id_str": "17280041", "listed_count": 8, "location": "New Orleans, LA", "name": "JamieJoy Loves Madam VP Harris \ud83c\udf0aPOTUS Biden\ud83c\udf0a#BLM", "profile_background_color": "F5E2C1", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme11/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme11/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/17280041/1537233953", "profile_image_url": "http://pbs.twimg.com/profile_images/1212460299032416263/h1z7A1Ia_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1212460299032416263/h1z7A1Ia_normal.jpg", "profile_link_color": "E81C4F", "profile_sidebar_border_color": "DBE9ED", "profile_sidebar_fill_color": "5C0B05", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "mindcaviar", "statuses_count": 102793, "url": "https://t.co/kP8RuibYYd", "withheld_in_countries": []}, "user_mentions": [{"id": 324707378, "id_str": "324707378", "name": "apathetic Tim", "screen_name": "DoctorDirtNasty"}, {"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Wed Jul 28 06:27:23 +0000 2021", "hashtags": [], "id": 1420269635472019460, "id_str": "1420269635472019460", "lang": "en", "retweet_count": 9, "retweeted_status": {"created_at": "Tue Jul 27 13:37:31 +0000 2021", "favorite_count": 22, "hashtags": [], "id": 1420015494850129930, "id_str": "1420015494850129930", "in_reply_to_screen_name": "reassuringURL", "in_reply_to_status_id": 1420015089302654977, "in_reply_to_user_id": 3187056242, "lang": "en", "retweet_count": 9, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Uni\u2026 https://t.co/4CTPEuQTUF", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420015494850129930", "url": "https://t.co/4CTPEuQTUF"}], "user": {"created_at": "Mon Jun 27 02:44:44 +0000 2011", "description": "Finance | Tech | China \ud83d\udc40| Navy vet | #GoHoos", "favourites_count": 12892, "followers_count": 224, "friends_count": 1195, "id": 324707378, "id_str": "324707378", "listed_count": 3, "location": "Alpha Centauri", "name": "apathetic Tim", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/324707378/1413625214", "profile_image_url": "http://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_link_color": "C91616", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "0084B4", "profile_use_background_image": true, "screen_name": "DoctorDirtNasty", "statuses_count": 16942, "withheld_in_countries": []}, "user_mentions": [{"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"http://twitter.com/download/android\" rel=\"nofollow\"&gt;Twitter for Android&lt;/a&gt;", "text": "RT @DoctorDirtNasty: @reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Univer\u2026", "urls": [], "user": {"created_at": "Wed Apr 03 09:55:40 +0000 2013", "default_profile": true, "description": "Community Activist, Guitar Picker, Blues Harmonica, Rabble Rouser, Smart Aleck, Widower, Dad, Brother, Amigo/Friend, WarriorBrother, Santa,El Camino de Santiago", "favourites_count": 548, "followers_count": 790, "friends_count": 2524, "geo_enabled": true, "id": 1324265089, "id_str": "1324265089", "listed_count": 9, "location": "Everett, WA", "name": "Michael Trujillo", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1324265089/1466688941", "profile_image_url": "http://pbs.twimg.com/profile_images/803849515098841088/dZRSdHdW_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/803849515098841088/dZRSdHdW_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "lionman47", "statuses_count": 119281, "withheld_in_countries": []}, "user_mentions": [{"id": 324707378, "id_str": "324707378", "name": "apathetic Tim", "screen_name": "DoctorDirtNasty"}, {"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Tue Jul 27 22:27:30 +0000 2021", "favorite_count": 1, "hashtags": [], "id": 1420148868944068614, "id_str": "1420148868944068614", "in_reply_to_screen_name": "DecoderOfTruth", "in_reply_to_status_id": 1420137058991964164, "in_reply_to_user_id": 2996519460, "lang": "en", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "Sr. psychiatrist at NY University-Bellevue Medical Center, Albert is known for curing people from drug/alcohol addi\u2026 https://t.co/0DBVJaUYRm", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420148868944068614", "url": "https://t.co/0DBVJaUYRm"}], "user": {"created_at": "Mon Jan 26 04:40:16 +0000 2015", "default_profile": true, "favourites_count": 129, "followers_count": 254, "friends_count": 7, "id": 2996519460, "id_str": "2996519460", "listed_count": 1, "name": "Julie", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/2996519460/1551662427", "profile_image_url": "http://pbs.twimg.com/profile_images/1413891794719285248/x771zpyU_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1413891794719285248/x771zpyU_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "DecoderOfTruth", "statuses_count": 4251, "withheld_in_countries": []}, "user_mentions": []}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Tue Jul 27 21:33:00 +0000 2021", "hashtags": [], "id": 1420135155880976387, "id_str": "1420135155880976387", "in_reply_to_screen_name": "DecoderOfTruth", "in_reply_to_status_id": 1420130449477701633, "in_reply_to_user_id": 2996519460, "lang": "en", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "8.1/ Bellevue opened \u201cpavilion for the insane\u201d in 1879 and a alcoholic ward in 1892. These were part of the main ho\u2026 https://t.co/sywGoNTzWf", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420135155880976387", "url": "https://t.co/sywGoNTzWf"}], "user": {"created_at": "Mon Jan 26 04:40:16 +0000 2015", "default_profile": true, "favourites_count": 129, "followers_count": 254, "friends_count": 7, "id": 2996519460, "id_str": "2996519460", "listed_count": 1, "name": "Julie", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/2996519460/1551662427", "profile_image_url": "http://pbs.twimg.com/profile_images/1413891794719285248/x771zpyU_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1413891794719285248/x771zpyU_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "DecoderOfTruth", "statuses_count": 4251, "withheld_in_countries": []}, "user_mentions": []}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Tue Jul 27 19:41:54 +0000 2021", "favorite_count": 2, "hashtags": [], "id": 1420107195060944896, "id_str": "1420107195060944896", "lang": "en", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "Bellevue-based Gaia Platform, along with two of its Snoqualmie Valley employees, are working with AI Racing Tech an\u2026 https://t.co/rsZGCJwAXS", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420107195060944896", "url": "https://t.co/rsZGCJwAXS"}], "user": {"created_at": "Wed Sep 22 17:34:23 +0000 2010", "description": "Snoqualmie Valley News. Real resident. Up to date happenings and breaking news in the Snoqualmie Valley.", "favourites_count": 1307, "followers_count": 2243, "friends_count": 501, "id": 193780411, "id_str": "193780411", "listed_count": 30, "location": "Snoqualmie Valley, WA", "name": "Livingsnoqualmie.com", "profile_background_color": "022330", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/193780411/1539109526", "profile_image_url": "http://pbs.twimg.com/profile_images/938535260718997504/9GHoWzOV_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/938535260718997504/9GHoWzOV_normal.jpg", "profile_link_color": "0084B4", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "LivingSno", "statuses_count": 5817, "url": "http://t.co/CN8HLNkKuz", "withheld_in_countries": []}, "user_mentions": []}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Tue Jul 27 17:53:59 +0000 2021", "hashtags": [], "id": 1420080035797553162, "id_str": "1420080035797553162", "lang": "en", "retweet_count": 9, "retweeted_status": {"created_at": "Tue Jul 27 13:37:31 +0000 2021", "favorite_count": 22, "hashtags": [], "id": 1420015494850129930, "id_str": "1420015494850129930", "in_reply_to_screen_name": "reassuringURL", "in_reply_to_status_id": 1420015089302654977, "in_reply_to_user_id": 3187056242, "lang": "en", "retweet_count": 9, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Uni\u2026 https://t.co/4CTPEuQTUF", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420015494850129930", "url": "https://t.co/4CTPEuQTUF"}], "user": {"created_at": "Mon Jun 27 02:44:44 +0000 2011", "description": "Finance | Tech | China \ud83d\udc40| Navy vet | #GoHoos", "favourites_count": 12892, "followers_count": 224, "friends_count": 1195, "id": 324707378, "id_str": "324707378", "listed_count": 3, "location": "Alpha Centauri", "name": "apathetic Tim", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/324707378/1413625214", "profile_image_url": "http://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_link_color": "C91616", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "0084B4", "profile_use_background_image": true, "screen_name": "DoctorDirtNasty", "statuses_count": 16942, "withheld_in_countries": []}, "user_mentions": [{"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "RT @DoctorDirtNasty: @reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Univer\u2026", "urls": [], "user": {"created_at": "Sun Jan 26 01:19:55 +0000 2014", "default_profile": true, "description": "Educational Futurist. Associate Director. Parent. Womanist. Researcher. Proud FSU Seminole. KDX \ud83d\udc27. ODK. Retweets are not endorsements just evidence of reading", "favourites_count": 53649, "followers_count": 550, "friends_count": 419, "geo_enabled": true, "id": 2310977114, "id_str": "2310977114", "listed_count": 103, "location": "FSU Tallahassee, Fl", "name": "Dr. Barefoot Scholar", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/2310977114/1592108441", "profile_image_url": "http://pbs.twimg.com/profile_images/1314247200852017152/Lr-RVEkc_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1314247200852017152/Lr-RVEkc_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "SophiaRahming1", "statuses_count": 187492, "withheld_in_countries": []}, "user_mentions": [{"id": 324707378, "id_str": "324707378", "name": "apathetic Tim", "screen_name": "DoctorDirtNasty"}, {"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Tue Jul 27 17:39:00 +0000 2021", "favorite_count": 10, "hashtags": [], "id": 1420076266208776193, "id_str": "1420076266208776193", "in_reply_to_screen_name": "carlquintanilla", "in_reply_to_status_id": 1420014215255965699, "in_reply_to_user_id": 114782468, "lang": "en", "retweet_count": 1, "source": "&lt;a href=\"http://twitter.com/download/android\" rel=\"nofollow\"&gt;Twitter for Android&lt;/a&gt;", "text": "@carlquintanilla All they're doing is playing catchup to other multi-billion $ companies.\nAnd this free tuition onl\u2026 https://t.co/r2w7oW5LAE", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420076266208776193", "url": "https://t.co/r2w7oW5LAE"}], "user": {"created_at": "Wed Oct 16 03:47:56 +0000 2013", "default_profile": true, "description": "Progressive woman who believes in calling out the injustices in America, whether by Democrats or GOP; strong gun laws; science; books; baseball; rock n roll\ud83c\udfb6\ud83c\udfb5", "favourites_count": 31814, "followers_count": 189, "friends_count": 752, "geo_enabled": true, "id": 717006051, "id_str": "717006051", "listed_count": 3, "location": "Belleville, IL", "name": "Diana - The O.H.", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/717006051/1613862055", "profile_image_url": "http://pbs.twimg.com/profile_images/1369357580255002626/AM3394Bp_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1369357580255002626/AM3394Bp_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "DianaWandersOn", "statuses_count": 6172, "withheld_in_countries": []}, "user_mentions": [{"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Tue Jul 27 16:32:50 +0000 2021", "hashtags": [], "id": 1420059615732064260, "id_str": "1420059615732064260", "lang": "en", "retweet_count": 9, "retweeted_status": {"created_at": "Tue Jul 27 13:37:31 +0000 2021", "favorite_count": 22, "hashtags": [], "id": 1420015494850129930, "id_str": "1420015494850129930", "in_reply_to_screen_name": "reassuringURL", "in_reply_to_status_id": 1420015089302654977, "in_reply_to_user_id": 3187056242, "lang": "en", "retweet_count": 9, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Uni\u2026 https://t.co/4CTPEuQTUF", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420015494850129930", "url": "https://t.co/4CTPEuQTUF"}], "user": {"created_at": "Mon Jun 27 02:44:44 +0000 2011", "description": "Finance | Tech | China \ud83d\udc40| Navy vet | #GoHoos", "favourites_count": 12892, "followers_count": 224, "friends_count": 1195, "id": 324707378, "id_str": "324707378", "listed_count": 3, "location": "Alpha Centauri", "name": "apathetic Tim", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/324707378/1413625214", "profile_image_url": "http://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_link_color": "C91616", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "0084B4", "profile_use_background_image": true, "screen_name": "DoctorDirtNasty", "statuses_count": 16942, "withheld_in_countries": []}, "user_mentions": [{"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "RT @DoctorDirtNasty: @reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Univer\u2026", "urls": [], "user": {"created_at": "Sun Mar 22 15:19:23 +0000 2009", "description": "openly black. boston. los angeles. duke. bama. memphis.", "favourites_count": 1851, "followers_count": 385, "friends_count": 304, "geo_enabled": true, "id": 25829276, "id_str": "25829276", "listed_count": 19, "location": "twitter.", "name": "maxine shaw", "profile_background_color": "BADFCD", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme12/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme12/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/25829276/1407940765", "profile_image_url": "http://pbs.twimg.com/profile_images/1317811173501358080/hasJGqMi_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1317811173501358080/hasJGqMi_normal.jpg", "profile_link_color": "FF0000", "profile_sidebar_border_color": "F2E195", "profile_sidebar_fill_color": "FFF7CC", "profile_text_color": "0C3E53", "profile_use_background_image": true, "screen_name": "SuperRegular", "statuses_count": 68406, "withheld_in_countries": []}, "user_mentions": [{"id": 324707378, "id_str": "324707378", "name": "apathetic Tim", "screen_name": "DoctorDirtNasty"}, {"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Tue Jul 27 16:10:29 +0000 2021", "hashtags": [], "id": 1420053990541348872, "id_str": "1420053990541348872", "lang": "en", "retweet_count": 9, "retweeted_status": {"created_at": "Tue Jul 27 13:37:31 +0000 2021", "favorite_count": 22, "hashtags": [], "id": 1420015494850129930, "id_str": "1420015494850129930", "in_reply_to_screen_name": "reassuringURL", "in_reply_to_status_id": 1420015089302654977, "in_reply_to_user_id": 3187056242, "lang": "en", "retweet_count": 9, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Uni\u2026 https://t.co/4CTPEuQTUF", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420015494850129930", "url": "https://t.co/4CTPEuQTUF"}], "user": {"created_at": "Mon Jun 27 02:44:44 +0000 2011", "description": "Finance | Tech | China \ud83d\udc40| Navy vet | #GoHoos", "favourites_count": 12892, "followers_count": 224, "friends_count": 1195, "id": 324707378, "id_str": "324707378", "listed_count": 3, "location": "Alpha Centauri", "name": "apathetic Tim", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/324707378/1413625214", "profile_image_url": "http://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_link_color": "C91616", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "0084B4", "profile_use_background_image": true, "screen_name": "DoctorDirtNasty", "statuses_count": 16942, "withheld_in_countries": []}, "user_mentions": [{"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @DoctorDirtNasty: @reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Univer\u2026", "urls": [], "user": {"created_at": "Sat Mar 21 00:24:34 +0000 2009", "description": "\ud83d\uddfd", "favourites_count": 29688, "followers_count": 164, "friends_count": 1254, "id": 25607309, "id_str": "25607309", "location": "NJ", "name": "D80s", "profile_background_color": "352726", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme5/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme5/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/25607309/1597543506", "profile_image_url": "http://pbs.twimg.com/profile_images/858122100820910081/6yUh3jU-_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/858122100820910081/6yUh3jU-_normal.jpg", "profile_link_color": "D02B55", "profile_sidebar_border_color": "829D5E", "profile_sidebar_fill_color": "99CC33", "profile_text_color": "3E4415", "profile_use_background_image": true, "screen_name": "D80s", "statuses_count": 96785, "withheld_in_countries": []}, "user_mentions": [{"id": 324707378, "id_str": "324707378", "name": "apathetic Tim", "screen_name": "DoctorDirtNasty"}, {"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Tue Jul 27 15:40:37 +0000 2021", "hashtags": [], "id": 1420046473241137153, "id_str": "1420046473241137153", "lang": "en", "retweet_count": 9, "retweeted_status": {"created_at": "Tue Jul 27 13:37:31 +0000 2021", "favorite_count": 22, "hashtags": [], "id": 1420015494850129930, "id_str": "1420015494850129930", "in_reply_to_screen_name": "reassuringURL", "in_reply_to_status_id": 1420015089302654977, "in_reply_to_user_id": 3187056242, "lang": "en", "retweet_count": 9, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Uni\u2026 https://t.co/4CTPEuQTUF", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420015494850129930", "url": "https://t.co/4CTPEuQTUF"}], "user": {"created_at": "Mon Jun 27 02:44:44 +0000 2011", "description": "Finance | Tech | China \ud83d\udc40| Navy vet | #GoHoos", "favourites_count": 12892, "followers_count": 224, "friends_count": 1195, "id": 324707378, "id_str": "324707378", "listed_count": 3, "location": "Alpha Centauri", "name": "apathetic Tim", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/324707378/1413625214", "profile_image_url": "http://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_link_color": "C91616", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "0084B4", "profile_use_background_image": true, "screen_name": "DoctorDirtNasty", "statuses_count": 16942, "withheld_in_countries": []}, "user_mentions": [{"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"http://twitter.com/download/android\" rel=\"nofollow\"&gt;Twitter for Android&lt;/a&gt;", "text": "RT @DoctorDirtNasty: @reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Univer\u2026", "urls": [], "user": {"created_at": "Mon Sep 28 03:03:22 +0000 2009", "default_profile": true, "favourites_count": 27217, "followers_count": 784, "friends_count": 1794, "id": 77908436, "id_str": "77908436", "listed_count": 33, "name": "Jennifer Bills", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_image_url": "http://pbs.twimg.com/profile_images/712391911353372672/V7vEnQ81_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/712391911353372672/V7vEnQ81_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "JJBills14", "statuses_count": 78351, "withheld_in_countries": []}, "user_mentions": [{"id": 324707378, "id_str": "324707378", "name": "apathetic Tim", "screen_name": "DoctorDirtNasty"}, {"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Tue Jul 27 15:01:14 +0000 2021", "hashtags": [], "id": 1420036564667846657, "id_str": "1420036564667846657", "lang": "en", "retweet_count": 9, "retweeted_status": {"created_at": "Tue Jul 27 13:37:31 +0000 2021", "favorite_count": 22, "hashtags": [], "id": 1420015494850129930, "id_str": "1420015494850129930", "in_reply_to_screen_name": "reassuringURL", "in_reply_to_status_id": 1420015089302654977, "in_reply_to_user_id": 3187056242, "lang": "en", "retweet_count": 9, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Uni\u2026 https://t.co/4CTPEuQTUF", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420015494850129930", "url": "https://t.co/4CTPEuQTUF"}], "user": {"created_at": "Mon Jun 27 02:44:44 +0000 2011", "description": "Finance | Tech | China \ud83d\udc40| Navy vet | #GoHoos", "favourites_count": 12892, "followers_count": 224, "friends_count": 1195, "id": 324707378, "id_str": "324707378", "listed_count": 3, "location": "Alpha Centauri", "name": "apathetic Tim", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/324707378/1413625214", "profile_image_url": "http://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_link_color": "C91616", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "0084B4", "profile_use_background_image": true, "screen_name": "DoctorDirtNasty", "statuses_count": 16942, "withheld_in_countries": []}, "user_mentions": [{"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @DoctorDirtNasty: @reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Univer\u2026", "urls": [], "user": {"created_at": "Fri Apr 08 22:19:12 +0000 2016", "description": "product mgr | project mgr | data wrangler | novice data viz designer | Vegetarian", "favourites_count": 122508, "followers_count": 876, "friends_count": 1030, "id": 718563872806805504, "id_str": "718563872806805504", "listed_count": 163, "location": "Kingston/Boston", "name": "Glen Dixon", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/718563872806805504/1627132416", "profile_image_url": "http://pbs.twimg.com/profile_images/1420412487615270917/6wyxU2Dv_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1420412487615270917/6wyxU2Dv_normal.jpg", "profile_link_color": "19CF86", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "000000", "profile_text_color": "000000", "screen_name": "glenrdixon", "statuses_count": 75372, "withheld_in_countries": []}, "user_mentions": [{"id": 324707378, "id_str": "324707378", "name": "apathetic Tim", "screen_name": "DoctorDirtNasty"}, {"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Tue Jul 27 13:58:47 +0000 2021", "hashtags": [], "id": 1420020847767658506, "id_str": "1420020847767658506", "lang": "en", "quoted_status": {"created_at": "Tue Jul 27 13:32:26 +0000 2021", "favorite_count": 9117, "hashtags": [], "id": 1420014215255965699, "id_str": "1420014215255965699", "lang": "en", "retweet_count": 1703, "source": "&lt;a href=\"https://about.twitter.com/products/tweetdeck\" rel=\"nofollow\"&gt;TweetDeck&lt;/a&gt;", "text": "(Reuters) - Walmart Inc on Tuesday  said it will pay the full cost of college tuition and books for  its roughly 1.\u2026 https://t.co/2c7ZZRrTs2", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420014215255965699", "url": "https://t.co/2c7ZZRrTs2"}], "user": {"created_at": "Tue Feb 16 15:59:04 +0000 2010", "description": "20+ years @CNBC &amp; @NBCNews / Peabody Award, Emmy, DuPont recipient / @WSJ alum / \u201cOnly one rule that I know of: goddamn it, you\u2019ve got to be kind.\u201d - Vonnegut", "favourites_count": 2396, "followers_count": 308176, "friends_count": 5378, "geo_enabled": true, "id": 114782468, "id_str": "114782468", "listed_count": 4822, "location": "nyc", "name": "Carl Quintanilla", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/114782468/1627376325", "profile_image_url": "http://pbs.twimg.com/profile_images/1214244686786965510/OAxLuUGH_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1214244686786965510/OAxLuUGH_normal.jpg", "profile_link_color": "3B94D9", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "FFFFFF", "profile_text_color": "000000", "profile_use_background_image": true, "screen_name": "carlquintanilla", "statuses_count": 90245, "url": "https://t.co/CHozTuBfc5", "verified": true, "withheld_in_countries": []}, "user_mentions": []}, "quoted_status_id": 1420014215255965699, "quoted_status_id_str": "1420014215255965699", "source": "&lt;a href=\"https://about.twitter.com/products/tweetdeck\" rel=\"nofollow\"&gt;TweetDeck&lt;/a&gt;", "text": "Dang, Carl, did you switch to Walmart PR team?\n\nWalmart is offering these workers a subsidy to take courses at thre\u2026 https://t.co/VvsLbuIjsm", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420020847767658506", "url": "https://t.co/VvsLbuIjsm"}], "user": {"created_at": "Wed Dec 03 07:58:06 +0000 2008", "description": "2021: Phil considers paying someone to badmouth Amazon online. He gets married for the second time in one year. || He/Him", "favourites_count": 85852, "followers_count": 1604, "friends_count": 1405, "geo_enabled": true, "id": 17832004, "id_str": "17832004", "listed_count": 103, "name": "Phil", "profile_background_color": "691B1B", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/17832004/1623003730", "profile_image_url": "http://pbs.twimg.com/profile_images/1401605199345692674/sKg3B2aD_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1401605199345692674/sKg3B2aD_normal.jpg", "profile_link_color": "611212", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "170C46", "profile_text_color": "666666", "screen_name": "PhilPhorever", "statuses_count": 271035, "withheld_in_countries": []}, "user_mentions": []}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Tue Jul 27 13:58:05 +0000 2021", "hashtags": [], "id": 1420020672483446795, "id_str": "1420020672483446795", "lang": "en", "retweet_count": 9, "retweeted_status": {"created_at": "Tue Jul 27 13:37:31 +0000 2021", "favorite_count": 22, "hashtags": [], "id": 1420015494850129930, "id_str": "1420015494850129930", "in_reply_to_screen_name": "reassuringURL", "in_reply_to_status_id": 1420015089302654977, "in_reply_to_user_id": 3187056242, "lang": "en", "retweet_count": 9, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Uni\u2026 https://t.co/4CTPEuQTUF", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420015494850129930", "url": "https://t.co/4CTPEuQTUF"}], "user": {"created_at": "Mon Jun 27 02:44:44 +0000 2011", "description": "Finance | Tech | China \ud83d\udc40| Navy vet | #GoHoos", "favourites_count": 12892, "followers_count": 224, "friends_count": 1195, "id": 324707378, "id_str": "324707378", "listed_count": 3, "location": "Alpha Centauri", "name": "apathetic Tim", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/324707378/1413625214", "profile_image_url": "http://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_link_color": "C91616", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "0084B4", "profile_use_background_image": true, "screen_name": "DoctorDirtNasty", "statuses_count": 16942, "withheld_in_countries": []}, "user_mentions": [{"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "RT @DoctorDirtNasty: @reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Univer\u2026", "urls": [], "user": {"created_at": "Sat Apr 02 01:47:50 +0000 2011", "description": "I'm the bronzed, muscly dude chillin' out in the Financial District. I see it all, baby. I hear it all, too. Unofficial af. He/him. Header by @BadgersTweetToo.", "favourites_count": 330655, "followers_count": 2388, "friends_count": 1404, "id": 275809002, "id_str": "275809002", "listed_count": 45, "location": "New York City", "name": "The Wall Street Bull", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/275809002/1352949738", "profile_image_url": "http://pbs.twimg.com/profile_images/2780666566/d26194502eec916ab63b64e436f011e4_normal.jpeg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/2780666566/d26194502eec916ab63b64e436f011e4_normal.jpeg", "profile_link_color": "0084B4", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "TheWallStBull", "statuses_count": 264397, "withheld_in_countries": []}, "user_mentions": [{"id": 324707378, "id_str": "324707378", "name": "apathetic Tim", "screen_name": "DoctorDirtNasty"}, {"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Tue Jul 27 13:39:47 +0000 2021", "favorite_count": 3, "hashtags": [], "id": 1420016068353921024, "id_str": "1420016068353921024", "in_reply_to_screen_name": "Bonecondor", "in_reply_to_status_id": 1420014586422509577, "in_reply_to_user_id": 709822647652196353, "lang": "en", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@Bonecondor \"Walmart's university partners, operating through Guild, include Southern New Hampshire University, Pur\u2026 https://t.co/N3MGufrqgx", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420016068353921024", "url": "https://t.co/N3MGufrqgx"}], "user": {"created_at": "Mon Dec 16 01:36:17 +0000 2019", "default_profile": true, "description": "Yeah, I went vegan for the chicks \n\nHere's why...\nhttps://t.co/hdqdhzQF3R", "favourites_count": 1080, "followers_count": 3, "friends_count": 259, "id": 1206387246095458305, "id_str": "1206387246095458305", "location": "Retired", "name": "ElectricVegan", "profile_background_color": "F5F8FA", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1206387246095458305/1613314623", "profile_image_url": "http://pbs.twimg.com/profile_images/1308834265581281281/3KYmYzI1_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1308834265581281281/3KYmYzI1_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "VeganElectric", "statuses_count": 1061, "url": "https://t.co/wjQjr73TAD", "withheld_in_countries": []}, "user_mentions": [{"id": 709822647652196353, "id_str": "709822647652196353", "name": "Chairman Birb Bernanke", "screen_name": "Bonecondor"}]}</t>
+    <t>{"created_at": "Wed Jul 28 15:21:10 +0000 2021", "favorite_count": 3, "hashtags": [], "id": 1420403967448674310, "id_str": "1420403967448674310", "in_reply_to_screen_name": "GrossmanManny", "in_reply_to_status_id": 1420382926005542915, "in_reply_to_user_id": 1391739495796596742, "lang": "en", "quoted_status": {"created_at": "Wed Jul 28 03:53:57 +0000 2021", "hashtags": [], "id": 1420231023900590086, "id_str": "1420231023900590086", "in_reply_to_screen_name": "DecoderOfTruth", "in_reply_to_status_id": 1419822806154375170, "in_reply_to_user_id": 2996519460, "lang": "en", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "HIV/AIDS at the same place where Dr. Albert LaVerne was on staff.\n\nHis wife Paule Passavant LaVerne, was gunned dow\u2026 https://t.co/9sHbDQb8D9", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420231023900590086", "url": "https://t.co/9sHbDQb8D9"}], "user": {"created_at": "Mon Jan 26 04:40:16 +0000 2015", "default_profile": true, "favourites_count": 129, "followers_count": 254, "friends_count": 7, "id": 2996519460, "id_str": "2996519460", "listed_count": 1, "name": "Julie", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/2996519460/1551662427", "profile_image_url": "http://pbs.twimg.com/profile_images/1413891794719285248/x771zpyU_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1413891794719285248/x771zpyU_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "DecoderOfTruth", "statuses_count": 4262, "withheld_in_countries": []}, "user_mentions": []}, "quoted_status_id": 1420231023900590086, "quoted_status_id_str": "1420231023900590086", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@GrossmanManny Your SOS research is bleeding over into my research\ud83d\ude2e\n\nDr. Albert LaVerne Senior psychiatrist at NY U\u2026 https://t.co/TIxqcp9kpk", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420403967448674310", "url": "https://t.co/TIxqcp9kpk"}], "user": {"created_at": "Mon Jan 26 04:40:16 +0000 2015", "default_profile": true, "favourites_count": 129, "followers_count": 254, "friends_count": 7, "id": 2996519460, "id_str": "2996519460", "listed_count": 1, "name": "Julie", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/2996519460/1551662427", "profile_image_url": "http://pbs.twimg.com/profile_images/1413891794719285248/x771zpyU_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1413891794719285248/x771zpyU_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "DecoderOfTruth", "statuses_count": 4262, "withheld_in_countries": []}, "user_mentions": [{"id": 1391739495796596742, "id_str": "1391739495796596742", "name": "Manny Grossman", "screen_name": "GrossmanManny"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Wed Jul 28 07:44:47 +0000 2021", "hashtags": [], "id": 1420289114918854656, "id_str": "1420289114918854656", "lang": "en", "retweet_count": 1, "retweeted_status": {"created_at": "Tue Jul 27 17:39:00 +0000 2021", "favorite_count": 10, "hashtags": [], "id": 1420076266208776193, "id_str": "1420076266208776193", "in_reply_to_screen_name": "carlquintanilla", "in_reply_to_status_id": 1420014215255965699, "in_reply_to_user_id": 114782468, "lang": "en", "retweet_count": 1, "source": "&lt;a href=\"http://twitter.com/download/android\" rel=\"nofollow\"&gt;Twitter for Android&lt;/a&gt;", "text": "@carlquintanilla All they're doing is playing catchup to other multi-billion $ companies.\nAnd this free tuition onl\u2026 https://t.co/r2w7oW5LAE", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420076266208776193", "url": "https://t.co/r2w7oW5LAE"}], "user": {"created_at": "Wed Oct 16 03:47:56 +0000 2013", "default_profile": true, "description": "Progressive woman who believes in calling out the injustices in America, whether by Democrats or GOP; strong gun laws; science; books; baseball; rock n roll\ud83c\udfb6\ud83c\udfb5", "favourites_count": 31814, "followers_count": 189, "friends_count": 752, "geo_enabled": true, "id": 717006051, "id_str": "717006051", "listed_count": 3, "location": "Belleville, IL", "name": "Diana - The O.H.", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/717006051/1613862055", "profile_image_url": "http://pbs.twimg.com/profile_images/1369357580255002626/AM3394Bp_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1369357580255002626/AM3394Bp_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "DianaWandersOn", "statuses_count": 6173, "withheld_in_countries": []}, "user_mentions": [{"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @DianaWandersOn: @carlquintanilla All they're doing is playing catchup to other multi-billion $ companies.\nAnd this free tuition only ap\u2026", "urls": [], "user": {"created_at": "Mon Nov 10 03:45:00 +0000 2008", "description": "\ud83c\udf0a\ud83c\udf0a#Spoonie, #Disabled #Vaccinated #LGBTQI+ #Humanist #Democrat #BLM #TimesUp #MeToo sexuality/human rights advocate #RESIST #Resistance #VoteBlue \ud83c\udf0a\ud83c\udf0a #FBR", "favourites_count": 288088, "followers_count": 7480, "friends_count": 7493, "id": 17280041, "id_str": "17280041", "listed_count": 8, "location": "New Orleans, LA", "name": "JamieJoy Loves Madam VP Harris \ud83c\udf0aPOTUS Biden\ud83c\udf0a#BLM", "profile_background_color": "F5E2C1", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme11/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme11/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/17280041/1537233953", "profile_image_url": "http://pbs.twimg.com/profile_images/1212460299032416263/h1z7A1Ia_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1212460299032416263/h1z7A1Ia_normal.jpg", "profile_link_color": "E81C4F", "profile_sidebar_border_color": "DBE9ED", "profile_sidebar_fill_color": "5C0B05", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "mindcaviar", "statuses_count": 102808, "url": "https://t.co/kP8RuibYYd", "withheld_in_countries": []}, "user_mentions": [{"id": 717006051, "id_str": "717006051", "name": "Diana - The O.H.", "screen_name": "DianaWandersOn"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Wed Jul 28 07:44:26 +0000 2021", "hashtags": [], "id": 1420289027337564161, "id_str": "1420289027337564161", "lang": "en", "retweet_count": 9, "retweeted_status": {"created_at": "Tue Jul 27 13:37:31 +0000 2021", "favorite_count": 22, "hashtags": [], "id": 1420015494850129930, "id_str": "1420015494850129930", "in_reply_to_screen_name": "reassuringURL", "in_reply_to_status_id": 1420015089302654977, "in_reply_to_user_id": 3187056242, "lang": "en", "retweet_count": 9, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Uni\u2026 https://t.co/4CTPEuQTUF", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420015494850129930", "url": "https://t.co/4CTPEuQTUF"}], "user": {"created_at": "Mon Jun 27 02:44:44 +0000 2011", "description": "Finance | Tech | China \ud83d\udc40| Navy vet | #GoHoos", "favourites_count": 12892, "followers_count": 224, "friends_count": 1195, "id": 324707378, "id_str": "324707378", "listed_count": 3, "location": "Alpha Centauri", "name": "apathetic Tim", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/324707378/1413625214", "profile_image_url": "http://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_link_color": "C91616", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "0084B4", "profile_use_background_image": true, "screen_name": "DoctorDirtNasty", "statuses_count": 16942, "withheld_in_countries": []}, "user_mentions": [{"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @DoctorDirtNasty: @reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Univer\u2026", "urls": [], "user": {"created_at": "Mon Nov 10 03:45:00 +0000 2008", "description": "\ud83c\udf0a\ud83c\udf0a#Spoonie, #Disabled #Vaccinated #LGBTQI+ #Humanist #Democrat #BLM #TimesUp #MeToo sexuality/human rights advocate #RESIST #Resistance #VoteBlue \ud83c\udf0a\ud83c\udf0a #FBR", "favourites_count": 288088, "followers_count": 7480, "friends_count": 7493, "id": 17280041, "id_str": "17280041", "listed_count": 8, "location": "New Orleans, LA", "name": "JamieJoy Loves Madam VP Harris \ud83c\udf0aPOTUS Biden\ud83c\udf0a#BLM", "profile_background_color": "F5E2C1", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme11/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme11/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/17280041/1537233953", "profile_image_url": "http://pbs.twimg.com/profile_images/1212460299032416263/h1z7A1Ia_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1212460299032416263/h1z7A1Ia_normal.jpg", "profile_link_color": "E81C4F", "profile_sidebar_border_color": "DBE9ED", "profile_sidebar_fill_color": "5C0B05", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "mindcaviar", "statuses_count": 102808, "url": "https://t.co/kP8RuibYYd", "withheld_in_countries": []}, "user_mentions": [{"id": 324707378, "id_str": "324707378", "name": "apathetic Tim", "screen_name": "DoctorDirtNasty"}, {"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Wed Jul 28 06:27:23 +0000 2021", "hashtags": [], "id": 1420269635472019460, "id_str": "1420269635472019460", "lang": "en", "retweet_count": 9, "retweeted_status": {"created_at": "Tue Jul 27 13:37:31 +0000 2021", "favorite_count": 22, "hashtags": [], "id": 1420015494850129930, "id_str": "1420015494850129930", "in_reply_to_screen_name": "reassuringURL", "in_reply_to_status_id": 1420015089302654977, "in_reply_to_user_id": 3187056242, "lang": "en", "retweet_count": 9, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Uni\u2026 https://t.co/4CTPEuQTUF", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420015494850129930", "url": "https://t.co/4CTPEuQTUF"}], "user": {"created_at": "Mon Jun 27 02:44:44 +0000 2011", "description": "Finance | Tech | China \ud83d\udc40| Navy vet | #GoHoos", "favourites_count": 12892, "followers_count": 224, "friends_count": 1195, "id": 324707378, "id_str": "324707378", "listed_count": 3, "location": "Alpha Centauri", "name": "apathetic Tim", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/324707378/1413625214", "profile_image_url": "http://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_link_color": "C91616", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "0084B4", "profile_use_background_image": true, "screen_name": "DoctorDirtNasty", "statuses_count": 16942, "withheld_in_countries": []}, "user_mentions": [{"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"http://twitter.com/download/android\" rel=\"nofollow\"&gt;Twitter for Android&lt;/a&gt;", "text": "RT @DoctorDirtNasty: @reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Univer\u2026", "urls": [], "user": {"created_at": "Wed Apr 03 09:55:40 +0000 2013", "default_profile": true, "description": "Community Activist, Guitar Picker, Blues Harmonica, Rabble Rouser, Smart Aleck, Widower, Dad, Brother, Amigo/Friend, WarriorBrother, Santa,El Camino de Santiago", "favourites_count": 548, "followers_count": 788, "friends_count": 2524, "geo_enabled": true, "id": 1324265089, "id_str": "1324265089", "listed_count": 9, "location": "Everett, WA", "name": "Michael Trujillo", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1324265089/1466688941", "profile_image_url": "http://pbs.twimg.com/profile_images/803849515098841088/dZRSdHdW_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/803849515098841088/dZRSdHdW_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "lionman47", "statuses_count": 119351, "withheld_in_countries": []}, "user_mentions": [{"id": 324707378, "id_str": "324707378", "name": "apathetic Tim", "screen_name": "DoctorDirtNasty"}, {"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Tue Jul 27 22:27:30 +0000 2021", "favorite_count": 1, "hashtags": [], "id": 1420148868944068614, "id_str": "1420148868944068614", "in_reply_to_screen_name": "DecoderOfTruth", "in_reply_to_status_id": 1420137058991964164, "in_reply_to_user_id": 2996519460, "lang": "en", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "Sr. psychiatrist at NY University-Bellevue Medical Center, Albert is known for curing people from drug/alcohol addi\u2026 https://t.co/0DBVJaUYRm", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420148868944068614", "url": "https://t.co/0DBVJaUYRm"}], "user": {"created_at": "Mon Jan 26 04:40:16 +0000 2015", "default_profile": true, "favourites_count": 129, "followers_count": 254, "friends_count": 7, "id": 2996519460, "id_str": "2996519460", "listed_count": 1, "name": "Julie", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/2996519460/1551662427", "profile_image_url": "http://pbs.twimg.com/profile_images/1413891794719285248/x771zpyU_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1413891794719285248/x771zpyU_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "DecoderOfTruth", "statuses_count": 4262, "withheld_in_countries": []}, "user_mentions": []}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Tue Jul 27 21:33:00 +0000 2021", "hashtags": [], "id": 1420135155880976387, "id_str": "1420135155880976387", "in_reply_to_screen_name": "DecoderOfTruth", "in_reply_to_status_id": 1420130449477701633, "in_reply_to_user_id": 2996519460, "lang": "en", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "8.1/ Bellevue opened \u201cpavilion for the insane\u201d in 1879 and a alcoholic ward in 1892. These were part of the main ho\u2026 https://t.co/sywGoNTzWf", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420135155880976387", "url": "https://t.co/sywGoNTzWf"}], "user": {"created_at": "Mon Jan 26 04:40:16 +0000 2015", "default_profile": true, "favourites_count": 129, "followers_count": 254, "friends_count": 7, "id": 2996519460, "id_str": "2996519460", "listed_count": 1, "name": "Julie", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/2996519460/1551662427", "profile_image_url": "http://pbs.twimg.com/profile_images/1413891794719285248/x771zpyU_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1413891794719285248/x771zpyU_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "DecoderOfTruth", "statuses_count": 4262, "withheld_in_countries": []}, "user_mentions": []}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Tue Jul 27 19:41:54 +0000 2021", "favorite_count": 2, "hashtags": [], "id": 1420107195060944896, "id_str": "1420107195060944896", "lang": "en", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "Bellevue-based Gaia Platform, along with two of its Snoqualmie Valley employees, are working with AI Racing Tech an\u2026 https://t.co/rsZGCJwAXS", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420107195060944896", "url": "https://t.co/rsZGCJwAXS"}], "user": {"created_at": "Wed Sep 22 17:34:23 +0000 2010", "description": "Snoqualmie Valley News. Real resident. Up to date happenings and breaking news in the Snoqualmie Valley.", "favourites_count": 1307, "followers_count": 2243, "friends_count": 501, "id": 193780411, "id_str": "193780411", "listed_count": 30, "location": "Snoqualmie Valley, WA", "name": "Livingsnoqualmie.com", "profile_background_color": "022330", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/193780411/1539109526", "profile_image_url": "http://pbs.twimg.com/profile_images/938535260718997504/9GHoWzOV_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/938535260718997504/9GHoWzOV_normal.jpg", "profile_link_color": "0084B4", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "LivingSno", "statuses_count": 5818, "url": "http://t.co/CN8HLNkKuz", "withheld_in_countries": []}, "user_mentions": []}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Tue Jul 27 17:53:59 +0000 2021", "hashtags": [], "id": 1420080035797553162, "id_str": "1420080035797553162", "lang": "en", "retweet_count": 9, "retweeted_status": {"created_at": "Tue Jul 27 13:37:31 +0000 2021", "favorite_count": 22, "hashtags": [], "id": 1420015494850129930, "id_str": "1420015494850129930", "in_reply_to_screen_name": "reassuringURL", "in_reply_to_status_id": 1420015089302654977, "in_reply_to_user_id": 3187056242, "lang": "en", "retweet_count": 9, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Uni\u2026 https://t.co/4CTPEuQTUF", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420015494850129930", "url": "https://t.co/4CTPEuQTUF"}], "user": {"created_at": "Mon Jun 27 02:44:44 +0000 2011", "description": "Finance | Tech | China \ud83d\udc40| Navy vet | #GoHoos", "favourites_count": 12892, "followers_count": 224, "friends_count": 1195, "id": 324707378, "id_str": "324707378", "listed_count": 3, "location": "Alpha Centauri", "name": "apathetic Tim", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/324707378/1413625214", "profile_image_url": "http://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_link_color": "C91616", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "0084B4", "profile_use_background_image": true, "screen_name": "DoctorDirtNasty", "statuses_count": 16942, "withheld_in_countries": []}, "user_mentions": [{"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "RT @DoctorDirtNasty: @reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Univer\u2026", "urls": [], "user": {"created_at": "Sun Jan 26 01:19:55 +0000 2014", "default_profile": true, "description": "Educational Futurist. Associate Director. Parent. Womanist. Researcher. Proud FSU Seminole. KDX \ud83d\udc27. ODK. Retweets are not endorsements just evidence of reading", "favourites_count": 53648, "followers_count": 550, "friends_count": 419, "geo_enabled": true, "id": 2310977114, "id_str": "2310977114", "listed_count": 103, "location": "FSU Tallahassee, Fl", "name": "Dr. Barefoot Scholar", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/2310977114/1592108441", "profile_image_url": "http://pbs.twimg.com/profile_images/1314247200852017152/Lr-RVEkc_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1314247200852017152/Lr-RVEkc_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "SophiaRahming1", "statuses_count": 187517, "withheld_in_countries": []}, "user_mentions": [{"id": 324707378, "id_str": "324707378", "name": "apathetic Tim", "screen_name": "DoctorDirtNasty"}, {"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Tue Jul 27 17:39:00 +0000 2021", "favorite_count": 10, "hashtags": [], "id": 1420076266208776193, "id_str": "1420076266208776193", "in_reply_to_screen_name": "carlquintanilla", "in_reply_to_status_id": 1420014215255965699, "in_reply_to_user_id": 114782468, "lang": "en", "retweet_count": 1, "source": "&lt;a href=\"http://twitter.com/download/android\" rel=\"nofollow\"&gt;Twitter for Android&lt;/a&gt;", "text": "@carlquintanilla All they're doing is playing catchup to other multi-billion $ companies.\nAnd this free tuition onl\u2026 https://t.co/r2w7oW5LAE", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420076266208776193", "url": "https://t.co/r2w7oW5LAE"}], "user": {"created_at": "Wed Oct 16 03:47:56 +0000 2013", "default_profile": true, "description": "Progressive woman who believes in calling out the injustices in America, whether by Democrats or GOP; strong gun laws; science; books; baseball; rock n roll\ud83c\udfb6\ud83c\udfb5", "favourites_count": 31814, "followers_count": 189, "friends_count": 752, "geo_enabled": true, "id": 717006051, "id_str": "717006051", "listed_count": 3, "location": "Belleville, IL", "name": "Diana - The O.H.", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/717006051/1613862055", "profile_image_url": "http://pbs.twimg.com/profile_images/1369357580255002626/AM3394Bp_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1369357580255002626/AM3394Bp_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "DianaWandersOn", "statuses_count": 6173, "withheld_in_countries": []}, "user_mentions": [{"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Tue Jul 27 16:32:50 +0000 2021", "hashtags": [], "id": 1420059615732064260, "id_str": "1420059615732064260", "lang": "en", "retweet_count": 9, "retweeted_status": {"created_at": "Tue Jul 27 13:37:31 +0000 2021", "favorite_count": 22, "hashtags": [], "id": 1420015494850129930, "id_str": "1420015494850129930", "in_reply_to_screen_name": "reassuringURL", "in_reply_to_status_id": 1420015089302654977, "in_reply_to_user_id": 3187056242, "lang": "en", "retweet_count": 9, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Uni\u2026 https://t.co/4CTPEuQTUF", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420015494850129930", "url": "https://t.co/4CTPEuQTUF"}], "user": {"created_at": "Mon Jun 27 02:44:44 +0000 2011", "description": "Finance | Tech | China \ud83d\udc40| Navy vet | #GoHoos", "favourites_count": 12892, "followers_count": 224, "friends_count": 1195, "id": 324707378, "id_str": "324707378", "listed_count": 3, "location": "Alpha Centauri", "name": "apathetic Tim", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/324707378/1413625214", "profile_image_url": "http://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_link_color": "C91616", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "0084B4", "profile_use_background_image": true, "screen_name": "DoctorDirtNasty", "statuses_count": 16942, "withheld_in_countries": []}, "user_mentions": [{"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "RT @DoctorDirtNasty: @reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Univer\u2026", "urls": [], "user": {"created_at": "Sun Mar 22 15:19:23 +0000 2009", "description": "openly black. boston. los angeles. duke. bama. memphis.", "favourites_count": 1851, "followers_count": 385, "friends_count": 304, "geo_enabled": true, "id": 25829276, "id_str": "25829276", "listed_count": 19, "location": "twitter.", "name": "maxine shaw", "profile_background_color": "BADFCD", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme12/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme12/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/25829276/1407940765", "profile_image_url": "http://pbs.twimg.com/profile_images/1317811173501358080/hasJGqMi_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1317811173501358080/hasJGqMi_normal.jpg", "profile_link_color": "FF0000", "profile_sidebar_border_color": "F2E195", "profile_sidebar_fill_color": "FFF7CC", "profile_text_color": "0C3E53", "profile_use_background_image": true, "screen_name": "SuperRegular", "statuses_count": 68413, "withheld_in_countries": []}, "user_mentions": [{"id": 324707378, "id_str": "324707378", "name": "apathetic Tim", "screen_name": "DoctorDirtNasty"}, {"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Tue Jul 27 16:10:29 +0000 2021", "hashtags": [], "id": 1420053990541348872, "id_str": "1420053990541348872", "lang": "en", "retweet_count": 9, "retweeted_status": {"created_at": "Tue Jul 27 13:37:31 +0000 2021", "favorite_count": 22, "hashtags": [], "id": 1420015494850129930, "id_str": "1420015494850129930", "in_reply_to_screen_name": "reassuringURL", "in_reply_to_status_id": 1420015089302654977, "in_reply_to_user_id": 3187056242, "lang": "en", "retweet_count": 9, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Uni\u2026 https://t.co/4CTPEuQTUF", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420015494850129930", "url": "https://t.co/4CTPEuQTUF"}], "user": {"created_at": "Mon Jun 27 02:44:44 +0000 2011", "description": "Finance | Tech | China \ud83d\udc40| Navy vet | #GoHoos", "favourites_count": 12892, "followers_count": 224, "friends_count": 1195, "id": 324707378, "id_str": "324707378", "listed_count": 3, "location": "Alpha Centauri", "name": "apathetic Tim", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/324707378/1413625214", "profile_image_url": "http://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_link_color": "C91616", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "0084B4", "profile_use_background_image": true, "screen_name": "DoctorDirtNasty", "statuses_count": 16942, "withheld_in_countries": []}, "user_mentions": [{"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @DoctorDirtNasty: @reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Univer\u2026", "urls": [], "user": {"created_at": "Sat Mar 21 00:24:34 +0000 2009", "description": "\ud83d\uddfd", "favourites_count": 29696, "followers_count": 165, "friends_count": 1254, "id": 25607309, "id_str": "25607309", "location": "NJ", "name": "D80s", "profile_background_color": "352726", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme5/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme5/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/25607309/1597543506", "profile_image_url": "http://pbs.twimg.com/profile_images/858122100820910081/6yUh3jU-_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/858122100820910081/6yUh3jU-_normal.jpg", "profile_link_color": "D02B55", "profile_sidebar_border_color": "829D5E", "profile_sidebar_fill_color": "99CC33", "profile_text_color": "3E4415", "profile_use_background_image": true, "screen_name": "D80s", "statuses_count": 96813, "withheld_in_countries": []}, "user_mentions": [{"id": 324707378, "id_str": "324707378", "name": "apathetic Tim", "screen_name": "DoctorDirtNasty"}, {"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Tue Jul 27 15:40:37 +0000 2021", "hashtags": [], "id": 1420046473241137153, "id_str": "1420046473241137153", "lang": "en", "retweet_count": 9, "retweeted_status": {"created_at": "Tue Jul 27 13:37:31 +0000 2021", "favorite_count": 22, "hashtags": [], "id": 1420015494850129930, "id_str": "1420015494850129930", "in_reply_to_screen_name": "reassuringURL", "in_reply_to_status_id": 1420015089302654977, "in_reply_to_user_id": 3187056242, "lang": "en", "retweet_count": 9, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Uni\u2026 https://t.co/4CTPEuQTUF", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420015494850129930", "url": "https://t.co/4CTPEuQTUF"}], "user": {"created_at": "Mon Jun 27 02:44:44 +0000 2011", "description": "Finance | Tech | China \ud83d\udc40| Navy vet | #GoHoos", "favourites_count": 12892, "followers_count": 224, "friends_count": 1195, "id": 324707378, "id_str": "324707378", "listed_count": 3, "location": "Alpha Centauri", "name": "apathetic Tim", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/324707378/1413625214", "profile_image_url": "http://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_link_color": "C91616", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "0084B4", "profile_use_background_image": true, "screen_name": "DoctorDirtNasty", "statuses_count": 16942, "withheld_in_countries": []}, "user_mentions": [{"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"http://twitter.com/download/android\" rel=\"nofollow\"&gt;Twitter for Android&lt;/a&gt;", "text": "RT @DoctorDirtNasty: @reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Univer\u2026", "urls": [], "user": {"created_at": "Mon Sep 28 03:03:22 +0000 2009", "default_profile": true, "favourites_count": 27224, "followers_count": 784, "friends_count": 1794, "id": 77908436, "id_str": "77908436", "listed_count": 33, "name": "Jennifer Bills", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_image_url": "http://pbs.twimg.com/profile_images/712391911353372672/V7vEnQ81_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/712391911353372672/V7vEnQ81_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "JJBills14", "statuses_count": 78368, "withheld_in_countries": []}, "user_mentions": [{"id": 324707378, "id_str": "324707378", "name": "apathetic Tim", "screen_name": "DoctorDirtNasty"}, {"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Tue Jul 27 15:01:14 +0000 2021", "hashtags": [], "id": 1420036564667846657, "id_str": "1420036564667846657", "lang": "en", "retweet_count": 9, "retweeted_status": {"created_at": "Tue Jul 27 13:37:31 +0000 2021", "favorite_count": 22, "hashtags": [], "id": 1420015494850129930, "id_str": "1420015494850129930", "in_reply_to_screen_name": "reassuringURL", "in_reply_to_status_id": 1420015089302654977, "in_reply_to_user_id": 3187056242, "lang": "en", "retweet_count": 9, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Uni\u2026 https://t.co/4CTPEuQTUF", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420015494850129930", "url": "https://t.co/4CTPEuQTUF"}], "user": {"created_at": "Mon Jun 27 02:44:44 +0000 2011", "description": "Finance | Tech | China \ud83d\udc40| Navy vet | #GoHoos", "favourites_count": 12892, "followers_count": 224, "friends_count": 1195, "id": 324707378, "id_str": "324707378", "listed_count": 3, "location": "Alpha Centauri", "name": "apathetic Tim", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/324707378/1413625214", "profile_image_url": "http://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_link_color": "C91616", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "0084B4", "profile_use_background_image": true, "screen_name": "DoctorDirtNasty", "statuses_count": 16942, "withheld_in_countries": []}, "user_mentions": [{"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @DoctorDirtNasty: @reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Univer\u2026", "urls": [], "user": {"created_at": "Fri Apr 08 22:19:12 +0000 2016", "description": "product mgr | project mgr | data wrangler | novice data viz designer | Vegetarian", "favourites_count": 122505, "followers_count": 875, "friends_count": 1030, "id": 718563872806805504, "id_str": "718563872806805504", "listed_count": 163, "location": "Kingston/Boston", "name": "Glen Dixon", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/718563872806805504/1627132416", "profile_image_url": "http://pbs.twimg.com/profile_images/1420412487615270917/6wyxU2Dv_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1420412487615270917/6wyxU2Dv_normal.jpg", "profile_link_color": "19CF86", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "000000", "profile_text_color": "000000", "screen_name": "glenrdixon", "statuses_count": 75370, "withheld_in_countries": []}, "user_mentions": [{"id": 324707378, "id_str": "324707378", "name": "apathetic Tim", "screen_name": "DoctorDirtNasty"}, {"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Tue Jul 27 13:58:47 +0000 2021", "hashtags": [], "id": 1420020847767658506, "id_str": "1420020847767658506", "lang": "en", "quoted_status": {"created_at": "Tue Jul 27 13:32:26 +0000 2021", "favorite_count": 9119, "hashtags": [], "id": 1420014215255965699, "id_str": "1420014215255965699", "lang": "en", "retweet_count": 1705, "source": "&lt;a href=\"https://about.twitter.com/products/tweetdeck\" rel=\"nofollow\"&gt;TweetDeck&lt;/a&gt;", "text": "(Reuters) - Walmart Inc on Tuesday  said it will pay the full cost of college tuition and books for  its roughly 1.\u2026 https://t.co/2c7ZZRrTs2", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420014215255965699", "url": "https://t.co/2c7ZZRrTs2"}], "user": {"created_at": "Tue Feb 16 15:59:04 +0000 2010", "description": "20+ years @CNBC &amp; @NBCNews / Peabody Award, Emmy, DuPont recipient / @WSJ alum / \u201cOnly one rule that I know of: goddamn it, you\u2019ve got to be kind.\u201d - Vonnegut", "favourites_count": 2396, "followers_count": 308199, "friends_count": 5379, "geo_enabled": true, "id": 114782468, "id_str": "114782468", "listed_count": 4822, "location": "nyc", "name": "Carl Quintanilla", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/114782468/1627376325", "profile_image_url": "http://pbs.twimg.com/profile_images/1214244686786965510/OAxLuUGH_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1214244686786965510/OAxLuUGH_normal.jpg", "profile_link_color": "3B94D9", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "FFFFFF", "profile_text_color": "000000", "profile_use_background_image": true, "screen_name": "carlquintanilla", "statuses_count": 90245, "url": "https://t.co/CHozTuBfc5", "verified": true, "withheld_in_countries": []}, "user_mentions": []}, "quoted_status_id": 1420014215255965699, "quoted_status_id_str": "1420014215255965699", "source": "&lt;a href=\"https://about.twitter.com/products/tweetdeck\" rel=\"nofollow\"&gt;TweetDeck&lt;/a&gt;", "text": "Dang, Carl, did you switch to Walmart PR team?\n\nWalmart is offering these workers a subsidy to take courses at thre\u2026 https://t.co/VvsLbuIjsm", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420020847767658506", "url": "https://t.co/VvsLbuIjsm"}], "user": {"created_at": "Wed Dec 03 07:58:06 +0000 2008", "description": "2021: Phil considers paying someone to badmouth Amazon online. He gets married for the second time in one year. || He/Him", "favourites_count": 85858, "followers_count": 1604, "friends_count": 1405, "geo_enabled": true, "id": 17832004, "id_str": "17832004", "listed_count": 103, "name": "Phil", "profile_background_color": "691B1B", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/17832004/1623003730", "profile_image_url": "http://pbs.twimg.com/profile_images/1401605199345692674/sKg3B2aD_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1401605199345692674/sKg3B2aD_normal.jpg", "profile_link_color": "611212", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "170C46", "profile_text_color": "666666", "screen_name": "PhilPhorever", "statuses_count": 271038, "withheld_in_countries": []}, "user_mentions": []}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Tue Jul 27 13:58:05 +0000 2021", "hashtags": [], "id": 1420020672483446795, "id_str": "1420020672483446795", "lang": "en", "retweet_count": 9, "retweeted_status": {"created_at": "Tue Jul 27 13:37:31 +0000 2021", "favorite_count": 22, "hashtags": [], "id": 1420015494850129930, "id_str": "1420015494850129930", "in_reply_to_screen_name": "reassuringURL", "in_reply_to_status_id": 1420015089302654977, "in_reply_to_user_id": 3187056242, "lang": "en", "retweet_count": 9, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Uni\u2026 https://t.co/4CTPEuQTUF", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420015494850129930", "url": "https://t.co/4CTPEuQTUF"}], "user": {"created_at": "Mon Jun 27 02:44:44 +0000 2011", "description": "Finance | Tech | China \ud83d\udc40| Navy vet | #GoHoos", "favourites_count": 12892, "followers_count": 224, "friends_count": 1195, "id": 324707378, "id_str": "324707378", "listed_count": 3, "location": "Alpha Centauri", "name": "apathetic Tim", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/324707378/1413625214", "profile_image_url": "http://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_link_color": "C91616", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "0084B4", "profile_use_background_image": true, "screen_name": "DoctorDirtNasty", "statuses_count": 16942, "withheld_in_countries": []}, "user_mentions": [{"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}, "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "RT @DoctorDirtNasty: @reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Univer\u2026", "urls": [], "user": {"created_at": "Sat Apr 02 01:47:50 +0000 2011", "description": "I'm the bronzed, muscly dude chillin' out in the Financial District. I see it all, baby. I hear it all, too. Unofficial af. He/him. Header by @BadgersTweetToo.", "favourites_count": 330679, "followers_count": 2388, "friends_count": 1404, "id": 275809002, "id_str": "275809002", "listed_count": 45, "location": "New York City", "name": "The Wall Street Bull", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/275809002/1352949738", "profile_image_url": "http://pbs.twimg.com/profile_images/2780666566/d26194502eec916ab63b64e436f011e4_normal.jpeg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/2780666566/d26194502eec916ab63b64e436f011e4_normal.jpeg", "profile_link_color": "0084B4", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "TheWallStBull", "statuses_count": 264421, "withheld_in_countries": []}, "user_mentions": [{"id": 324707378, "id_str": "324707378", "name": "apathetic Tim", "screen_name": "DoctorDirtNasty"}, {"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Tue Jul 27 13:39:47 +0000 2021", "favorite_count": 3, "hashtags": [], "id": 1420016068353921024, "id_str": "1420016068353921024", "in_reply_to_screen_name": "Bonecondor", "in_reply_to_status_id": 1420014586422509577, "in_reply_to_user_id": 709822647652196353, "lang": "en", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@Bonecondor \"Walmart's university partners, operating through Guild, include Southern New Hampshire University, Pur\u2026 https://t.co/N3MGufrqgx", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420016068353921024", "url": "https://t.co/N3MGufrqgx"}], "user": {"created_at": "Mon Dec 16 01:36:17 +0000 2019", "default_profile": true, "description": "Yeah, I went vegan for the chicks \n\nHere's why...\nhttps://t.co/hdqdhzQF3R", "favourites_count": 1082, "followers_count": 3, "friends_count": 259, "id": 1206387246095458305, "id_str": "1206387246095458305", "location": "Retired", "name": "ElectricVegan", "profile_background_color": "F5F8FA", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1206387246095458305/1613314623", "profile_image_url": "http://pbs.twimg.com/profile_images/1308834265581281281/3KYmYzI1_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1308834265581281281/3KYmYzI1_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "VeganElectric", "statuses_count": 1061, "url": "https://t.co/wjQjr73TAD", "withheld_in_countries": []}, "user_mentions": [{"id": 709822647652196353, "id_str": "709822647652196353", "name": "Chairman Birb Bernanke", "screen_name": "Bonecondor"}]}</t>
   </si>
   <si>
     <t>{"created_at": "Tue Jul 27 13:37:31 +0000 2021", "favorite_count": 22, "hashtags": [], "id": 1420015494850129930, "id_str": "1420015494850129930", "in_reply_to_screen_name": "reassuringURL", "in_reply_to_status_id": 1420015089302654977, "in_reply_to_user_id": 3187056242, "lang": "en", "retweet_count": 9, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@reassuringURL @carlquintanilla \"Full- and part-time Walmart workers can use the subsidy to take courses at the Uni\u2026 https://t.co/4CTPEuQTUF", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1420015494850129930", "url": "https://t.co/4CTPEuQTUF"}], "user": {"created_at": "Mon Jun 27 02:44:44 +0000 2011", "description": "Finance | Tech | China \ud83d\udc40| Navy vet | #GoHoos", "favourites_count": 12892, "followers_count": 224, "friends_count": 1195, "id": 324707378, "id_str": "324707378", "listed_count": 3, "location": "Alpha Centauri", "name": "apathetic Tim", "profile_background_color": "000000", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/324707378/1413625214", "profile_image_url": "http://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1271131761846759424/K7kV2-0K_normal.jpg", "profile_link_color": "C91616", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "0084B4", "profile_use_background_image": true, "screen_name": "DoctorDirtNasty", "statuses_count": 16942, "withheld_in_countries": []}, "user_mentions": [{"id": 3187056242, "id_str": "3187056242", "name": "Brad", "screen_name": "reassuringURL"}, {"id": 114782468, "id_str": "114782468", "name": "Carl Quintanilla", "screen_name": "carlquintanilla"}]}</t>
@@ -181,7 +187,7 @@
     <t>{"created_at": "Tue Jul 27 01:03:10 +0000 2021", "hashtags": [], "id": 1419825659380109314, "id_str": "1419825659380109314", "lang": "en", "retweet_count": 2, "retweeted_status": {"created_at": "Mon Jul 12 17:01:00 +0000 2021", "favorite_count": 6, "hashtags": [], "id": 1414630885295546373, "id_str": "1414630885295546373", "lang": "en", "retweet_count": 2, "source": "&lt;a href=\"http://gainapp.com\" rel=\"nofollow\"&gt;Gain Platform&lt;/a&gt;", "text": "\"Earning my degree would not have been possible without the support of my amazing family. It takes a village and I\u2026 https://t.co/gjZmjf2sTd", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1414630885295546373", "url": "https://t.co/gjZmjf2sTd"}], "user": {"created_at": "Tue Oct 23 13:48:23 +0000 2007", "description": "Our learning programs combine mastery of deep, career-relevant knowledge and powerful professional skills, so you are prepared with tools for success.", "favourites_count": 4123, "followers_count": 9169, "friends_count": 2576, "id": 9623092, "id_str": "9623092", "listed_count": 210, "location": "Nebraska", "name": "Bellevue University", "profile_background_color": "4F3674", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme10/bg.gif", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/9623092/1614634074", "profile_image_url": "http://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1250129239669645312/Qym44FTM_normal.png", "profile_link_color": "4F3674", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "4A2334", "profile_text_color": "D5EC08", "screen_name": "BellevueU", "statuses_count": 6051, "url": "https://t.co/0hQEZBjUQK", "withheld_in_countries": []}, "user_mentions": []}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @BellevueU: \"Earning my degree would not have been possible without the support of my amazing family. It takes a village and I am gratef\u2026", "urls": [], "user": {"created_at": "Wed Apr 15 02:04:59 +0000 2009", "description": "#Multichannel #Marketing #PublicRelations #Content #Education #HigherLearning #HigherEd #EdTech #Online #APR @BellevueU Tweets are my own", "favourites_count": 19579, "followers_count": 1613, "friends_count": 3451, "geo_enabled": true, "id": 31305344, "id_str": "31305344", "listed_count": 47, "location": "Omaha, NE, USA", "name": "Cris Hay-Merchant, APR", "profile_background_color": "022330", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/31305344/1550669488", "profile_image_url": "http://pbs.twimg.com/profile_images/677951382775709696/azMKWnDc_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/677951382775709696/azMKWnDc_normal.jpg", "profile_link_color": "981CEB", "profile_sidebar_border_color": "000000", "profile_sidebar_fill_color": "000000", "profile_text_color": "000000", "profile_use_background_image": true, "screen_name": "crishm", "statuses_count": 7226, "url": "https://t.co/MtmXUxu29p", "withheld_in_countries": []}, "user_mentions": [{"id": 9623092, "id_str": "9623092", "name": "Bellevue University", "screen_name": "BellevueU"}]}</t>
   </si>
   <si>
-    <t>{"created_at": "Mon Jul 26 19:30:14 +0000 2021", "favorite_count": 1, "hashtags": [], "id": 1419741871211962378, "id_str": "1419741871211962378", "lang": "en", "source": "&lt;a href=\"http://www.socialnewsdesk.com\" rel=\"nofollow\"&gt;SocialNewsDesk&lt;/a&gt;", "text": "Current USL League One member, Union Omaha, will host an exhibition match against the Bellevue University men\u2019s soc\u2026 https://t.co/zVC83khPS2", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1419741871211962378", "url": "https://t.co/zVC83khPS2"}], "user": {"created_at": "Tue Apr 21 13:09:29 +0000 2009", "default_profile": true, "description": "Your news source for the City of Bellevue.", "favourites_count": 140, "followers_count": 2887, "friends_count": 243, "id": 33897176, "id_str": "33897176", "listed_count": 58, "location": "Bellevue, Nebraska", "name": "Bellevue Leader", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/33897176/1423597716", "profile_image_url": "http://pbs.twimg.com/profile_images/557633017326235648/CqiyR7PD_normal.jpeg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/557633017326235648/CqiyR7PD_normal.jpeg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "BellevueLeader", "statuses_count": 6329, "url": "http://t.co/J6hztG06af", "withheld_in_countries": []}, "user_mentions": []}</t>
+    <t>{"created_at": "Mon Jul 26 19:30:14 +0000 2021", "favorite_count": 1, "hashtags": [], "id": 1419741871211962378, "id_str": "1419741871211962378", "lang": "en", "source": "&lt;a href=\"http://www.socialnewsdesk.com\" rel=\"nofollow\"&gt;SocialNewsDesk&lt;/a&gt;", "text": "Current USL League One member, Union Omaha, will host an exhibition match against the Bellevue University men\u2019s soc\u2026 https://t.co/zVC83khPS2", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1419741871211962378", "url": "https://t.co/zVC83khPS2"}], "user": {"created_at": "Tue Apr 21 13:09:29 +0000 2009", "default_profile": true, "description": "Your news source for the City of Bellevue.", "favourites_count": 140, "followers_count": 2886, "friends_count": 243, "id": 33897176, "id_str": "33897176", "listed_count": 58, "location": "Bellevue, Nebraska", "name": "Bellevue Leader", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/33897176/1423597716", "profile_image_url": "http://pbs.twimg.com/profile_images/557633017326235648/CqiyR7PD_normal.jpeg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/557633017326235648/CqiyR7PD_normal.jpeg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "BellevueLeader", "statuses_count": 6330, "url": "http://t.co/J6hztG06af", "withheld_in_countries": []}, "user_mentions": []}</t>
   </si>
   <si>
     <t>{"created_at": "Mon Jul 26 18:31:13 +0000 2021", "favorite_count": 1, "hashtags": [], "id": 1419727018791428100, "id_str": "1419727018791428100", "lang": "en", "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "\ud83c\udf92 Free backpack giveaway this Saturday, 7/31 for Shelby County school children\n\ud83d\udcd3\u270f\ufe0f Elementary-age school supplies i\u2026 https://t.co/4VO2ttBI5b", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1419727018791428100", "url": "https://t.co/4VO2ttBI5b"}], "user": {"created_at": "Fri Apr 24 15:56:16 +0000 2009", "description": "Providing high quality, cost-effective patient and family-centered care in Memphis, TN.", "favourites_count": 1024, "followers_count": 5093, "friends_count": 479, "geo_enabled": true, "id": 34960612, "id_str": "34960612", "listed_count": 164, "location": "Memphis, TN", "name": "Methodist Healthcare", "profile_background_color": "536AB2", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/34960612/1622558416", "profile_image_url": "http://pbs.twimg.com/profile_images/1083478110144790528/yHCOsEOP_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1083478110144790528/yHCOsEOP_normal.jpg", "profile_link_color": "91004B", "profile_sidebar_border_color": "FFFFFF", "profile_sidebar_fill_color": "E5E5E5", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "MethodistHlth", "statuses_count": 3348, "url": "https://t.co/p7clUT9oaD", "withheld_in_countries": []}, "user_mentions": []}</t>
@@ -193,22 +199,22 @@
     <t>{"created_at": "Mon Jul 26 14:03:20 +0000 2021", "favorite_count": 1, "hashtags": [], "id": 1419659604926083075, "id_str": "1419659604926083075", "lang": "en", "media": [{"display_url": "pic.twitter.com/keu6G5IVwb", "expanded_url": "https://twitter.com/DrWalwyn/status/1419659604926083075/photo/1", "id": 1419659600329072644, "media_url": "http://pbs.twimg.com/media/E7Ok4oOWYAQyWv0.jpg", "media_url_https": "https://pbs.twimg.com/media/E7Ok4oOWYAQyWv0.jpg", "sizes": {"large": {"h": 1198, "resize": "fit", "w": 1598}, "medium": {"h": 900, "resize": "fit", "w": 1200}, "small": {"h": 510, "resize": "fit", "w": 680}, "thumb": {"h": 150, "resize": "crop", "w": 150}}, "type": "photo", "url": "https://t.co/keu6G5IVwb"}], "retweet_count": 1, "source": "&lt;a href=\"http://twitter.com/download/iphone\" rel=\"nofollow\"&gt;Twitter for iPhone&lt;/a&gt;", "text": "Bellevue University in 2008 with my masters. Thanks Bellevue and my professor. https://t.co/keu6G5IVwb", "urls": [], "user": {"created_at": "Mon Sep 17 10:18:35 +0000 2012", "default_profile": true, "favourites_count": 43, "followers_count": 466, "friends_count": 205, "geo_enabled": true, "id": 828777422, "id_str": "828777422", "listed_count": 9, "location": "United States Virgin Islands", "name": "cgwalwyn@gmail.com", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_image_url": "http://pbs.twimg.com/profile_images/1216345664768086016/C66vTzCr_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1216345664768086016/C66vTzCr_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "DrWalwyn", "statuses_count": 3012, "url": "https://t.co/eOWYVVQc2u", "withheld_in_countries": []}, "user_mentions": []}</t>
   </si>
   <si>
-    <t>{"created_at": "Mon Jul 26 02:29:34 +0000 2021", "hashtags": [], "id": 1419485012886360064, "id_str": "1419485012886360064", "lang": "en", "retweet_count": 2, "retweeted_status": {"created_at": "Sun Jul 25 21:55:43 +0000 2021", "favorite_count": 4, "hashtags": [], "id": 1419416096583536640, "id_str": "1419416096583536640", "in_reply_to_screen_name": "mister_wynn", "in_reply_to_status_id": 1419228058813296646, "in_reply_to_user_id": 1239700053498855424, "lang": "en", "retweet_count": 2, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@mister_wynn @RBJRON @randlight @3wombats Van Onselen was born in Sydney, New South Wales and grew up in the easter\u2026 https://t.co/NxXawIqBny", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1419416096583536640", "url": "https://t.co/NxXawIqBny"}], "user": {"created_at": "Thu Apr 23 08:04:39 +0000 2009", "description": "Born Ostraleyan, 70, East coast, Scorpio, Time sees all things right ! Verbal Cartoonist! I plead Dissociative Fugue!", "favourites_count": 25098, "followers_count": 1505, "friends_count": 610, "id": 34564954, "id_str": "34564954", "listed_count": 38, "location": "Aus.", "name": "Sir Geoff", "profile_background_color": "89C9FA", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme9/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme9/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/34564954/1431421029", "profile_image_url": "http://pbs.twimg.com/profile_images/487617917/bridge002_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/487617917/bridge002_normal.jpg", "profile_link_color": "89C9FA", "profile_sidebar_border_color": "181A1E", "profile_sidebar_fill_color": "252429", "profile_text_color": "666666", "profile_use_background_image": true, "screen_name": "nanoview", "statuses_count": 92348, "withheld_in_countries": []}, "user_mentions": [{"id": 1239700053498855424, "id_str": "1239700053498855424", "name": "Lord - Sir Thomas Wynn", "screen_name": "mister_wynn"}, {"id": 1601937732, "id_str": "1601937732", "name": "\ud83d\udca7Ron Jones\u2744", "screen_name": "RBJRON"}, {"id": 384233102, "id_str": "384233102", "name": "Mari R", "screen_name": "randlight"}, {"id": 243882040, "id_str": "243882040", "name": "Battle Weary Woman", "screen_name": "3wombats"}]}, "source": "&lt;a href=\"http://twitter.com/download/android\" rel=\"nofollow\"&gt;Twitter for Android&lt;/a&gt;", "text": "RT @nanoview: @mister_wynn @RBJRON @randlight @3wombats Van Onselen was born in Sydney, New South Wales and grew up in the eastern suburbs\u2026", "urls": [], "user": {"created_at": "Mon Oct 03 09:46:09 +0000 2011", "description": "Travel  a lot and realise that Oz is the best country in the world to  live in, despite having an LNP government and now 3rd PM 5 years.\ud83d\udc4enext? Hopefully Albo\ud83e\udd1e", "favourites_count": 58601, "followers_count": 17297, "friends_count": 11176, "geo_enabled": true, "id": 384233102, "id_str": "384233102", "listed_count": 216, "location": "Australia", "name": "Mari R", "profile_background_color": "8B542B", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme8/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme8/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/384233102/1388653033", "profile_image_url": "http://pbs.twimg.com/profile_images/1719274208/greece_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1719274208/greece_normal.jpg", "profile_link_color": "9D582E", "profile_sidebar_border_color": "D9B17E", "profile_sidebar_fill_color": "EADEAA", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "randlight", "statuses_count": 665516, "withheld_in_countries": []}, "user_mentions": [{"id": 34564954, "id_str": "34564954", "name": "Sir Geoff", "screen_name": "nanoview"}, {"id": 1239700053498855424, "id_str": "1239700053498855424", "name": "Lord - Sir Thomas Wynn", "screen_name": "mister_wynn"}, {"id": 1601937732, "id_str": "1601937732", "name": "\ud83d\udca7Ron Jones\u2744", "screen_name": "RBJRON"}, {"id": 384233102, "id_str": "384233102", "name": "Mari R", "screen_name": "randlight"}, {"id": 243882040, "id_str": "243882040", "name": "Battle Weary Woman", "screen_name": "3wombats"}]}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Sun Jul 25 21:59:52 +0000 2021", "hashtags": [], "id": 1419417140411572225, "id_str": "1419417140411572225", "lang": "en", "retweet_count": 2, "retweeted_status": {"created_at": "Sun Jul 25 21:55:43 +0000 2021", "favorite_count": 4, "hashtags": [], "id": 1419416096583536640, "id_str": "1419416096583536640", "in_reply_to_screen_name": "mister_wynn", "in_reply_to_status_id": 1419228058813296646, "in_reply_to_user_id": 1239700053498855424, "lang": "en", "retweet_count": 2, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@mister_wynn @RBJRON @randlight @3wombats Van Onselen was born in Sydney, New South Wales and grew up in the easter\u2026 https://t.co/NxXawIqBny", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1419416096583536640", "url": "https://t.co/NxXawIqBny"}], "user": {"created_at": "Thu Apr 23 08:04:39 +0000 2009", "description": "Born Ostraleyan, 70, East coast, Scorpio, Time sees all things right ! Verbal Cartoonist! I plead Dissociative Fugue!", "favourites_count": 25098, "followers_count": 1505, "friends_count": 610, "id": 34564954, "id_str": "34564954", "listed_count": 38, "location": "Aus.", "name": "Sir Geoff", "profile_background_color": "89C9FA", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme9/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme9/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/34564954/1431421029", "profile_image_url": "http://pbs.twimg.com/profile_images/487617917/bridge002_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/487617917/bridge002_normal.jpg", "profile_link_color": "89C9FA", "profile_sidebar_border_color": "181A1E", "profile_sidebar_fill_color": "252429", "profile_text_color": "666666", "profile_use_background_image": true, "screen_name": "nanoview", "statuses_count": 92348, "withheld_in_countries": []}, "user_mentions": [{"id": 1239700053498855424, "id_str": "1239700053498855424", "name": "Lord - Sir Thomas Wynn", "screen_name": "mister_wynn"}, {"id": 1601937732, "id_str": "1601937732", "name": "\ud83d\udca7Ron Jones\u2744", "screen_name": "RBJRON"}, {"id": 384233102, "id_str": "384233102", "name": "Mari R", "screen_name": "randlight"}, {"id": 243882040, "id_str": "243882040", "name": "Battle Weary Woman", "screen_name": "3wombats"}]}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @nanoview: @mister_wynn @RBJRON @randlight @3wombats Van Onselen was born in Sydney, New South Wales and grew up in the eastern suburbs\u2026", "urls": [], "user": {"created_at": "Mon Mar 16 23:48:44 +0000 2020", "default_profile": true, "description": "Lord of Aberdeenshire Scotland, Grandfather, retired Dep Principal, music editor &amp; arranger, blogger, author, geek, historian, (modest) &amp; slightly psychic!", "favourites_count": 261, "followers_count": 1955, "friends_count": 266, "id": 1239700053498855424, "id_str": "1239700053498855424", "listed_count": 8, "name": "Lord - Sir Thomas Wynn", "profile_background_color": "F5F8FA", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1239700053498855424/1585220092", "profile_image_url": "http://pbs.twimg.com/profile_images/1243129347973627904/OQMbxTMN_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1243129347973627904/OQMbxTMN_normal.png", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "mister_wynn", "statuses_count": 60246, "withheld_in_countries": []}, "user_mentions": [{"id": 34564954, "id_str": "34564954", "name": "Sir Geoff", "screen_name": "nanoview"}, {"id": 1239700053498855424, "id_str": "1239700053498855424", "name": "Lord - Sir Thomas Wynn", "screen_name": "mister_wynn"}, {"id": 1601937732, "id_str": "1601937732", "name": "\ud83d\udca7Ron Jones\u2744", "screen_name": "RBJRON"}, {"id": 384233102, "id_str": "384233102", "name": "Mari R", "screen_name": "randlight"}, {"id": 243882040, "id_str": "243882040", "name": "Battle Weary Woman", "screen_name": "3wombats"}]}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Sun Jul 25 21:55:43 +0000 2021", "favorite_count": 4, "hashtags": [], "id": 1419416096583536640, "id_str": "1419416096583536640", "in_reply_to_screen_name": "mister_wynn", "in_reply_to_status_id": 1419228058813296646, "in_reply_to_user_id": 1239700053498855424, "lang": "en", "retweet_count": 2, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@mister_wynn @RBJRON @randlight @3wombats Van Onselen was born in Sydney, New South Wales and grew up in the easter\u2026 https://t.co/NxXawIqBny", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1419416096583536640", "url": "https://t.co/NxXawIqBny"}], "user": {"created_at": "Thu Apr 23 08:04:39 +0000 2009", "description": "Born Ostraleyan, 70, East coast, Scorpio, Time sees all things right ! Verbal Cartoonist! I plead Dissociative Fugue!", "favourites_count": 25098, "followers_count": 1505, "friends_count": 610, "id": 34564954, "id_str": "34564954", "listed_count": 38, "location": "Aus.", "name": "Sir Geoff", "profile_background_color": "89C9FA", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme9/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme9/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/34564954/1431421029", "profile_image_url": "http://pbs.twimg.com/profile_images/487617917/bridge002_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/487617917/bridge002_normal.jpg", "profile_link_color": "89C9FA", "profile_sidebar_border_color": "181A1E", "profile_sidebar_fill_color": "252429", "profile_text_color": "666666", "profile_use_background_image": true, "screen_name": "nanoview", "statuses_count": 92348, "withheld_in_countries": []}, "user_mentions": [{"id": 1239700053498855424, "id_str": "1239700053498855424", "name": "Lord - Sir Thomas Wynn", "screen_name": "mister_wynn"}, {"id": 1601937732, "id_str": "1601937732", "name": "\ud83d\udca7Ron Jones\u2744", "screen_name": "RBJRON"}, {"id": 384233102, "id_str": "384233102", "name": "Mari R", "screen_name": "randlight"}, {"id": 243882040, "id_str": "243882040", "name": "Battle Weary Woman", "screen_name": "3wombats"}]}</t>
+    <t>{"created_at": "Mon Jul 26 02:29:34 +0000 2021", "hashtags": [], "id": 1419485012886360064, "id_str": "1419485012886360064", "lang": "en", "retweet_count": 2, "retweeted_status": {"created_at": "Sun Jul 25 21:55:43 +0000 2021", "favorite_count": 4, "hashtags": [], "id": 1419416096583536640, "id_str": "1419416096583536640", "in_reply_to_screen_name": "mister_wynn", "in_reply_to_status_id": 1419228058813296646, "in_reply_to_user_id": 1239700053498855424, "lang": "en", "retweet_count": 2, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@mister_wynn @RBJRON @randlight @3wombats Van Onselen was born in Sydney, New South Wales and grew up in the easter\u2026 https://t.co/NxXawIqBny", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1419416096583536640", "url": "https://t.co/NxXawIqBny"}], "user": {"created_at": "Thu Apr 23 08:04:39 +0000 2009", "description": "Born Ostraleyan, 70, East coast, Scorpio, Time sees all things right ! Verbal Cartoonist! I plead Dissociative Fugue!", "favourites_count": 25101, "followers_count": 1505, "friends_count": 610, "id": 34564954, "id_str": "34564954", "listed_count": 38, "location": "Aus.", "name": "Sir Geoff", "profile_background_color": "89C9FA", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme9/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme9/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/34564954/1431421029", "profile_image_url": "http://pbs.twimg.com/profile_images/487617917/bridge002_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/487617917/bridge002_normal.jpg", "profile_link_color": "89C9FA", "profile_sidebar_border_color": "181A1E", "profile_sidebar_fill_color": "252429", "profile_text_color": "666666", "profile_use_background_image": true, "screen_name": "nanoview", "statuses_count": 92357, "withheld_in_countries": []}, "user_mentions": [{"id": 1239700053498855424, "id_str": "1239700053498855424", "name": "Lord - Sir Thomas Wynn", "screen_name": "mister_wynn"}, {"id": 1601937732, "id_str": "1601937732", "name": "\ud83d\udca7Ron Jones\u2744", "screen_name": "RBJRON"}, {"id": 384233102, "id_str": "384233102", "name": "Mari R", "screen_name": "randlight"}, {"id": 243882040, "id_str": "243882040", "name": "Battle Weary Woman", "screen_name": "3wombats"}]}, "source": "&lt;a href=\"http://twitter.com/download/android\" rel=\"nofollow\"&gt;Twitter for Android&lt;/a&gt;", "text": "RT @nanoview: @mister_wynn @RBJRON @randlight @3wombats Van Onselen was born in Sydney, New South Wales and grew up in the eastern suburbs\u2026", "urls": [], "user": {"created_at": "Mon Oct 03 09:46:09 +0000 2011", "description": "Travel  a lot and realise that Oz is the best country in the world to  live in, despite having an LNP government and now 3rd PM 5 years.\ud83d\udc4enext? Hopefully Albo\ud83e\udd1e", "favourites_count": 58709, "followers_count": 17302, "friends_count": 11177, "geo_enabled": true, "id": 384233102, "id_str": "384233102", "listed_count": 216, "location": "Australia", "name": "Mari R", "profile_background_color": "8B542B", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme8/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme8/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/384233102/1388653033", "profile_image_url": "http://pbs.twimg.com/profile_images/1719274208/greece_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1719274208/greece_normal.jpg", "profile_link_color": "9D582E", "profile_sidebar_border_color": "D9B17E", "profile_sidebar_fill_color": "EADEAA", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "randlight", "statuses_count": 665566, "withheld_in_countries": []}, "user_mentions": [{"id": 34564954, "id_str": "34564954", "name": "Sir Geoff", "screen_name": "nanoview"}, {"id": 1239700053498855424, "id_str": "1239700053498855424", "name": "Lord - Sir Thomas Wynn", "screen_name": "mister_wynn"}, {"id": 1601937732, "id_str": "1601937732", "name": "\ud83d\udca7Ron Jones\u2744", "screen_name": "RBJRON"}, {"id": 384233102, "id_str": "384233102", "name": "Mari R", "screen_name": "randlight"}, {"id": 243882040, "id_str": "243882040", "name": "Battle Weary Woman", "screen_name": "3wombats"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Sun Jul 25 21:59:52 +0000 2021", "hashtags": [], "id": 1419417140411572225, "id_str": "1419417140411572225", "lang": "en", "retweet_count": 2, "retweeted_status": {"created_at": "Sun Jul 25 21:55:43 +0000 2021", "favorite_count": 4, "hashtags": [], "id": 1419416096583536640, "id_str": "1419416096583536640", "in_reply_to_screen_name": "mister_wynn", "in_reply_to_status_id": 1419228058813296646, "in_reply_to_user_id": 1239700053498855424, "lang": "en", "retweet_count": 2, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@mister_wynn @RBJRON @randlight @3wombats Van Onselen was born in Sydney, New South Wales and grew up in the easter\u2026 https://t.co/NxXawIqBny", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1419416096583536640", "url": "https://t.co/NxXawIqBny"}], "user": {"created_at": "Thu Apr 23 08:04:39 +0000 2009", "description": "Born Ostraleyan, 70, East coast, Scorpio, Time sees all things right ! Verbal Cartoonist! I plead Dissociative Fugue!", "favourites_count": 25101, "followers_count": 1505, "friends_count": 610, "id": 34564954, "id_str": "34564954", "listed_count": 38, "location": "Aus.", "name": "Sir Geoff", "profile_background_color": "89C9FA", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme9/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme9/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/34564954/1431421029", "profile_image_url": "http://pbs.twimg.com/profile_images/487617917/bridge002_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/487617917/bridge002_normal.jpg", "profile_link_color": "89C9FA", "profile_sidebar_border_color": "181A1E", "profile_sidebar_fill_color": "252429", "profile_text_color": "666666", "profile_use_background_image": true, "screen_name": "nanoview", "statuses_count": 92357, "withheld_in_countries": []}, "user_mentions": [{"id": 1239700053498855424, "id_str": "1239700053498855424", "name": "Lord - Sir Thomas Wynn", "screen_name": "mister_wynn"}, {"id": 1601937732, "id_str": "1601937732", "name": "\ud83d\udca7Ron Jones\u2744", "screen_name": "RBJRON"}, {"id": 384233102, "id_str": "384233102", "name": "Mari R", "screen_name": "randlight"}, {"id": 243882040, "id_str": "243882040", "name": "Battle Weary Woman", "screen_name": "3wombats"}]}, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "RT @nanoview: @mister_wynn @RBJRON @randlight @3wombats Van Onselen was born in Sydney, New South Wales and grew up in the eastern suburbs\u2026", "urls": [], "user": {"created_at": "Mon Mar 16 23:48:44 +0000 2020", "default_profile": true, "description": "Lord of Aberdeenshire Scotland, Grandfather, retired Dep Principal, music editor &amp; arranger, blogger, author, geek, historian, (modest) &amp; slightly psychic!", "favourites_count": 261, "followers_count": 1957, "friends_count": 266, "id": 1239700053498855424, "id_str": "1239700053498855424", "listed_count": 8, "name": "Lord - Sir Thomas Wynn", "profile_background_color": "F5F8FA", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1239700053498855424/1585220092", "profile_image_url": "http://pbs.twimg.com/profile_images/1243129347973627904/OQMbxTMN_normal.png", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1243129347973627904/OQMbxTMN_normal.png", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "mister_wynn", "statuses_count": 60281, "withheld_in_countries": []}, "user_mentions": [{"id": 34564954, "id_str": "34564954", "name": "Sir Geoff", "screen_name": "nanoview"}, {"id": 1239700053498855424, "id_str": "1239700053498855424", "name": "Lord - Sir Thomas Wynn", "screen_name": "mister_wynn"}, {"id": 1601937732, "id_str": "1601937732", "name": "\ud83d\udca7Ron Jones\u2744", "screen_name": "RBJRON"}, {"id": 384233102, "id_str": "384233102", "name": "Mari R", "screen_name": "randlight"}, {"id": 243882040, "id_str": "243882040", "name": "Battle Weary Woman", "screen_name": "3wombats"}]}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Sun Jul 25 21:55:43 +0000 2021", "favorite_count": 4, "hashtags": [], "id": 1419416096583536640, "id_str": "1419416096583536640", "in_reply_to_screen_name": "mister_wynn", "in_reply_to_status_id": 1419228058813296646, "in_reply_to_user_id": 1239700053498855424, "lang": "en", "retweet_count": 2, "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@mister_wynn @RBJRON @randlight @3wombats Van Onselen was born in Sydney, New South Wales and grew up in the easter\u2026 https://t.co/NxXawIqBny", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1419416096583536640", "url": "https://t.co/NxXawIqBny"}], "user": {"created_at": "Thu Apr 23 08:04:39 +0000 2009", "description": "Born Ostraleyan, 70, East coast, Scorpio, Time sees all things right ! Verbal Cartoonist! I plead Dissociative Fugue!", "favourites_count": 25101, "followers_count": 1505, "friends_count": 610, "id": 34564954, "id_str": "34564954", "listed_count": 38, "location": "Aus.", "name": "Sir Geoff", "profile_background_color": "89C9FA", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme9/bg.gif", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme9/bg.gif", "profile_banner_url": "https://pbs.twimg.com/profile_banners/34564954/1431421029", "profile_image_url": "http://pbs.twimg.com/profile_images/487617917/bridge002_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/487617917/bridge002_normal.jpg", "profile_link_color": "89C9FA", "profile_sidebar_border_color": "181A1E", "profile_sidebar_fill_color": "252429", "profile_text_color": "666666", "profile_use_background_image": true, "screen_name": "nanoview", "statuses_count": 92357, "withheld_in_countries": []}, "user_mentions": [{"id": 1239700053498855424, "id_str": "1239700053498855424", "name": "Lord - Sir Thomas Wynn", "screen_name": "mister_wynn"}, {"id": 1601937732, "id_str": "1601937732", "name": "\ud83d\udca7Ron Jones\u2744", "screen_name": "RBJRON"}, {"id": 384233102, "id_str": "384233102", "name": "Mari R", "screen_name": "randlight"}, {"id": 243882040, "id_str": "243882040", "name": "Battle Weary Woman", "screen_name": "3wombats"}]}</t>
   </si>
   <si>
     <t>{"created_at": "Sat Jul 24 14:18:11 +0000 2021", "hashtags": [], "id": 1418938564566556673, "id_str": "1418938564566556673", "lang": "en", "source": "&lt;a href=\"http://instagram.com\" rel=\"nofollow\"&gt;Instagram&lt;/a&gt;", "text": "Just posted a photo @ Bellevue University https://t.co/iUugiZS1ht", "urls": [{"expanded_url": "https://www.instagram.com/p/CRtoaaDF1cxEMR6FOYd53ZgCBfeCDMGwtm_2lg0/?utm_medium=twitter", "url": "https://t.co/iUugiZS1ht"}], "user": {"created_at": "Sun May 06 03:50:33 +0000 2012", "default_profile": true, "description": "I Provide Guidance and Understanding, Helping others Align their Actions with Intentions!\nhttps://t.co/swNiDMXL5C", "favourites_count": 2, "followers_count": 95, "friends_count": 263, "id": 572288128, "id_str": "572288128", "listed_count": 1, "location": "Centennial, CO", "name": "Mike Faulhaber, CFP", "profile_background_color": "C0DEED", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme1/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme1/bg.png", "profile_banner_url": "https://pbs.twimg.com/profile_banners/572288128/1617376486", "profile_image_url": "http://pbs.twimg.com/profile_images/1243919742546608128/QZtQitai_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1243919742546608128/QZtQitai_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "AreteKaiPistis", "statuses_count": 1948, "url": "https://t.co/c4d8FFPW5W", "withheld_in_countries": []}, "user_mentions": []}</t>
   </si>
   <si>
-    <t>{"created_at": "Sat Jul 24 12:05:21 +0000 2021", "hashtags": [], "id": 1418905139180617743, "id_str": "1418905139180617743", "lang": "en", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "In 1952, \nafter graduating with high honors from the College of the Holy Cross in Worcester, Mass., \nhe was offered\u2026 https://t.co/x9GWv62Pdm", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1418905139180617743", "url": "https://t.co/x9GWv62Pdm"}], "user": {"created_at": "Tue Jul 20 19:53:54 +0000 2021", "default_profile": true, "description": "please do not follow me.", "favourites_count": 75, "followers_count": 1, "friends_count": 9, "id": 1417573053266018309, "id_str": "1417573053266018309", "name": "MatterThatMatters", "profile_background_color": "F5F8FA", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1417573053266018309/1627662505", "profile_image_url": "http://pbs.twimg.com/profile_images/1421157506483638278/Sz4WYVqy_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1421157506483638278/Sz4WYVqy_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "MatterThatMatt6", "statuses_count": 1935, "url": "https://t.co/tYXVhIWQZA", "withheld_in_countries": []}, "user_mentions": []}</t>
-  </si>
-  <si>
-    <t>{"created_at": "Fri Jul 23 02:21:09 +0000 2021", "hashtags": [], "id": 1418395729165443074, "id_str": "1418395729165443074", "in_reply_to_screen_name": "DrLeanaWen", "in_reply_to_status_id": 1418335834940624898, "in_reply_to_user_id": 605153786, "lang": "en", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@DrLeanaWen Sarah Root killed on January 31st of 2016, hours after she graduated with honors from Bellevue Universi\u2026 https://t.co/edK6X817yO", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1418395729165443074", "url": "https://t.co/edK6X817yO"}], "user": {"created_at": "Wed Jan 25 07:44:39 +0000 2012", "description": "Please follow @PeckPolitics GO TRUMP AMERICA / What Free Speech? Pioneer Spirit \ud83d\ude81#HelicopterTwitter NATIONALIST https://t.co/zBnsj0MQxO", "favourites_count": 144448, "followers_count": 6013, "friends_count": 5713, "id": 473704565, "id_str": "473704565", "listed_count": 22, "location": "Iowa", "name": "Horse Lady Cornfield", "profile_background_color": "022330", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/473704565/1626341475", "profile_image_url": "http://pbs.twimg.com/profile_images/1415607970130452486/c5cf5POV_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1415607970130452486/c5cf5POV_normal.jpg", "profile_link_color": "0084B4", "profile_sidebar_border_color": "A8C7F7", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "TanyaCornfield", "statuses_count": 211869, "withheld_in_countries": []}, "user_mentions": [{"id": 605153786, "id_str": "605153786", "name": "Leana Wen, M.D.", "screen_name": "DrLeanaWen"}]}</t>
+    <t>{"created_at": "Sat Jul 24 12:05:21 +0000 2021", "hashtags": [], "id": 1418905139180617743, "id_str": "1418905139180617743", "lang": "en", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "In 1952, \nafter graduating with high honors from the College of the Holy Cross in Worcester, Mass., \nhe was offered\u2026 https://t.co/x9GWv62Pdm", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1418905139180617743", "url": "https://t.co/x9GWv62Pdm"}], "user": {"created_at": "Tue Jul 20 19:53:54 +0000 2021", "default_profile": true, "description": "please do not follow me.", "favourites_count": 75, "followers_count": 1, "friends_count": 9, "id": 1417573053266018309, "id_str": "1417573053266018309", "name": "MatterThatMatters", "profile_background_color": "F5F8FA", "profile_banner_url": "https://pbs.twimg.com/profile_banners/1417573053266018309/1627662505", "profile_image_url": "http://pbs.twimg.com/profile_images/1421157506483638278/Sz4WYVqy_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1421157506483638278/Sz4WYVqy_normal.jpg", "profile_link_color": "1DA1F2", "profile_sidebar_border_color": "C0DEED", "profile_sidebar_fill_color": "DDEEF6", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "MatterThatMatt6", "statuses_count": 1865, "url": "https://t.co/tYXVhIWQZA", "withheld_in_countries": []}, "user_mentions": []}</t>
+  </si>
+  <si>
+    <t>{"created_at": "Fri Jul 23 02:21:09 +0000 2021", "hashtags": [], "id": 1418395729165443074, "id_str": "1418395729165443074", "in_reply_to_screen_name": "DrLeanaWen", "in_reply_to_status_id": 1418335834940624898, "in_reply_to_user_id": 605153786, "lang": "en", "source": "&lt;a href=\"https://mobile.twitter.com\" rel=\"nofollow\"&gt;Twitter Web App&lt;/a&gt;", "text": "@DrLeanaWen Sarah Root killed on January 31st of 2016, hours after she graduated with honors from Bellevue Universi\u2026 https://t.co/edK6X817yO", "truncated": true, "urls": [{"expanded_url": "https://twitter.com/i/web/status/1418395729165443074", "url": "https://t.co/edK6X817yO"}], "user": {"created_at": "Wed Jan 25 07:44:39 +0000 2012", "description": "Please follow @PeckPolitics GO TRUMP AMERICA / What Free Speech? Pioneer Spirit \ud83d\ude81#HelicopterTwitter NATIONALIST https://t.co/zBnsj0MQxO", "favourites_count": 144534, "followers_count": 6013, "friends_count": 5715, "id": 473704565, "id_str": "473704565", "listed_count": 22, "location": "Iowa", "name": "Horse Lady Cornfield", "profile_background_color": "022330", "profile_background_image_url": "http://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_image_url_https": "https://abs.twimg.com/images/themes/theme15/bg.png", "profile_background_tile": true, "profile_banner_url": "https://pbs.twimg.com/profile_banners/473704565/1626341475", "profile_image_url": "http://pbs.twimg.com/profile_images/1415607970130452486/c5cf5POV_normal.jpg", "profile_image_url_https": "https://pbs.twimg.com/profile_images/1415607970130452486/c5cf5POV_normal.jpg", "profile_link_color": "0084B4", "profile_sidebar_border_color": "A8C7F7", "profile_sidebar_fill_color": "C0DFEC", "profile_text_color": "333333", "profile_use_background_image": true, "screen_name": "TanyaCornfield", "statuses_count": 211902, "withheld_in_countries": []}, "user_mentions": [{"id": 605153786, "id_str": "605153786", "name": "Leana Wen, M.D.", "screen_name": "DrLeanaWen"}]}</t>
   </si>
 </sst>
 </file>
@@ -566,7 +572,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1089,6 +1095,22 @@
         <v>64</v>
       </c>
     </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>